<commit_message>
Finished market data, started order statistics
</commit_message>
<xml_diff>
--- a/xlsx/analysis.xlsx
+++ b/xlsx/analysis.xlsx
@@ -476,12 +476,12 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>adtv30</t>
+          <t>adtv30d</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>adtv90</t>
+          <t>adtv90d</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -496,27 +496,27 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>obv30d</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>obv90d</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>ma30d</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>ma90d</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>ewm</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>adtv30d</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>adtv90d</t>
         </is>
       </c>
     </row>
@@ -535,34 +535,44 @@
       <c r="D2" t="n">
         <v>0.00113835116969252</v>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>0.03536765552462411</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.03890127454137432</v>
+      </c>
       <c r="G2" t="n">
         <v>478.4021741722594</v>
       </c>
       <c r="H2" t="n">
         <v>532.6817844559362</v>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+      <c r="I2" t="n">
+        <v>2781855.933333333</v>
+      </c>
+      <c r="J2" t="n">
+        <v>3445060.877777778</v>
+      </c>
       <c r="K2" t="n">
         <v>400.8687258687258</v>
       </c>
-      <c r="L2" t="inlineStr"/>
+      <c r="L2" t="n">
+        <v>2152416</v>
+      </c>
       <c r="M2" t="n">
+        <v>-17729448</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-80024909</v>
+      </c>
+      <c r="O2" t="n">
         <v>478.8986666666667</v>
       </c>
-      <c r="N2" t="n">
+      <c r="P2" t="n">
         <v>537.2432222222222</v>
       </c>
-      <c r="O2" t="n">
+      <c r="Q2" t="n">
         <v>486.6395954223248</v>
-      </c>
-      <c r="P2" t="n">
-        <v>2781855.933333333</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>3445060.877777778</v>
       </c>
     </row>
     <row r="3">
@@ -580,34 +590,44 @@
       <c r="D3" t="n">
         <v>-0.005102104578750932</v>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>0.03542220982864532</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.03895312133992412</v>
+      </c>
       <c r="G3" t="n">
         <v>478.6639327048821</v>
       </c>
       <c r="H3" t="n">
         <v>533.3567856095348</v>
       </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+      <c r="I3" t="n">
+        <v>2875863.9</v>
+      </c>
+      <c r="J3" t="n">
+        <v>3442555.355555556</v>
+      </c>
       <c r="K3" t="n">
         <v>770.3007518797011</v>
       </c>
-      <c r="L3" t="inlineStr"/>
+      <c r="L3" t="n">
+        <v>-2562865</v>
+      </c>
       <c r="M3" t="n">
+        <v>-24854519</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-80250406</v>
+      </c>
+      <c r="O3" t="n">
         <v>478.955</v>
       </c>
-      <c r="N3" t="n">
+      <c r="P3" t="n">
         <v>538.3851111111112</v>
       </c>
-      <c r="O3" t="n">
+      <c r="Q3" t="n">
         <v>486.860946830761</v>
-      </c>
-      <c r="P3" t="n">
-        <v>2875863.9</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>3442555.355555556</v>
       </c>
     </row>
     <row r="4">
@@ -625,34 +645,44 @@
       <c r="D4" t="n">
         <v>0.01955747346092096</v>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>0.03687471262381947</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.03930404669550656</v>
+      </c>
       <c r="G4" t="n">
         <v>478.86985859123</v>
       </c>
       <c r="H4" t="n">
         <v>534.204648694748</v>
       </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+      <c r="I4" t="n">
+        <v>2903879.3</v>
+      </c>
+      <c r="J4" t="n">
+        <v>3445523.022222222</v>
+      </c>
       <c r="K4" t="n">
         <v>378.6733837111665</v>
       </c>
-      <c r="L4" t="inlineStr"/>
+      <c r="L4" t="n">
+        <v>3491638</v>
+      </c>
       <c r="M4" t="n">
+        <v>-25694981</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-74857586</v>
+      </c>
+      <c r="O4" t="n">
         <v>479.0959999999999</v>
       </c>
-      <c r="N4" t="n">
+      <c r="P4" t="n">
         <v>539.4703333333333</v>
       </c>
-      <c r="O4" t="n">
+      <c r="Q4" t="n">
         <v>487.1354948880549</v>
-      </c>
-      <c r="P4" t="n">
-        <v>2903879.3</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>3445523.022222222</v>
       </c>
     </row>
     <row r="5">
@@ -670,34 +700,44 @@
       <c r="D5" t="n">
         <v>-0.01493156429691744</v>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>0.03518612570774039</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.03912338232045677</v>
+      </c>
       <c r="G5" t="n">
         <v>479.1553580864267</v>
       </c>
       <c r="H5" t="n">
         <v>534.9470117961548</v>
       </c>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
+      <c r="I5" t="n">
+        <v>2874305.633333333</v>
+      </c>
+      <c r="J5" t="n">
+        <v>3428096.377777778</v>
+      </c>
       <c r="K5" t="n">
         <v>-3051.28205128202</v>
       </c>
-      <c r="L5" t="inlineStr"/>
+      <c r="L5" t="n">
+        <v>-4287846</v>
+      </c>
       <c r="M5" t="n">
+        <v>-31791047</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-80272464</v>
+      </c>
+      <c r="O5" t="n">
         <v>479.4846666666666</v>
       </c>
-      <c r="N5" t="n">
+      <c r="P5" t="n">
         <v>540.3508888888888</v>
       </c>
-      <c r="O5" t="n">
+      <c r="Q5" t="n">
         <v>487.2586324665414</v>
-      </c>
-      <c r="P5" t="n">
-        <v>2874305.633333333</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>3428096.377777778</v>
       </c>
     </row>
     <row r="6">
@@ -715,34 +755,44 @@
       <c r="D6" t="n">
         <v>0.001698778117256161</v>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>0.03450671475965837</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.03907171119089434</v>
+      </c>
       <c r="G6" t="n">
         <v>480.0442540217421</v>
       </c>
       <c r="H6" t="n">
         <v>535.9920601809156</v>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
+      <c r="I6" t="n">
+        <v>2834153.2</v>
+      </c>
+      <c r="J6" t="n">
+        <v>3403699.188888889</v>
+      </c>
       <c r="K6" t="n">
         <v>390.9892262487743</v>
       </c>
-      <c r="L6" t="inlineStr"/>
+      <c r="L6" t="n">
+        <v>2458192</v>
+      </c>
       <c r="M6" t="n">
+        <v>-30586474</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-78076717</v>
+      </c>
+      <c r="O6" t="n">
         <v>480.26</v>
       </c>
-      <c r="N6" t="n">
+      <c r="P6" t="n">
         <v>541.3631111111112</v>
       </c>
-      <c r="O6" t="n">
+      <c r="Q6" t="n">
         <v>488.0385381538891</v>
-      </c>
-      <c r="P6" t="n">
-        <v>2834153.2</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>3403699.188888889</v>
       </c>
     </row>
     <row r="7">
@@ -760,34 +810,44 @@
       <c r="D7" t="n">
         <v>-0.0007461604176484116</v>
       </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>0.03452063001290907</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.03912833073819739</v>
+      </c>
       <c r="G7" t="n">
         <v>480.4908320871507</v>
       </c>
       <c r="H7" t="n">
         <v>536.7059491325657</v>
       </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>2820747.8</v>
+      </c>
+      <c r="J7" t="n">
+        <v>3403919.366666667</v>
+      </c>
       <c r="K7" t="n">
         <v>292.9220779220773</v>
       </c>
-      <c r="L7" t="inlineStr"/>
+      <c r="L7" t="n">
+        <v>-2741116</v>
+      </c>
       <c r="M7" t="n">
+        <v>-35100696</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-83012917</v>
+      </c>
+      <c r="O7" t="n">
         <v>480.8926666666667</v>
       </c>
-      <c r="N7" t="n">
+      <c r="P7" t="n">
         <v>542.3484444444445</v>
       </c>
-      <c r="O7" t="n">
+      <c r="Q7" t="n">
         <v>488.3784373369159</v>
-      </c>
-      <c r="P7" t="n">
-        <v>2820747.8</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>3403919.366666667</v>
       </c>
     </row>
     <row r="8">
@@ -805,7 +865,9 @@
       <c r="D8" t="n">
         <v>-0.01122854959847785</v>
       </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>0.03453321999914554</v>
+      </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
         <v>481.5286440971489</v>
@@ -813,26 +875,32 @@
       <c r="H8" t="n">
         <v>537.5945803701691</v>
       </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
+      <c r="I8" t="n">
+        <v>2859277.366666667</v>
+      </c>
+      <c r="J8" t="n">
+        <v>3405020.211111111</v>
+      </c>
       <c r="K8" t="n">
         <v>266.4775950085084</v>
       </c>
-      <c r="L8" t="inlineStr"/>
+      <c r="L8" t="n">
+        <v>-2301635</v>
+      </c>
       <c r="M8" t="n">
+        <v>-28462577</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-83111993</v>
+      </c>
+      <c r="O8" t="n">
         <v>481.6363333333333</v>
       </c>
-      <c r="N8" t="n">
+      <c r="P8" t="n">
         <v>543.4348888888888</v>
       </c>
-      <c r="O8" t="n">
+      <c r="Q8" t="n">
         <v>488.7983295670479</v>
-      </c>
-      <c r="P8" t="n">
-        <v>2859277.366666667</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>3405020.211111111</v>
       </c>
     </row>
     <row r="9">
@@ -850,29 +918,35 @@
       <c r="D9" t="n">
         <v>-0.008507043562066663</v>
       </c>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0.03422791723121955</v>
+      </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
         <v>482.6018842086505</v>
       </c>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
+      <c r="I9" t="n">
+        <v>2923503.366666667</v>
+      </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="n">
         <v>314.8793565683644</v>
       </c>
-      <c r="L9" t="inlineStr"/>
+      <c r="L9" t="n">
+        <v>-2165021</v>
+      </c>
       <c r="M9" t="n">
-        <v>482.3613333333333</v>
+        <v>-30389357</v>
       </c>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="n">
+        <v>482.3613333333333</v>
+      </c>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="n">
         <v>489.2223522958098</v>
       </c>
-      <c r="P9" t="n">
-        <v>2923503.366666667</v>
-      </c>
-      <c r="Q9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -889,29 +963,35 @@
       <c r="D10" t="n">
         <v>-0.002677866611500157</v>
       </c>
-      <c r="E10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>0.03401330847517651</v>
+      </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
         <v>483.2631420889487</v>
       </c>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
+      <c r="I10" t="n">
+        <v>2945113.633333333</v>
+      </c>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="n">
         <v>263.6363636363638</v>
       </c>
-      <c r="L10" t="inlineStr"/>
+      <c r="L10" t="n">
+        <v>-2518346</v>
+      </c>
       <c r="M10" t="n">
-        <v>483.0113333333333</v>
+        <v>-25411007</v>
       </c>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
+        <v>483.0113333333333</v>
+      </c>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="n">
         <v>489.2997559024173</v>
       </c>
-      <c r="P10" t="n">
-        <v>2945113.633333333</v>
-      </c>
-      <c r="Q10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -928,29 +1008,35 @@
       <c r="D11" t="n">
         <v>0.01512628736597943</v>
       </c>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="n">
+        <v>0.03507220677132652</v>
+      </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
         <v>484.1489801771236</v>
       </c>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
+      <c r="I11" t="n">
+        <v>3003736.633333333</v>
+      </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="n">
         <v>270.4663212435242</v>
       </c>
-      <c r="L11" t="inlineStr"/>
+      <c r="L11" t="n">
+        <v>2104030</v>
+      </c>
       <c r="M11" t="n">
-        <v>483.51</v>
+        <v>-18615625</v>
       </c>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="n">
+        <v>483.51</v>
+      </c>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="n">
         <v>489.0949114818943</v>
       </c>
-      <c r="P11" t="n">
-        <v>3003736.633333333</v>
-      </c>
-      <c r="Q11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -967,29 +1053,35 @@
       <c r="D12" t="n">
         <v>0.01996430888377621</v>
       </c>
-      <c r="E12" t="inlineStr"/>
+      <c r="E12" t="n">
+        <v>0.03601119675601534</v>
+      </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
         <v>484.8270782588708</v>
       </c>
       <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
+      <c r="I12" t="n">
+        <v>3114057.2</v>
+      </c>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="n">
         <v>284.1417910447767</v>
       </c>
-      <c r="L12" t="inlineStr"/>
+      <c r="L12" t="n">
+        <v>2833186</v>
+      </c>
       <c r="M12" t="n">
-        <v>483.7076666666667</v>
+        <v>-26133302</v>
       </c>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="n">
+        <v>483.7076666666667</v>
+      </c>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="n">
         <v>488.7849053771974</v>
       </c>
-      <c r="P12" t="n">
-        <v>3114057.2</v>
-      </c>
-      <c r="Q12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1006,29 +1098,35 @@
       <c r="D13" t="n">
         <v>0.015180637418994</v>
       </c>
-      <c r="E13" t="inlineStr"/>
+      <c r="E13" t="n">
+        <v>0.03468464322173136</v>
+      </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
         <v>486.2231826836464</v>
       </c>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
+      <c r="I13" t="n">
+        <v>3193170.333333333</v>
+      </c>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="n">
         <v>1454.838709677412</v>
       </c>
-      <c r="L13" t="inlineStr"/>
+      <c r="L13" t="n">
+        <v>2516422</v>
+      </c>
       <c r="M13" t="n">
-        <v>484.5433333333334</v>
+        <v>-34173068</v>
       </c>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
+        <v>484.5433333333334</v>
+      </c>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="n">
         <v>488.9645540239006</v>
       </c>
-      <c r="P13" t="n">
-        <v>3193170.333333333</v>
-      </c>
-      <c r="Q13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1045,29 +1143,35 @@
       <c r="D14" t="n">
         <v>0.01407416336167433</v>
       </c>
-      <c r="E14" t="inlineStr"/>
+      <c r="E14" t="n">
+        <v>0.03325130334787255</v>
+      </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
         <v>487.9033216622183</v>
       </c>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
+      <c r="I14" t="n">
+        <v>3250608.166666667</v>
+      </c>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="n">
         <v>-194.0899932840836</v>
       </c>
-      <c r="L14" t="inlineStr"/>
+      <c r="L14" t="n">
+        <v>2490171</v>
+      </c>
       <c r="M14" t="n">
-        <v>485.9623333333333</v>
+        <v>-40929047</v>
       </c>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
+        <v>485.9623333333333</v>
+      </c>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="n">
         <v>489.8193508531351</v>
       </c>
-      <c r="P14" t="n">
-        <v>3250608.166666667</v>
-      </c>
-      <c r="Q14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -1084,29 +1188,35 @@
       <c r="D15" t="n">
         <v>-0.02188355304935996</v>
       </c>
-      <c r="E15" t="inlineStr"/>
+      <c r="E15" t="n">
+        <v>0.03326504908992482</v>
+      </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
         <v>490.6633957101307</v>
       </c>
       <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
+      <c r="I15" t="n">
+        <v>3403662.333333333</v>
+      </c>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="n">
         <v>-91.59491594915943</v>
       </c>
-      <c r="L15" t="inlineStr"/>
+      <c r="L15" t="n">
+        <v>-3222618</v>
+      </c>
       <c r="M15" t="n">
-        <v>487.689</v>
+        <v>-36337422</v>
       </c>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="n">
+        <v>487.689</v>
+      </c>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="n">
         <v>491.2282716016272</v>
       </c>
-      <c r="P15" t="n">
-        <v>3403662.333333333</v>
-      </c>
-      <c r="Q15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -1123,29 +1233,35 @@
       <c r="D16" t="n">
         <v>-0.009446437391583018</v>
       </c>
-      <c r="E16" t="inlineStr"/>
+      <c r="E16" t="n">
+        <v>0.03977446001681783</v>
+      </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="n">
         <v>493.0543219827908</v>
       </c>
       <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
+      <c r="I16" t="n">
+        <v>3531330.966666667</v>
+      </c>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="n">
         <v>-114.681724845996</v>
       </c>
-      <c r="L16" t="inlineStr"/>
+      <c r="L16" t="n">
+        <v>-2954736</v>
+      </c>
       <c r="M16" t="n">
-        <v>489.39</v>
+        <v>-26062127</v>
       </c>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="n">
+        <v>489.39</v>
+      </c>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="n">
         <v>493.1867730913946</v>
       </c>
-      <c r="P16" t="n">
-        <v>3531330.966666667</v>
-      </c>
-      <c r="Q16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -1162,29 +1278,35 @@
       <c r="D17" t="n">
         <v>0.008664617825288268</v>
       </c>
-      <c r="E17" t="inlineStr"/>
+      <c r="E17" t="n">
+        <v>0.0867579276186084</v>
+      </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="n">
         <v>493.4411426438375</v>
       </c>
       <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
+      <c r="I17" t="n">
+        <v>4085534.366666667</v>
+      </c>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="n">
         <v>-455.5059523809553</v>
       </c>
-      <c r="L17" t="inlineStr"/>
+      <c r="L17" t="n">
+        <v>2460261</v>
+      </c>
       <c r="M17" t="n">
-        <v>490.0363333333333</v>
+        <v>-42688229</v>
       </c>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="n">
+        <v>490.0363333333333</v>
+      </c>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="n">
         <v>494.5741367528701</v>
       </c>
-      <c r="P17" t="n">
-        <v>4085534.366666667</v>
-      </c>
-      <c r="Q17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -1201,29 +1323,35 @@
       <c r="D18" t="n">
         <v>-0.007742842924473692</v>
       </c>
-      <c r="E18" t="inlineStr"/>
+      <c r="E18" t="n">
+        <v>0.08639123516373795</v>
+      </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="n">
         <v>497.3617351034494</v>
       </c>
       <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
+      <c r="I18" t="n">
+        <v>4200462.9</v>
+      </c>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="n">
         <v>-226.7979452054798</v>
       </c>
-      <c r="L18" t="inlineStr"/>
+      <c r="L18" t="n">
+        <v>-2250913</v>
+      </c>
       <c r="M18" t="n">
-        <v>493.1326666666666</v>
+        <v>-51056607</v>
       </c>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="n">
+        <v>493.1326666666666</v>
+      </c>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="n">
         <v>495.7475254944473</v>
       </c>
-      <c r="P18" t="n">
-        <v>4200462.9</v>
-      </c>
-      <c r="Q18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -1240,29 +1368,35 @@
       <c r="D19" t="n">
         <v>0.008884081926542997</v>
       </c>
-      <c r="E19" t="inlineStr"/>
+      <c r="E19" t="n">
+        <v>0.08640628292196673</v>
+      </c>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="n">
         <v>499.8605046983944</v>
       </c>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
+      <c r="I19" t="n">
+        <v>4240966.533333333</v>
+      </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="n">
         <v>-265.1651651651654</v>
       </c>
-      <c r="L19" t="inlineStr"/>
+      <c r="L19" t="n">
+        <v>2338044</v>
+      </c>
       <c r="M19" t="n">
-        <v>496.4696666666667</v>
+        <v>-52271716</v>
       </c>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="n">
+        <v>496.4696666666667</v>
+      </c>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="n">
         <v>497.2859755285471</v>
       </c>
-      <c r="P19" t="n">
-        <v>4240966.533333333</v>
-      </c>
-      <c r="Q19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -1279,29 +1413,35 @@
       <c r="D20" t="n">
         <v>0.01279026576480202</v>
       </c>
-      <c r="E20" t="inlineStr"/>
+      <c r="E20" t="n">
+        <v>0.08854412693456494</v>
+      </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="n">
         <v>502.4173864749558</v>
       </c>
       <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
+      <c r="I20" t="n">
+        <v>4278670.433333334</v>
+      </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="n">
         <v>-92.3683119037745</v>
       </c>
-      <c r="L20" t="inlineStr"/>
+      <c r="L20" t="n">
+        <v>2205836</v>
+      </c>
       <c r="M20" t="n">
-        <v>499.8703333333333</v>
+        <v>-51140599</v>
       </c>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="n">
+        <v>499.8703333333333</v>
+      </c>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="n">
         <v>498.6767324615503</v>
       </c>
-      <c r="P20" t="n">
-        <v>4278670.433333334</v>
-      </c>
-      <c r="Q20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -1318,29 +1458,35 @@
       <c r="D21" t="n">
         <v>0.004013268469919673</v>
       </c>
-      <c r="E21" t="inlineStr"/>
+      <c r="E21" t="n">
+        <v>0.08873294906050881</v>
+      </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
         <v>504.2069079065534</v>
       </c>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
+      <c r="I21" t="n">
+        <v>4300402.266666667</v>
+      </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="n">
         <v>-50.30940594059422</v>
       </c>
-      <c r="L21" t="inlineStr"/>
+      <c r="L21" t="n">
+        <v>2604256</v>
+      </c>
       <c r="M21" t="n">
-        <v>502.7876666666667</v>
+        <v>-50488644</v>
       </c>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
+        <v>502.7876666666667</v>
+      </c>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="n">
         <v>500.4544381485538</v>
       </c>
-      <c r="P21" t="n">
-        <v>4300402.266666667</v>
-      </c>
-      <c r="Q21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -1357,29 +1503,35 @@
       <c r="D22" t="n">
         <v>-0.01739545036903412</v>
       </c>
-      <c r="E22" t="inlineStr"/>
+      <c r="E22" t="n">
+        <v>0.08858404670506242</v>
+      </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="n">
         <v>505.999767312758</v>
       </c>
       <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
+      <c r="I22" t="n">
+        <v>4308033.066666666</v>
+      </c>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="n">
         <v>-38.81845157809562</v>
       </c>
-      <c r="L22" t="inlineStr"/>
+      <c r="L22" t="n">
+        <v>-3282142</v>
+      </c>
       <c r="M22" t="n">
-        <v>505.6143333333333</v>
+        <v>-55926080</v>
       </c>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="n">
+        <v>505.6143333333333</v>
+      </c>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="n">
         <v>502.769226986385</v>
       </c>
-      <c r="P22" t="n">
-        <v>4308033.066666666</v>
-      </c>
-      <c r="Q22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -1396,29 +1548,35 @@
       <c r="D23" t="n">
         <v>-0.002680372635625261</v>
       </c>
-      <c r="E23" t="inlineStr"/>
+      <c r="E23" t="n">
+        <v>0.08969686303251832</v>
+      </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
         <v>508.0806016874097</v>
       </c>
       <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
+      <c r="I23" t="n">
+        <v>4287313.133333334</v>
+      </c>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="n">
         <v>-45.79885423297276</v>
       </c>
-      <c r="L23" t="inlineStr"/>
+      <c r="L23" t="n">
+        <v>-2389742</v>
+      </c>
       <c r="M23" t="n">
-        <v>508.6483333333333</v>
+        <v>-49983394</v>
       </c>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="n">
+        <v>508.6483333333333</v>
+      </c>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="n">
         <v>505.3726219509633</v>
       </c>
-      <c r="P23" t="n">
-        <v>4287313.133333334</v>
-      </c>
-      <c r="Q23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -1435,29 +1593,35 @@
       <c r="D24" t="n">
         <v>-0.003723693911071635</v>
       </c>
-      <c r="E24" t="inlineStr"/>
+      <c r="E24" t="n">
+        <v>0.08969399695704329</v>
+      </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="n">
         <v>509.5930884791989</v>
       </c>
       <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
+      <c r="I24" t="n">
+        <v>4314647.266666667</v>
+      </c>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="n">
         <v>-48.714524207012</v>
       </c>
-      <c r="L24" t="inlineStr"/>
+      <c r="L24" t="n">
+        <v>-2034793</v>
+      </c>
       <c r="M24" t="n">
-        <v>510.9786666666666</v>
+        <v>-50803418</v>
       </c>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
+        <v>510.9786666666666</v>
+      </c>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="n">
         <v>507.5928027751676</v>
       </c>
-      <c r="P24" t="n">
-        <v>4314647.266666667</v>
-      </c>
-      <c r="Q24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -1474,29 +1638,35 @@
       <c r="D25" t="n">
         <v>0.01293449430075455</v>
       </c>
-      <c r="E25" t="inlineStr"/>
+      <c r="E25" t="n">
+        <v>0.09179135018978782</v>
+      </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="n">
         <v>511.2834529935612</v>
       </c>
       <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
+      <c r="I25" t="n">
+        <v>4389715.3</v>
+      </c>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="n">
         <v>-46.49458253664784</v>
       </c>
-      <c r="L25" t="inlineStr"/>
+      <c r="L25" t="n">
+        <v>2660097</v>
+      </c>
       <c r="M25" t="n">
-        <v>513.325</v>
+        <v>-53055459</v>
       </c>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="n">
+        <v>513.325</v>
+      </c>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="n">
         <v>509.878513311386</v>
       </c>
-      <c r="P25" t="n">
-        <v>4389715.3</v>
-      </c>
-      <c r="Q25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -1513,29 +1683,35 @@
       <c r="D26" t="n">
         <v>-0.008451739059037067</v>
       </c>
-      <c r="E26" t="inlineStr"/>
+      <c r="E26" t="n">
+        <v>0.09121476155296916</v>
+      </c>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="n">
         <v>513.09296796182</v>
       </c>
       <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
+      <c r="I26" t="n">
+        <v>4386259.366666666</v>
+      </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="n">
         <v>-23.80824131430136</v>
       </c>
-      <c r="L26" t="inlineStr"/>
+      <c r="L26" t="n">
+        <v>-3353225</v>
+      </c>
       <c r="M26" t="n">
-        <v>516.3823333333333</v>
+        <v>-58271975</v>
       </c>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="n">
+        <v>516.3823333333333</v>
+      </c>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="n">
         <v>512.1997900914815</v>
       </c>
-      <c r="P26" t="n">
-        <v>4386259.366666666</v>
-      </c>
-      <c r="Q26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -1552,29 +1728,35 @@
       <c r="D27" t="n">
         <v>-0.0212660747504172</v>
       </c>
-      <c r="E27" t="inlineStr"/>
+      <c r="E27" t="n">
+        <v>0.09218096384845327</v>
+      </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="n">
         <v>515.5001683078759</v>
       </c>
       <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
+      <c r="I27" t="n">
+        <v>4373421.8</v>
+      </c>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="n">
         <v>-65.08061344868312</v>
       </c>
-      <c r="L27" t="inlineStr"/>
+      <c r="L27" t="n">
+        <v>-5621945</v>
+      </c>
       <c r="M27" t="n">
-        <v>519.7433333333333</v>
+        <v>-51950652</v>
       </c>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="n">
+        <v>519.7433333333333</v>
+      </c>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="n">
         <v>515.103223890894</v>
       </c>
-      <c r="P27" t="n">
-        <v>4373421.8</v>
-      </c>
-      <c r="Q27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -1591,29 +1773,35 @@
       <c r="D28" t="n">
         <v>-0.006052514616702531</v>
       </c>
-      <c r="E28" t="inlineStr"/>
+      <c r="E28" t="n">
+        <v>0.09240243080309687</v>
+      </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="n">
         <v>518.6290500265889</v>
       </c>
       <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
+      <c r="I28" t="n">
+        <v>4314169.166666667</v>
+      </c>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="n">
         <v>-61.36447905079757</v>
       </c>
-      <c r="L28" t="inlineStr"/>
+      <c r="L28" t="n">
+        <v>-2978539</v>
+      </c>
       <c r="M28" t="n">
-        <v>522.6163333333333</v>
+        <v>-42484341</v>
       </c>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="n">
+        <v>522.6163333333333</v>
+      </c>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="n">
         <v>517.931722090266</v>
       </c>
-      <c r="P28" t="n">
-        <v>4314169.166666667</v>
-      </c>
-      <c r="Q28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
@@ -1630,29 +1818,35 @@
       <c r="D29" t="n">
         <v>-0.0108802118454463</v>
       </c>
-      <c r="E29" t="inlineStr"/>
+      <c r="E29" t="n">
+        <v>0.09241211326084665</v>
+      </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="n">
         <v>520.0199197779642</v>
       </c>
       <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
+      <c r="I29" t="n">
+        <v>4291991.966666667</v>
+      </c>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="n">
         <v>-51.84837092731877</v>
       </c>
-      <c r="L29" t="inlineStr"/>
+      <c r="L29" t="n">
+        <v>-2487870</v>
+      </c>
       <c r="M29" t="n">
-        <v>524.8676666666667</v>
+        <v>-41819025</v>
       </c>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="n">
+        <v>524.8676666666667</v>
+      </c>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="n">
         <v>520.2525305102844</v>
       </c>
-      <c r="P29" t="n">
-        <v>4291991.966666667</v>
-      </c>
-      <c r="Q29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
@@ -1669,29 +1863,35 @@
       <c r="D30" t="n">
         <v>0.01693272646214883</v>
       </c>
-      <c r="E30" t="inlineStr"/>
+      <c r="E30" t="n">
+        <v>0.09250331980762065</v>
+      </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="n">
         <v>521.4641109314838</v>
       </c>
       <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
+      <c r="I30" t="n">
+        <v>4317315.366666666</v>
+      </c>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="n">
         <v>-57.78631284916239</v>
       </c>
-      <c r="L30" t="inlineStr"/>
+      <c r="L30" t="n">
+        <v>2548566</v>
+      </c>
       <c r="M30" t="n">
-        <v>527.0433333333334</v>
+        <v>-42578727</v>
       </c>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="n">
+        <v>527.0433333333334</v>
+      </c>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="n">
         <v>522.5306360627178</v>
       </c>
-      <c r="P30" t="n">
-        <v>4317315.366666666</v>
-      </c>
-      <c r="Q30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
@@ -1708,29 +1908,35 @@
       <c r="D31" t="n">
         <v>-0.001733031174413036</v>
       </c>
-      <c r="E31" t="inlineStr"/>
+      <c r="E31" t="n">
+        <v>0.09224536645111683</v>
+      </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="n">
         <v>523.2896580674462</v>
       </c>
       <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
+      <c r="I31" t="n">
+        <v>4374068.266666667</v>
+      </c>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="n">
         <v>-52.77214334009503</v>
       </c>
-      <c r="L31" t="inlineStr"/>
+      <c r="L31" t="n">
+        <v>-3439211</v>
+      </c>
       <c r="M31" t="n">
-        <v>529.3076666666667</v>
+        <v>-40876140</v>
       </c>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="n">
+        <v>529.3076666666667</v>
+      </c>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="n">
         <v>524.5982661360086</v>
       </c>
-      <c r="P31" t="n">
-        <v>4374068.266666667</v>
-      </c>
-      <c r="Q31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
@@ -1747,29 +1953,35 @@
       <c r="D32" t="n">
         <v>-0.004093687253180711</v>
       </c>
-      <c r="E32" t="inlineStr"/>
+      <c r="E32" t="n">
+        <v>0.09393516349109694</v>
+      </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="n">
         <v>525.3393964797115</v>
       </c>
       <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
+      <c r="I32" t="n">
+        <v>4410977.366666666</v>
+      </c>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="n">
         <v>-504.223433242511</v>
       </c>
-      <c r="L32" t="inlineStr"/>
+      <c r="L32" t="n">
+        <v>-4972655</v>
+      </c>
       <c r="M32" t="n">
-        <v>531.6130000000001</v>
+        <v>-32890445</v>
       </c>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="n">
+        <v>531.6130000000001</v>
+      </c>
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="n">
         <v>527.3788362143541</v>
       </c>
-      <c r="P32" t="n">
-        <v>4410977.366666666</v>
-      </c>
-      <c r="Q32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
@@ -1786,29 +1998,35 @@
       <c r="D33" t="n">
         <v>-0.02012017635142271</v>
       </c>
-      <c r="E33" t="inlineStr"/>
+      <c r="E33" t="n">
+        <v>0.09393841981142968</v>
+      </c>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="n">
         <v>527.3142887263923</v>
       </c>
       <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
+      <c r="I33" t="n">
+        <v>4412668.766666667</v>
+      </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="n">
         <v>-44.40844732421425</v>
       </c>
-      <c r="L33" t="inlineStr"/>
+      <c r="L33" t="n">
+        <v>-3403327</v>
+      </c>
       <c r="M33" t="n">
-        <v>533.3613333333334</v>
+        <v>-32941187</v>
       </c>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="n">
+        <v>533.3613333333334</v>
+      </c>
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="n">
         <v>530.2932387118958</v>
       </c>
-      <c r="P33" t="n">
-        <v>4412668.766666667</v>
-      </c>
-      <c r="Q33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
@@ -1825,29 +2043,35 @@
       <c r="D34" t="n">
         <v>-0.004416702287305618</v>
       </c>
-      <c r="E34" t="inlineStr"/>
+      <c r="E34" t="n">
+        <v>0.09350694208025999</v>
+      </c>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="n">
         <v>528.7167103723795</v>
       </c>
       <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
+      <c r="I34" t="n">
+        <v>4449009.033333333</v>
+      </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="n">
         <v>-48.35380193362971</v>
       </c>
-      <c r="L34" t="inlineStr"/>
+      <c r="L34" t="n">
+        <v>-2604428</v>
+      </c>
       <c r="M34" t="n">
-        <v>535.075</v>
+        <v>-34031395</v>
       </c>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="n">
+        <v>535.075</v>
+      </c>
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="n">
         <v>533.2713931058197</v>
       </c>
-      <c r="P34" t="n">
-        <v>4449009.033333333</v>
-      </c>
-      <c r="Q34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -1864,29 +2088,35 @@
       <c r="D35" t="n">
         <v>-0.005752537585141049</v>
       </c>
-      <c r="E35" t="inlineStr"/>
+      <c r="E35" t="n">
+        <v>0.09355522566601722</v>
+      </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="n">
         <v>529.9480388377322</v>
       </c>
       <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
+      <c r="I35" t="n">
+        <v>4581113.7</v>
+      </c>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="n">
         <v>-46.30301513824617</v>
       </c>
-      <c r="L35" t="inlineStr"/>
+      <c r="L35" t="n">
+        <v>-3083273</v>
+      </c>
       <c r="M35" t="n">
-        <v>536.5716666666667</v>
+        <v>-37994535</v>
       </c>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="n">
+        <v>536.5716666666667</v>
+      </c>
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="n">
         <v>535.7721788372555</v>
       </c>
-      <c r="P35" t="n">
-        <v>4581113.7</v>
-      </c>
-      <c r="Q35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
@@ -1903,29 +2133,35 @@
       <c r="D36" t="n">
         <v>-0.004986649715955416</v>
       </c>
-      <c r="E36" t="inlineStr"/>
+      <c r="E36" t="n">
+        <v>0.1014303964785909</v>
+      </c>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="n">
         <v>531.7961421568878</v>
       </c>
       <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
+      <c r="I36" t="n">
+        <v>4822616.366666666</v>
+      </c>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="n">
         <v>-95.54260243442516</v>
       </c>
-      <c r="L36" t="inlineStr"/>
+      <c r="L36" t="n">
+        <v>-2056030</v>
+      </c>
       <c r="M36" t="n">
-        <v>538.1533333333333</v>
+        <v>-45239615</v>
       </c>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="n">
+        <v>538.1533333333333</v>
+      </c>
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="n">
         <v>538.2937084122386</v>
       </c>
-      <c r="P36" t="n">
-        <v>4822616.366666666</v>
-      </c>
-      <c r="Q36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
@@ -1942,29 +2178,35 @@
       <c r="D37" t="n">
         <v>0.0003964321161937789</v>
       </c>
-      <c r="E37" t="inlineStr"/>
+      <c r="E37" t="n">
+        <v>0.1018954089749918</v>
+      </c>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="n">
         <v>533.687676822758</v>
       </c>
       <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
+      <c r="I37" t="n">
+        <v>4876660.633333334</v>
+      </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="n">
         <v>-136.8868124867276</v>
       </c>
-      <c r="L37" t="inlineStr"/>
+      <c r="L37" t="n">
+        <v>3897003</v>
+      </c>
       <c r="M37" t="n">
-        <v>541.0983333333332</v>
+        <v>-46860943</v>
       </c>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="n">
+        <v>541.0983333333332</v>
+      </c>
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="n">
         <v>540.7905158889447</v>
       </c>
-      <c r="P37" t="n">
-        <v>4876660.633333334</v>
-      </c>
-      <c r="Q37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
@@ -1981,29 +2223,35 @@
       <c r="D38" t="n">
         <v>-0.006324131749468442</v>
       </c>
-      <c r="E38" t="inlineStr"/>
+      <c r="E38" t="n">
+        <v>0.1019961788166949</v>
+      </c>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="n">
         <v>535.2706984893236</v>
       </c>
       <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr"/>
+      <c r="I38" t="n">
+        <v>4800597.833333333</v>
+      </c>
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="n">
         <v>-124.4384198295896</v>
       </c>
-      <c r="L38" t="inlineStr"/>
+      <c r="L38" t="n">
+        <v>-4228415</v>
+      </c>
       <c r="M38" t="n">
-        <v>544.4336666666667</v>
+        <v>-49142827</v>
       </c>
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="n">
+        <v>544.4336666666667</v>
+      </c>
+      <c r="P38" t="inlineStr"/>
+      <c r="Q38" t="n">
         <v>543.2864135364581</v>
       </c>
-      <c r="P38" t="n">
-        <v>4800597.833333333</v>
-      </c>
-      <c r="Q38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
@@ -2020,29 +2268,35 @@
       <c r="D39" t="n">
         <v>0.0007291862014220385</v>
       </c>
-      <c r="E39" t="inlineStr"/>
+      <c r="E39" t="n">
+        <v>0.102147721850943</v>
+      </c>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="n">
         <v>537.5778891970526</v>
       </c>
       <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr"/>
+      <c r="I39" t="n">
+        <v>4759158.6</v>
+      </c>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="n">
         <v>-217.5542406311637</v>
       </c>
-      <c r="L39" t="inlineStr"/>
+      <c r="L39" t="n">
+        <v>2813329</v>
+      </c>
       <c r="M39" t="n">
-        <v>547.6833333333333</v>
+        <v>-47899650</v>
       </c>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="n">
+        <v>547.6833333333333</v>
+      </c>
+      <c r="P39" t="inlineStr"/>
+      <c r="Q39" t="n">
         <v>545.9682351596621</v>
       </c>
-      <c r="P39" t="n">
-        <v>4759158.6</v>
-      </c>
-      <c r="Q39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
@@ -2059,29 +2313,35 @@
       <c r="D40" t="n">
         <v>0.01531691231174293</v>
       </c>
-      <c r="E40" t="inlineStr"/>
+      <c r="E40" t="n">
+        <v>0.1025372709846265</v>
+      </c>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="n">
         <v>539.3801321335113</v>
       </c>
       <c r="H40" t="inlineStr"/>
-      <c r="I40" t="inlineStr"/>
+      <c r="I40" t="n">
+        <v>4742622.266666667</v>
+      </c>
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="n">
         <v>-204.3073650624832</v>
       </c>
-      <c r="L40" t="inlineStr"/>
+      <c r="L40" t="n">
+        <v>4277036</v>
+      </c>
       <c r="M40" t="n">
-        <v>551.158</v>
+        <v>-53030218</v>
       </c>
       <c r="N40" t="inlineStr"/>
       <c r="O40" t="n">
+        <v>551.158</v>
+      </c>
+      <c r="P40" t="inlineStr"/>
+      <c r="Q40" t="n">
         <v>548.614320343087</v>
       </c>
-      <c r="P40" t="n">
-        <v>4742622.266666667</v>
-      </c>
-      <c r="Q40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
@@ -2098,29 +2358,35 @@
       <c r="D41" t="n">
         <v>-0.02321107002994438</v>
       </c>
-      <c r="E41" t="inlineStr"/>
+      <c r="E41" t="n">
+        <v>0.1027352127155134</v>
+      </c>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="n">
         <v>541.672827447213</v>
       </c>
       <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr"/>
+      <c r="I41" t="n">
+        <v>4669766.166666667</v>
+      </c>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="n">
         <v>-101.0377082724348</v>
       </c>
-      <c r="L41" t="inlineStr"/>
+      <c r="L41" t="n">
+        <v>-5413647</v>
+      </c>
       <c r="M41" t="n">
-        <v>555.1573333333333</v>
+        <v>-55215901</v>
       </c>
       <c r="N41" t="inlineStr"/>
       <c r="O41" t="n">
+        <v>555.1573333333333</v>
+      </c>
+      <c r="P41" t="inlineStr"/>
+      <c r="Q41" t="n">
         <v>551.4684114012309</v>
       </c>
-      <c r="P41" t="n">
-        <v>4669766.166666667</v>
-      </c>
-      <c r="Q41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
@@ -2137,29 +2403,35 @@
       <c r="D42" t="n">
         <v>-0.01531488895132149</v>
       </c>
-      <c r="E42" t="inlineStr"/>
+      <c r="E42" t="n">
+        <v>0.1024068905138023</v>
+      </c>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="n">
         <v>544.3315386711545</v>
       </c>
       <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr"/>
+      <c r="I42" t="n">
+        <v>4549834</v>
+      </c>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="n">
         <v>-115.8344504021448</v>
       </c>
-      <c r="L42" t="inlineStr"/>
+      <c r="L42" t="n">
+        <v>-5206580</v>
+      </c>
       <c r="M42" t="n">
-        <v>559.0353333333334</v>
+        <v>-47986572</v>
       </c>
       <c r="N42" t="inlineStr"/>
       <c r="O42" t="n">
+        <v>559.0353333333334</v>
+      </c>
+      <c r="P42" t="inlineStr"/>
+      <c r="Q42" t="n">
         <v>555.0510604633847</v>
       </c>
-      <c r="P42" t="n">
-        <v>4549834</v>
-      </c>
-      <c r="Q42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
@@ -2176,29 +2448,35 @@
       <c r="D43" t="n">
         <v>-0.003941062265584883</v>
       </c>
-      <c r="E43" t="inlineStr"/>
+      <c r="E43" t="n">
+        <v>0.1028387894383462</v>
+      </c>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="n">
         <v>546.8593611778165</v>
       </c>
       <c r="H43" t="inlineStr"/>
-      <c r="I43" t="inlineStr"/>
+      <c r="I43" t="n">
+        <v>4453408.8</v>
+      </c>
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="n">
         <v>-193.9231891103547</v>
       </c>
-      <c r="L43" t="inlineStr"/>
+      <c r="L43" t="n">
+        <v>-4239557</v>
+      </c>
       <c r="M43" t="n">
-        <v>562.522</v>
+        <v>-40466168</v>
       </c>
       <c r="N43" t="inlineStr"/>
       <c r="O43" t="n">
+        <v>562.522</v>
+      </c>
+      <c r="P43" t="inlineStr"/>
+      <c r="Q43" t="n">
         <v>558.0718232539629</v>
       </c>
-      <c r="P43" t="n">
-        <v>4453408.8</v>
-      </c>
-      <c r="Q43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
@@ -2215,29 +2493,35 @@
       <c r="D44" t="n">
         <v>0.01416380376001936</v>
       </c>
-      <c r="E44" t="inlineStr"/>
+      <c r="E44" t="n">
+        <v>0.1042635955866898</v>
+      </c>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="n">
         <v>549.3040852719537</v>
       </c>
       <c r="H44" t="inlineStr"/>
-      <c r="I44" t="inlineStr"/>
+      <c r="I44" t="n">
+        <v>4426631.7</v>
+      </c>
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="n">
         <v>-288.083578191315</v>
       </c>
-      <c r="L44" t="inlineStr"/>
+      <c r="L44" t="n">
+        <v>7081796</v>
+      </c>
       <c r="M44" t="n">
-        <v>565.4553333333333</v>
+        <v>-39662855</v>
       </c>
       <c r="N44" t="inlineStr"/>
       <c r="O44" t="n">
+        <v>565.4553333333333</v>
+      </c>
+      <c r="P44" t="inlineStr"/>
+      <c r="Q44" t="n">
         <v>560.7567765818224</v>
       </c>
-      <c r="P44" t="n">
-        <v>4426631.7</v>
-      </c>
-      <c r="Q44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
@@ -2254,29 +2538,35 @@
       <c r="D45" t="n">
         <v>0.04253761577424964</v>
       </c>
-      <c r="E45" t="inlineStr"/>
+      <c r="E45" t="n">
+        <v>0.103657478779518</v>
+      </c>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="n">
         <v>552.2149281445055</v>
       </c>
       <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr"/>
+      <c r="I45" t="n">
+        <v>4261613.333333333</v>
+      </c>
       <c r="J45" t="inlineStr"/>
       <c r="K45" t="n">
         <v>-209.4486150660103</v>
       </c>
-      <c r="L45" t="inlineStr"/>
+      <c r="L45" t="n">
+        <v>7052677</v>
+      </c>
       <c r="M45" t="n">
-        <v>569.099</v>
+        <v>-48875896</v>
       </c>
       <c r="N45" t="inlineStr"/>
       <c r="O45" t="n">
+        <v>569.099</v>
+      </c>
+      <c r="P45" t="inlineStr"/>
+      <c r="Q45" t="n">
         <v>563.4855197943618</v>
       </c>
-      <c r="P45" t="n">
-        <v>4261613.333333333</v>
-      </c>
-      <c r="Q45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
@@ -2293,29 +2583,35 @@
       <c r="D46" t="n">
         <v>-0.147012284002729</v>
       </c>
-      <c r="E46" t="inlineStr"/>
+      <c r="E46" t="n">
+        <v>0.1005776835781166</v>
+      </c>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="n">
         <v>556.109880074659</v>
       </c>
       <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
+      <c r="I46" t="n">
+        <v>4111282.866666667</v>
+      </c>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="n">
         <v>-87.48897383122568</v>
       </c>
-      <c r="L46" t="inlineStr"/>
+      <c r="L46" t="n">
+        <v>-19580838</v>
+      </c>
       <c r="M46" t="n">
-        <v>573.129</v>
+        <v>-53385810</v>
       </c>
       <c r="N46" t="inlineStr"/>
       <c r="O46" t="n">
+        <v>573.129</v>
+      </c>
+      <c r="P46" t="inlineStr"/>
+      <c r="Q46" t="n">
         <v>566.9079694353522</v>
       </c>
-      <c r="P46" t="n">
-        <v>4111282.866666667</v>
-      </c>
-      <c r="Q46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
@@ -2332,29 +2628,35 @@
       <c r="D47" t="n">
         <v>-0.005419593684898416</v>
       </c>
-      <c r="E47" t="inlineStr"/>
+      <c r="E47" t="n">
+        <v>0.06664082041118792</v>
+      </c>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="n">
         <v>569.0785881349376</v>
       </c>
       <c r="H47" t="inlineStr"/>
-      <c r="I47" t="inlineStr"/>
+      <c r="I47" t="n">
+        <v>3514842.033333333</v>
+      </c>
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="n">
         <v>391.2404467960009</v>
       </c>
-      <c r="L47" t="inlineStr"/>
+      <c r="L47" t="n">
+        <v>-5908117</v>
+      </c>
       <c r="M47" t="n">
-        <v>577.6440000000001</v>
+        <v>-32117359</v>
       </c>
       <c r="N47" t="inlineStr"/>
       <c r="O47" t="n">
+        <v>577.6440000000001</v>
+      </c>
+      <c r="P47" t="inlineStr"/>
+      <c r="Q47" t="n">
         <v>572.0423121550317</v>
       </c>
-      <c r="P47" t="n">
-        <v>3514842.033333333</v>
-      </c>
-      <c r="Q47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
@@ -2371,29 +2673,35 @@
       <c r="D48" t="n">
         <v>-0.009699127818073805</v>
       </c>
-      <c r="E48" t="inlineStr"/>
+      <c r="E48" t="n">
+        <v>0.06702163413979741</v>
+      </c>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="n">
         <v>570.2700614860962</v>
       </c>
       <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr"/>
+      <c r="I48" t="n">
+        <v>3406797.3</v>
+      </c>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="n">
         <v>229.071706503613</v>
       </c>
-      <c r="L48" t="inlineStr"/>
+      <c r="L48" t="n">
+        <v>-3466022</v>
+      </c>
       <c r="M48" t="n">
-        <v>579.2216666666667</v>
+        <v>-28876017</v>
       </c>
       <c r="N48" t="inlineStr"/>
       <c r="O48" t="n">
+        <v>579.2216666666667</v>
+      </c>
+      <c r="P48" t="inlineStr"/>
+      <c r="Q48" t="n">
         <v>572.1521267864132</v>
       </c>
-      <c r="P48" t="n">
-        <v>3406797.3</v>
-      </c>
-      <c r="Q48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
@@ -2410,29 +2718,35 @@
       <c r="D49" t="n">
         <v>0.03285774192560975</v>
       </c>
-      <c r="E49" t="inlineStr"/>
+      <c r="E49" t="n">
+        <v>0.06692326564188041</v>
+      </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="n">
         <v>571.306737733419</v>
       </c>
       <c r="H49" t="inlineStr"/>
-      <c r="I49" t="inlineStr"/>
+      <c r="I49" t="n">
+        <v>3358177.633333333</v>
+      </c>
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="n">
         <v>202.9049729197433</v>
       </c>
-      <c r="L49" t="inlineStr"/>
+      <c r="L49" t="n">
+        <v>3469161</v>
+      </c>
       <c r="M49" t="n">
-        <v>581.0353333333334</v>
+        <v>-27417427</v>
       </c>
       <c r="N49" t="inlineStr"/>
       <c r="O49" t="n">
+        <v>581.0353333333334</v>
+      </c>
+      <c r="P49" t="inlineStr"/>
+      <c r="Q49" t="n">
         <v>572.0557217372003</v>
       </c>
-      <c r="P49" t="n">
-        <v>3358177.633333333</v>
-      </c>
-      <c r="Q49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
@@ -2449,29 +2763,35 @@
       <c r="D50" t="n">
         <v>0.01570020829863328</v>
       </c>
-      <c r="E50" t="inlineStr"/>
+      <c r="E50" t="n">
+        <v>0.06598183981524074</v>
+      </c>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="n">
         <v>572.9198369735478</v>
       </c>
       <c r="H50" t="inlineStr"/>
-      <c r="I50" t="inlineStr"/>
+      <c r="I50" t="n">
+        <v>3349611.833333333</v>
+      </c>
       <c r="J50" t="inlineStr"/>
       <c r="K50" t="n">
         <v>344.1383036196637</v>
       </c>
-      <c r="L50" t="inlineStr"/>
+      <c r="L50" t="n">
+        <v>2857791</v>
+      </c>
       <c r="M50" t="n">
-        <v>582.7383333333332</v>
+        <v>-27674401</v>
       </c>
       <c r="N50" t="inlineStr"/>
       <c r="O50" t="n">
+        <v>582.7383333333332</v>
+      </c>
+      <c r="P50" t="inlineStr"/>
+      <c r="Q50" t="n">
         <v>571.5671508225245</v>
       </c>
-      <c r="P50" t="n">
-        <v>3349611.833333333</v>
-      </c>
-      <c r="Q50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
@@ -2488,29 +2808,35 @@
       <c r="D51" t="n">
         <v>-0.00785393978778437</v>
       </c>
-      <c r="E51" t="inlineStr"/>
+      <c r="E51" t="n">
+        <v>0.06540724057847283</v>
+      </c>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="n">
         <v>574.1566486856885</v>
       </c>
       <c r="H51" t="inlineStr"/>
-      <c r="I51" t="inlineStr"/>
+      <c r="I51" t="n">
+        <v>3325613.166666667</v>
+      </c>
       <c r="J51" t="inlineStr"/>
       <c r="K51" t="n">
         <v>1092.842942345903</v>
       </c>
-      <c r="L51" t="inlineStr"/>
+      <c r="L51" t="n">
+        <v>-2833180</v>
+      </c>
       <c r="M51" t="n">
-        <v>584.522</v>
+        <v>-32670023</v>
       </c>
       <c r="N51" t="inlineStr"/>
       <c r="O51" t="n">
+        <v>584.522</v>
+      </c>
+      <c r="P51" t="inlineStr"/>
+      <c r="Q51" t="n">
         <v>572.3359198447675</v>
       </c>
-      <c r="P51" t="n">
-        <v>3325613.166666667</v>
-      </c>
-      <c r="Q51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
@@ -2527,29 +2853,35 @@
       <c r="D52" t="n">
         <v>0.02356518205292968</v>
       </c>
-      <c r="E52" t="inlineStr"/>
+      <c r="E52" t="n">
+        <v>0.06728576494287829</v>
+      </c>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="n">
         <v>576.6180122600018</v>
       </c>
       <c r="H52" t="inlineStr"/>
-      <c r="I52" t="inlineStr"/>
+      <c r="I52" t="n">
+        <v>3358047.333333333</v>
+      </c>
       <c r="J52" t="inlineStr"/>
       <c r="K52" t="n">
         <v>-159.7965116279059</v>
       </c>
-      <c r="L52" t="inlineStr"/>
+      <c r="L52" t="n">
+        <v>2660544</v>
+      </c>
       <c r="M52" t="n">
-        <v>586.8850000000001</v>
+        <v>-26030638</v>
       </c>
       <c r="N52" t="inlineStr"/>
       <c r="O52" t="n">
+        <v>586.8850000000001</v>
+      </c>
+      <c r="P52" t="inlineStr"/>
+      <c r="Q52" t="n">
         <v>573.7597763857859</v>
       </c>
-      <c r="P52" t="n">
-        <v>3358047.333333333</v>
-      </c>
-      <c r="Q52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
@@ -2566,29 +2898,35 @@
       <c r="D53" t="n">
         <v>-0.003217121523178434</v>
       </c>
-      <c r="E53" t="inlineStr"/>
+      <c r="E53" t="n">
+        <v>0.06649403132514584</v>
+      </c>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="n">
         <v>578.0456526953902</v>
       </c>
       <c r="H53" t="inlineStr"/>
-      <c r="I53" t="inlineStr"/>
+      <c r="I53" t="n">
+        <v>3369330.266666667</v>
+      </c>
       <c r="J53" t="inlineStr"/>
       <c r="K53" t="n">
         <v>-68.24752314438834</v>
       </c>
-      <c r="L53" t="inlineStr"/>
+      <c r="L53" t="n">
+        <v>-3209766</v>
+      </c>
       <c r="M53" t="n">
-        <v>588.5663333333334</v>
+        <v>-25692150</v>
       </c>
       <c r="N53" t="inlineStr"/>
       <c r="O53" t="n">
+        <v>588.5663333333334</v>
+      </c>
+      <c r="P53" t="inlineStr"/>
+      <c r="Q53" t="n">
         <v>574.9818299296331</v>
       </c>
-      <c r="P53" t="n">
-        <v>3369330.266666667</v>
-      </c>
-      <c r="Q53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
@@ -2605,29 +2943,35 @@
       <c r="D54" t="n">
         <v>-0.04152360575955072</v>
       </c>
-      <c r="E54" t="inlineStr"/>
+      <c r="E54" t="n">
+        <v>0.06661278084842709</v>
+      </c>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="n">
         <v>579.6790681838075</v>
       </c>
       <c r="H54" t="inlineStr"/>
-      <c r="I54" t="inlineStr"/>
+      <c r="I54" t="n">
+        <v>3353120.166666667</v>
+      </c>
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="n">
         <v>-78.51007887817684</v>
       </c>
-      <c r="L54" t="inlineStr"/>
+      <c r="L54" t="n">
+        <v>-4286834</v>
+      </c>
       <c r="M54" t="n">
-        <v>590.3693333333334</v>
+        <v>-25205847</v>
       </c>
       <c r="N54" t="inlineStr"/>
       <c r="O54" t="n">
+        <v>590.3693333333334</v>
+      </c>
+      <c r="P54" t="inlineStr"/>
+      <c r="Q54" t="n">
         <v>577.1812664765044</v>
       </c>
-      <c r="P54" t="n">
-        <v>3353120.166666667</v>
-      </c>
-      <c r="Q54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
@@ -2644,29 +2988,35 @@
       <c r="D55" t="n">
         <v>-0.005250830858353872</v>
       </c>
-      <c r="E55" t="inlineStr"/>
+      <c r="E55" t="n">
+        <v>0.06352919850384618</v>
+      </c>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="n">
         <v>582.2254459518539</v>
       </c>
       <c r="H55" t="inlineStr"/>
-      <c r="I55" t="inlineStr"/>
+      <c r="I55" t="n">
+        <v>3359825.7</v>
+      </c>
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="n">
         <v>-102.0273348519359</v>
       </c>
-      <c r="L55" t="inlineStr"/>
+      <c r="L55" t="n">
+        <v>-2556419</v>
+      </c>
       <c r="M55" t="n">
-        <v>592.3276666666667</v>
+        <v>-25407013</v>
       </c>
       <c r="N55" t="inlineStr"/>
       <c r="O55" t="n">
+        <v>592.3276666666667</v>
+      </c>
+      <c r="P55" t="inlineStr"/>
+      <c r="Q55" t="n">
         <v>579.4116986472978</v>
       </c>
-      <c r="P55" t="n">
-        <v>3359825.7</v>
-      </c>
-      <c r="Q55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
@@ -2683,29 +3033,35 @@
       <c r="D56" t="n">
         <v>0.01882995142619937</v>
       </c>
-      <c r="E56" t="inlineStr"/>
+      <c r="E56" t="n">
+        <v>0.06572839836790101</v>
+      </c>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="n">
         <v>583.6632133039798</v>
       </c>
       <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
+      <c r="I56" t="n">
+        <v>3399789.666666667</v>
+      </c>
       <c r="J56" t="inlineStr"/>
       <c r="K56" t="n">
         <v>-79.58422174840049</v>
       </c>
-      <c r="L56" t="inlineStr"/>
+      <c r="L56" t="n">
+        <v>2968098</v>
+      </c>
       <c r="M56" t="n">
-        <v>593.7813333333335</v>
+        <v>-19095256</v>
       </c>
       <c r="N56" t="inlineStr"/>
       <c r="O56" t="n">
+        <v>593.7813333333335</v>
+      </c>
+      <c r="P56" t="inlineStr"/>
+      <c r="Q56" t="n">
         <v>580.2028502781459</v>
       </c>
-      <c r="P56" t="n">
-        <v>3399789.666666667</v>
-      </c>
-      <c r="Q56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
@@ -2722,29 +3078,35 @@
       <c r="D57" t="n">
         <v>0.01521475262818406</v>
       </c>
-      <c r="E57" t="inlineStr"/>
+      <c r="E57" t="n">
+        <v>0.06480679263056284</v>
+      </c>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="n">
         <v>584.3097739853628</v>
       </c>
       <c r="H57" t="inlineStr"/>
-      <c r="I57" t="inlineStr"/>
+      <c r="I57" t="n">
+        <v>3393973.4</v>
+      </c>
       <c r="J57" t="inlineStr"/>
       <c r="K57" t="n">
         <v>-81.845987765383</v>
       </c>
-      <c r="L57" t="inlineStr"/>
+      <c r="L57" t="n">
+        <v>3844366</v>
+      </c>
       <c r="M57" t="n">
-        <v>594.5403333333335</v>
+        <v>-24856964</v>
       </c>
       <c r="N57" t="inlineStr"/>
       <c r="O57" t="n">
+        <v>594.5403333333335</v>
+      </c>
+      <c r="P57" t="inlineStr"/>
+      <c r="Q57" t="n">
         <v>580.84235719388</v>
       </c>
-      <c r="P57" t="n">
-        <v>3393973.4</v>
-      </c>
-      <c r="Q57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
@@ -2761,29 +3123,35 @@
       <c r="D58" t="n">
         <v>-0.00121342753793563</v>
       </c>
-      <c r="E58" t="inlineStr"/>
+      <c r="E58" t="n">
+        <v>0.06411273250622607</v>
+      </c>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="n">
         <v>585.5318501755251</v>
       </c>
       <c r="H58" t="inlineStr"/>
-      <c r="I58" t="inlineStr"/>
+      <c r="I58" t="n">
+        <v>3352104.3</v>
+      </c>
       <c r="J58" t="inlineStr"/>
       <c r="K58" t="n">
         <v>-57.84788380446662</v>
       </c>
-      <c r="L58" t="inlineStr"/>
+      <c r="L58" t="n">
+        <v>-2313223</v>
+      </c>
       <c r="M58" t="n">
-        <v>595.7343333333333</v>
+        <v>-31289623</v>
       </c>
       <c r="N58" t="inlineStr"/>
       <c r="O58" t="n">
+        <v>595.7343333333333</v>
+      </c>
+      <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="n">
         <v>582.2604507934579</v>
       </c>
-      <c r="P58" t="n">
-        <v>3352104.3</v>
-      </c>
-      <c r="Q58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
@@ -2800,29 +3168,35 @@
       <c r="D59" t="n">
         <v>-0.01435822576857948</v>
       </c>
-      <c r="E59" t="inlineStr"/>
+      <c r="E59" t="n">
+        <v>0.06415443490003665</v>
+      </c>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="n">
         <v>586.5660730762121</v>
       </c>
       <c r="H59" t="inlineStr"/>
-      <c r="I59" t="inlineStr"/>
+      <c r="I59" t="n">
+        <v>3345866.733333333</v>
+      </c>
       <c r="J59" t="inlineStr"/>
       <c r="K59" t="n">
         <v>-83.71454711802383</v>
       </c>
-      <c r="L59" t="inlineStr"/>
+      <c r="L59" t="n">
+        <v>-3247572</v>
+      </c>
       <c r="M59" t="n">
-        <v>597.263</v>
+        <v>-26850304</v>
       </c>
       <c r="N59" t="inlineStr"/>
       <c r="O59" t="n">
+        <v>597.263</v>
+      </c>
+      <c r="P59" t="inlineStr"/>
+      <c r="Q59" t="n">
         <v>584.3597922274895</v>
       </c>
-      <c r="P59" t="n">
-        <v>3345866.733333333</v>
-      </c>
-      <c r="Q59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
@@ -2839,29 +3213,35 @@
       <c r="D60" t="n">
         <v>0.01264021426031814</v>
       </c>
-      <c r="E60" t="inlineStr"/>
+      <c r="E60" t="n">
+        <v>0.0638290544444587</v>
+      </c>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="n">
         <v>587.8373411078838</v>
       </c>
       <c r="H60" t="inlineStr"/>
-      <c r="I60" t="inlineStr"/>
+      <c r="I60" t="n">
+        <v>3286686.566666667</v>
+      </c>
       <c r="J60" t="inlineStr"/>
       <c r="K60" t="n">
         <v>-65.33847472150813</v>
       </c>
-      <c r="L60" t="inlineStr"/>
+      <c r="L60" t="n">
+        <v>4251153</v>
+      </c>
       <c r="M60" t="n">
-        <v>598.7313333333334</v>
+        <v>-25074899</v>
       </c>
       <c r="N60" t="inlineStr"/>
       <c r="O60" t="n">
+        <v>598.7313333333334</v>
+      </c>
+      <c r="P60" t="inlineStr"/>
+      <c r="Q60" t="n">
         <v>586.5577089328335</v>
       </c>
-      <c r="P60" t="n">
-        <v>3286686.566666667</v>
-      </c>
-      <c r="Q60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
@@ -2878,29 +3258,35 @@
       <c r="D61" t="n">
         <v>0.02909436110842467</v>
       </c>
-      <c r="E61" t="inlineStr"/>
+      <c r="E61" t="n">
+        <v>0.06371721141515538</v>
+      </c>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="n">
         <v>589.2730752119587</v>
       </c>
       <c r="H61" t="inlineStr"/>
-      <c r="I61" t="inlineStr"/>
+      <c r="I61" t="n">
+        <v>3222709.133333333</v>
+      </c>
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="n">
         <v>-47.60206591244474</v>
       </c>
-      <c r="L61" t="inlineStr"/>
+      <c r="L61" t="n">
+        <v>4546484</v>
+      </c>
       <c r="M61" t="n">
-        <v>599.965</v>
+        <v>-26994222</v>
       </c>
       <c r="N61" t="inlineStr"/>
       <c r="O61" t="n">
+        <v>599.965</v>
+      </c>
+      <c r="P61" t="inlineStr"/>
+      <c r="Q61" t="n">
         <v>588.3561716178565</v>
       </c>
-      <c r="P61" t="n">
-        <v>3222709.133333333</v>
-      </c>
-      <c r="Q61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
@@ -2917,29 +3303,35 @@
       <c r="D62" t="n">
         <v>-0.001765652030599973</v>
       </c>
-      <c r="E62" t="inlineStr"/>
+      <c r="E62" t="n">
+        <v>0.06167235567272367</v>
+      </c>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="n">
         <v>591.0410385216029</v>
       </c>
       <c r="H62" t="inlineStr"/>
-      <c r="I62" t="inlineStr"/>
+      <c r="I62" t="n">
+        <v>3142349.333333333</v>
+      </c>
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="n">
         <v>-32.86473323002002</v>
       </c>
-      <c r="L62" t="inlineStr"/>
+      <c r="L62" t="n">
+        <v>-5023397</v>
+      </c>
       <c r="M62" t="n">
-        <v>601.2180000000001</v>
+        <v>-29405016</v>
       </c>
       <c r="N62" t="inlineStr"/>
       <c r="O62" t="n">
+        <v>601.2180000000001</v>
+      </c>
+      <c r="P62" t="inlineStr"/>
+      <c r="Q62" t="n">
         <v>590.7641834535707</v>
       </c>
-      <c r="P62" t="n">
-        <v>3142349.333333333</v>
-      </c>
-      <c r="Q62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
@@ -2956,29 +3348,35 @@
       <c r="D63" t="n">
         <v>-0.006275299879992424</v>
       </c>
-      <c r="E63" t="inlineStr"/>
+      <c r="E63" t="n">
+        <v>0.0620292649493256</v>
+      </c>
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="n">
         <v>593.8848093301863</v>
       </c>
       <c r="H63" t="inlineStr"/>
-      <c r="I63" t="inlineStr"/>
+      <c r="I63" t="n">
+        <v>3039133.4</v>
+      </c>
       <c r="J63" t="inlineStr"/>
       <c r="K63" t="n">
         <v>-50.23971738581886</v>
       </c>
-      <c r="L63" t="inlineStr"/>
+      <c r="L63" t="n">
+        <v>-4493535</v>
+      </c>
       <c r="M63" t="n">
-        <v>602.8389999999999</v>
+        <v>-22454700</v>
       </c>
       <c r="N63" t="inlineStr"/>
       <c r="O63" t="n">
+        <v>602.8389999999999</v>
+      </c>
+      <c r="P63" t="inlineStr"/>
+      <c r="Q63" t="n">
         <v>594.4327478296789</v>
       </c>
-      <c r="P63" t="n">
-        <v>3039133.4</v>
-      </c>
-      <c r="Q63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
@@ -2995,29 +3393,35 @@
       <c r="D64" t="n">
         <v>-0.008727100962795831</v>
       </c>
-      <c r="E64" t="inlineStr"/>
+      <c r="E64" t="n">
+        <v>0.06402583482395495</v>
+      </c>
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="n">
         <v>596.2425995566191</v>
       </c>
       <c r="H64" t="inlineStr"/>
-      <c r="I64" t="inlineStr"/>
+      <c r="I64" t="n">
+        <v>2983680.733333333</v>
+      </c>
       <c r="J64" t="inlineStr"/>
       <c r="K64" t="n">
         <v>-46.27542126670542</v>
       </c>
-      <c r="L64" t="inlineStr"/>
+      <c r="L64" t="n">
+        <v>-6567568</v>
+      </c>
       <c r="M64" t="n">
-        <v>604.24</v>
+        <v>-15131210</v>
       </c>
       <c r="N64" t="inlineStr"/>
       <c r="O64" t="n">
+        <v>604.24</v>
+      </c>
+      <c r="P64" t="inlineStr"/>
+      <c r="Q64" t="n">
         <v>598.2887994041395</v>
       </c>
-      <c r="P64" t="n">
-        <v>2983680.733333333</v>
-      </c>
-      <c r="Q64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
@@ -3034,29 +3438,35 @@
       <c r="D65" t="n">
         <v>-0.07704098471497378</v>
       </c>
-      <c r="E65" t="inlineStr"/>
+      <c r="E65" t="n">
+        <v>0.06392161986598364</v>
+      </c>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="n">
         <v>599.7301729217089</v>
       </c>
       <c r="H65" t="inlineStr"/>
-      <c r="I65" t="inlineStr"/>
+      <c r="I65" t="n">
+        <v>2828869.8</v>
+      </c>
       <c r="J65" t="inlineStr"/>
       <c r="K65" t="n">
         <v>-47.64867775517536</v>
       </c>
-      <c r="L65" t="inlineStr"/>
+      <c r="L65" t="n">
+        <v>-10328353</v>
+      </c>
       <c r="M65" t="n">
-        <v>604.9963333333333</v>
+        <v>-10486882</v>
       </c>
       <c r="N65" t="inlineStr"/>
       <c r="O65" t="n">
+        <v>604.9963333333333</v>
+      </c>
+      <c r="P65" t="inlineStr"/>
+      <c r="Q65" t="n">
         <v>602.1769924664939</v>
       </c>
-      <c r="P65" t="n">
-        <v>2828869.8</v>
-      </c>
-      <c r="Q65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
@@ -3073,29 +3483,35 @@
       <c r="D66" t="n">
         <v>-0.02379829491907248</v>
       </c>
-      <c r="E66" t="inlineStr"/>
+      <c r="E66" t="n">
+        <v>0.04888611626965295</v>
+      </c>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="n">
         <v>605.9908844489299</v>
       </c>
       <c r="H66" t="inlineStr"/>
-      <c r="I66" t="inlineStr"/>
+      <c r="I66" t="n">
+        <v>2554328</v>
+      </c>
       <c r="J66" t="inlineStr"/>
       <c r="K66" t="n">
         <v>-238.91017454236</v>
       </c>
-      <c r="L66" t="inlineStr"/>
+      <c r="L66" t="n">
+        <v>-3677358</v>
+      </c>
       <c r="M66" t="n">
-        <v>605.6759999999999</v>
+        <v>-2250628</v>
       </c>
       <c r="N66" t="inlineStr"/>
       <c r="O66" t="n">
+        <v>605.6759999999999</v>
+      </c>
+      <c r="P66" t="inlineStr"/>
+      <c r="Q66" t="n">
         <v>606.0057505676314</v>
       </c>
-      <c r="P66" t="n">
-        <v>2554328</v>
-      </c>
-      <c r="Q66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
@@ -3112,29 +3528,35 @@
       <c r="D67" t="n">
         <v>0.004591612227649478</v>
       </c>
-      <c r="E67" t="inlineStr"/>
+      <c r="E67" t="n">
+        <v>0.04773864799702436</v>
+      </c>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="n">
         <v>605.6254633050906</v>
       </c>
       <c r="H67" t="inlineStr"/>
-      <c r="I67" t="inlineStr"/>
+      <c r="I67" t="n">
+        <v>2514349.666666667</v>
+      </c>
       <c r="J67" t="inlineStr"/>
       <c r="K67" t="n">
         <v>-313.1696428571422</v>
       </c>
-      <c r="L67" t="inlineStr"/>
+      <c r="L67" t="n">
+        <v>1615119</v>
+      </c>
       <c r="M67" t="n">
-        <v>605.0543333333334</v>
+        <v>-1051278</v>
       </c>
       <c r="N67" t="inlineStr"/>
       <c r="O67" t="n">
+        <v>605.0543333333334</v>
+      </c>
+      <c r="P67" t="inlineStr"/>
+      <c r="Q67" t="n">
         <v>607.0792506067783</v>
       </c>
-      <c r="P67" t="n">
-        <v>2514349.666666667</v>
-      </c>
-      <c r="Q67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
@@ -3157,23 +3579,27 @@
         <v>604.6989410602854</v>
       </c>
       <c r="H68" t="inlineStr"/>
-      <c r="I68" t="inlineStr"/>
+      <c r="I68" t="n">
+        <v>2555185.433333333</v>
+      </c>
       <c r="J68" t="inlineStr"/>
       <c r="K68" t="n">
         <v>-1513.071895424828</v>
       </c>
-      <c r="L68" t="inlineStr"/>
+      <c r="L68" t="n">
+        <v>-2985238</v>
+      </c>
       <c r="M68" t="n">
-        <v>604.2346666666667</v>
+        <v>-5506589</v>
       </c>
       <c r="N68" t="inlineStr"/>
       <c r="O68" t="n">
+        <v>604.2346666666667</v>
+      </c>
+      <c r="P68" t="inlineStr"/>
+      <c r="Q68" t="n">
         <v>607.2460954762112</v>
       </c>
-      <c r="P68" t="n">
-        <v>2555185.433333333</v>
-      </c>
-      <c r="Q68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
@@ -3199,14 +3625,16 @@
       <c r="K69" t="n">
         <v>537.1759890859469</v>
       </c>
-      <c r="L69" t="inlineStr"/>
+      <c r="L69" t="n">
+        <v>-2317239</v>
+      </c>
       <c r="M69" t="inlineStr"/>
       <c r="N69" t="inlineStr"/>
-      <c r="O69" t="n">
+      <c r="O69" t="inlineStr"/>
+      <c r="P69" t="inlineStr"/>
+      <c r="Q69" t="n">
         <v>607.6154813711222</v>
       </c>
-      <c r="P69" t="inlineStr"/>
-      <c r="Q69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
@@ -3232,14 +3660,16 @@
       <c r="K70" t="n">
         <v>333.4038950042346</v>
       </c>
-      <c r="L70" t="inlineStr"/>
+      <c r="L70" t="n">
+        <v>2091353</v>
+      </c>
       <c r="M70" t="inlineStr"/>
       <c r="N70" t="inlineStr"/>
-      <c r="O70" t="n">
+      <c r="O70" t="inlineStr"/>
+      <c r="P70" t="inlineStr"/>
+      <c r="Q70" t="n">
         <v>607.3241352587858</v>
       </c>
-      <c r="P70" t="inlineStr"/>
-      <c r="Q70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
@@ -3265,14 +3695,16 @@
       <c r="K71" t="n">
         <v>1563.805104408332</v>
       </c>
-      <c r="L71" t="inlineStr"/>
+      <c r="L71" t="n">
+        <v>1815682</v>
+      </c>
       <c r="M71" t="inlineStr"/>
       <c r="N71" t="inlineStr"/>
-      <c r="O71" t="n">
+      <c r="O71" t="inlineStr"/>
+      <c r="P71" t="inlineStr"/>
+      <c r="Q71" t="n">
         <v>605.9526963111157</v>
       </c>
-      <c r="P71" t="inlineStr"/>
-      <c r="Q71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
@@ -3298,14 +3730,16 @@
       <c r="K72" t="n">
         <v>384.8306997742673</v>
       </c>
-      <c r="L72" t="inlineStr"/>
+      <c r="L72" t="n">
+        <v>2313824</v>
+      </c>
       <c r="M72" t="inlineStr"/>
       <c r="N72" t="inlineStr"/>
-      <c r="O72" t="n">
+      <c r="O72" t="inlineStr"/>
+      <c r="P72" t="inlineStr"/>
+      <c r="Q72" t="n">
         <v>605.2694339877443</v>
       </c>
-      <c r="P72" t="inlineStr"/>
-      <c r="Q72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
@@ -3331,14 +3765,16 @@
       <c r="K73" t="n">
         <v>693.206521739133</v>
       </c>
-      <c r="L73" t="inlineStr"/>
+      <c r="L73" t="n">
+        <v>-3436244</v>
+      </c>
       <c r="M73" t="inlineStr"/>
       <c r="N73" t="inlineStr"/>
-      <c r="O73" t="n">
+      <c r="O73" t="inlineStr"/>
+      <c r="P73" t="inlineStr"/>
+      <c r="Q73" t="n">
         <v>604.5397397800024</v>
       </c>
-      <c r="P73" t="inlineStr"/>
-      <c r="Q73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
@@ -3364,14 +3800,16 @@
       <c r="K74" t="n">
         <v>233.1809872029249</v>
       </c>
-      <c r="L74" t="inlineStr"/>
+      <c r="L74" t="n">
+        <v>-2131245</v>
+      </c>
       <c r="M74" t="inlineStr"/>
       <c r="N74" t="inlineStr"/>
-      <c r="O74" t="n">
+      <c r="O74" t="inlineStr"/>
+      <c r="P74" t="inlineStr"/>
+      <c r="Q74" t="n">
         <v>604.3604114889681</v>
       </c>
-      <c r="P74" t="inlineStr"/>
-      <c r="Q74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
@@ -3397,14 +3835,16 @@
       <c r="K75" t="n">
         <v>203.2182103610675</v>
       </c>
-      <c r="L75" t="inlineStr"/>
+      <c r="L75" t="n">
+        <v>2542763</v>
+      </c>
       <c r="M75" t="inlineStr"/>
       <c r="N75" t="inlineStr"/>
-      <c r="O75" t="n">
+      <c r="O75" t="inlineStr"/>
+      <c r="P75" t="inlineStr"/>
+      <c r="Q75" t="n">
         <v>602.557681246828</v>
       </c>
-      <c r="P75" t="inlineStr"/>
-      <c r="Q75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
@@ -3430,14 +3870,16 @@
       <c r="K76" t="n">
         <v>232.8073635765948</v>
       </c>
-      <c r="L76" t="inlineStr"/>
+      <c r="L76" t="n">
+        <v>1687613</v>
+      </c>
       <c r="M76" t="inlineStr"/>
       <c r="N76" t="inlineStr"/>
-      <c r="O76" t="n">
+      <c r="O76" t="inlineStr"/>
+      <c r="P76" t="inlineStr"/>
+      <c r="Q76" t="n">
         <v>600.3368316776437</v>
       </c>
-      <c r="P76" t="inlineStr"/>
-      <c r="Q76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
@@ -3463,14 +3905,16 @@
       <c r="K77" t="n">
         <v>251.0280373831779</v>
       </c>
-      <c r="L77" t="inlineStr"/>
+      <c r="L77" t="n">
+        <v>-2666775</v>
+      </c>
       <c r="M77" t="inlineStr"/>
       <c r="N77" t="inlineStr"/>
-      <c r="O77" t="n">
+      <c r="O77" t="inlineStr"/>
+      <c r="P77" t="inlineStr"/>
+      <c r="Q77" t="n">
         <v>598.4352338623087</v>
       </c>
-      <c r="P77" t="inlineStr"/>
-      <c r="Q77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
@@ -3496,14 +3940,16 @@
       <c r="K78" t="n">
         <v>172.3659003831419</v>
       </c>
-      <c r="L78" t="inlineStr"/>
+      <c r="L78" t="n">
+        <v>-2007432</v>
+      </c>
       <c r="M78" t="inlineStr"/>
       <c r="N78" t="inlineStr"/>
-      <c r="O78" t="n">
+      <c r="O78" t="inlineStr"/>
+      <c r="P78" t="inlineStr"/>
+      <c r="Q78" t="n">
         <v>597.1011120597092</v>
       </c>
-      <c r="P78" t="inlineStr"/>
-      <c r="Q78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
@@ -3529,14 +3975,16 @@
       <c r="K79" t="n">
         <v>156.2600644122383</v>
       </c>
-      <c r="L79" t="inlineStr"/>
+      <c r="L79" t="n">
+        <v>3212187</v>
+      </c>
       <c r="M79" t="inlineStr"/>
       <c r="N79" t="inlineStr"/>
-      <c r="O79" t="n">
+      <c r="O79" t="inlineStr"/>
+      <c r="P79" t="inlineStr"/>
+      <c r="Q79" t="n">
         <v>594.9729128914132</v>
       </c>
-      <c r="P79" t="inlineStr"/>
-      <c r="Q79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
@@ -3562,14 +4010,16 @@
       <c r="K80" t="n">
         <v>156.6592337320091</v>
       </c>
-      <c r="L80" t="inlineStr"/>
+      <c r="L80" t="n">
+        <v>-2137831</v>
+      </c>
       <c r="M80" t="inlineStr"/>
       <c r="N80" t="inlineStr"/>
-      <c r="O80" t="n">
+      <c r="O80" t="inlineStr"/>
+      <c r="P80" t="inlineStr"/>
+      <c r="Q80" t="n">
         <v>592.5413896425451</v>
       </c>
-      <c r="P80" t="inlineStr"/>
-      <c r="Q80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
@@ -3595,14 +4045,16 @@
       <c r="K81" t="n">
         <v>139.1680172879522</v>
       </c>
-      <c r="L81" t="inlineStr"/>
+      <c r="L81" t="n">
+        <v>3806205</v>
+      </c>
       <c r="M81" t="inlineStr"/>
       <c r="N81" t="inlineStr"/>
-      <c r="O81" t="n">
+      <c r="O81" t="inlineStr"/>
+      <c r="P81" t="inlineStr"/>
+      <c r="Q81" t="n">
         <v>591.0663130661688</v>
       </c>
-      <c r="P81" t="inlineStr"/>
-      <c r="Q81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
@@ -3628,14 +4080,16 @@
       <c r="K82" t="n">
         <v>176.3620639953873</v>
       </c>
-      <c r="L82" t="inlineStr"/>
+      <c r="L82" t="n">
+        <v>2999032</v>
+      </c>
       <c r="M82" t="inlineStr"/>
       <c r="N82" t="inlineStr"/>
-      <c r="O82" t="n">
+      <c r="O82" t="inlineStr"/>
+      <c r="P82" t="inlineStr"/>
+      <c r="Q82" t="n">
         <v>588.8929553465942</v>
       </c>
-      <c r="P82" t="inlineStr"/>
-      <c r="Q82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
@@ -3661,14 +4115,16 @@
       <c r="K83" t="n">
         <v>303.2144944476925</v>
       </c>
-      <c r="L83" t="inlineStr"/>
+      <c r="L83" t="n">
+        <v>-2723463</v>
+      </c>
       <c r="M83" t="inlineStr"/>
       <c r="N83" t="inlineStr"/>
-      <c r="O83" t="n">
+      <c r="O83" t="inlineStr"/>
+      <c r="P83" t="inlineStr"/>
+      <c r="Q83" t="n">
         <v>587.6800557153249</v>
       </c>
-      <c r="P83" t="inlineStr"/>
-      <c r="Q83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
@@ -3694,14 +4150,16 @@
       <c r="K84" t="n">
         <v>220.5782312925167</v>
       </c>
-      <c r="L84" t="inlineStr"/>
+      <c r="L84" t="n">
+        <v>-4488000</v>
+      </c>
       <c r="M84" t="inlineStr"/>
       <c r="N84" t="inlineStr"/>
-      <c r="O84" t="n">
+      <c r="O84" t="inlineStr"/>
+      <c r="P84" t="inlineStr"/>
+      <c r="Q84" t="n">
         <v>587.0248871439679</v>
       </c>
-      <c r="P84" t="inlineStr"/>
-      <c r="Q84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
@@ -3725,14 +4183,16 @@
       <c r="I85" t="inlineStr"/>
       <c r="J85" t="inlineStr"/>
       <c r="K85" t="inlineStr"/>
-      <c r="L85" t="inlineStr"/>
+      <c r="L85" t="n">
+        <v>3755338</v>
+      </c>
       <c r="M85" t="inlineStr"/>
       <c r="N85" t="inlineStr"/>
-      <c r="O85" t="n">
+      <c r="O85" t="inlineStr"/>
+      <c r="P85" t="inlineStr"/>
+      <c r="Q85" t="n">
         <v>585.8824655676898</v>
       </c>
-      <c r="P85" t="inlineStr"/>
-      <c r="Q85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
@@ -3756,14 +4216,16 @@
       <c r="I86" t="inlineStr"/>
       <c r="J86" t="inlineStr"/>
       <c r="K86" t="inlineStr"/>
-      <c r="L86" t="inlineStr"/>
+      <c r="L86" t="n">
+        <v>-2793610</v>
+      </c>
       <c r="M86" t="inlineStr"/>
       <c r="N86" t="inlineStr"/>
-      <c r="O86" t="n">
+      <c r="O86" t="inlineStr"/>
+      <c r="P86" t="inlineStr"/>
+      <c r="Q86" t="n">
         <v>584.1122907792545</v>
       </c>
-      <c r="P86" t="inlineStr"/>
-      <c r="Q86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
@@ -3787,14 +4249,16 @@
       <c r="I87" t="inlineStr"/>
       <c r="J87" t="inlineStr"/>
       <c r="K87" t="inlineStr"/>
-      <c r="L87" t="inlineStr"/>
+      <c r="L87" t="n">
+        <v>-2588293</v>
+      </c>
       <c r="M87" t="inlineStr"/>
       <c r="N87" t="inlineStr"/>
-      <c r="O87" t="n">
+      <c r="O87" t="inlineStr"/>
+      <c r="P87" t="inlineStr"/>
+      <c r="Q87" t="n">
         <v>583.4510694536859</v>
       </c>
-      <c r="P87" t="inlineStr"/>
-      <c r="Q87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
@@ -3818,14 +4282,16 @@
       <c r="I88" t="inlineStr"/>
       <c r="J88" t="inlineStr"/>
       <c r="K88" t="inlineStr"/>
-      <c r="L88" t="inlineStr"/>
+      <c r="L88" t="n">
+        <v>2126096</v>
+      </c>
       <c r="M88" t="inlineStr"/>
       <c r="N88" t="inlineStr"/>
-      <c r="O88" t="n">
+      <c r="O88" t="inlineStr"/>
+      <c r="P88" t="inlineStr"/>
+      <c r="Q88" t="n">
         <v>582.578729416009</v>
       </c>
-      <c r="P88" t="inlineStr"/>
-      <c r="Q88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
@@ -3849,14 +4315,16 @@
       <c r="I89" t="inlineStr"/>
       <c r="J89" t="inlineStr"/>
       <c r="K89" t="inlineStr"/>
-      <c r="L89" t="inlineStr"/>
+      <c r="L89" t="n">
+        <v>-1472167</v>
+      </c>
       <c r="M89" t="inlineStr"/>
       <c r="N89" t="inlineStr"/>
-      <c r="O89" t="n">
+      <c r="O89" t="inlineStr"/>
+      <c r="P89" t="inlineStr"/>
+      <c r="Q89" t="n">
         <v>581.537262479182</v>
       </c>
-      <c r="P89" t="inlineStr"/>
-      <c r="Q89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
@@ -3880,14 +4348,16 @@
       <c r="I90" t="inlineStr"/>
       <c r="J90" t="inlineStr"/>
       <c r="K90" t="inlineStr"/>
-      <c r="L90" t="inlineStr"/>
+      <c r="L90" t="n">
+        <v>2331830</v>
+      </c>
       <c r="M90" t="inlineStr"/>
       <c r="N90" t="inlineStr"/>
-      <c r="O90" t="n">
+      <c r="O90" t="inlineStr"/>
+      <c r="P90" t="inlineStr"/>
+      <c r="Q90" t="n">
         <v>580.5025909260221</v>
       </c>
-      <c r="P90" t="inlineStr"/>
-      <c r="Q90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
@@ -3911,14 +4381,16 @@
       <c r="I91" t="inlineStr"/>
       <c r="J91" t="inlineStr"/>
       <c r="K91" t="inlineStr"/>
-      <c r="L91" t="inlineStr"/>
+      <c r="L91" t="n">
+        <v>2135690</v>
+      </c>
       <c r="M91" t="inlineStr"/>
       <c r="N91" t="inlineStr"/>
-      <c r="O91" t="n">
+      <c r="O91" t="inlineStr"/>
+      <c r="P91" t="inlineStr"/>
+      <c r="Q91" t="n">
         <v>579.3310454726443</v>
       </c>
-      <c r="P91" t="inlineStr"/>
-      <c r="Q91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
@@ -3942,14 +4414,16 @@
       <c r="I92" t="inlineStr"/>
       <c r="J92" t="inlineStr"/>
       <c r="K92" t="inlineStr"/>
-      <c r="L92" t="inlineStr"/>
+      <c r="L92" t="n">
+        <v>1926919</v>
+      </c>
       <c r="M92" t="inlineStr"/>
       <c r="N92" t="inlineStr"/>
-      <c r="O92" t="n">
+      <c r="O92" t="inlineStr"/>
+      <c r="P92" t="inlineStr"/>
+      <c r="Q92" t="n">
         <v>578.5242210224818</v>
       </c>
-      <c r="P92" t="inlineStr"/>
-      <c r="Q92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
@@ -3973,14 +4447,16 @@
       <c r="I93" t="inlineStr"/>
       <c r="J93" t="inlineStr"/>
       <c r="K93" t="inlineStr"/>
-      <c r="L93" t="inlineStr"/>
+      <c r="L93" t="n">
+        <v>2829955</v>
+      </c>
       <c r="M93" t="inlineStr"/>
       <c r="N93" t="inlineStr"/>
-      <c r="O93" t="n">
+      <c r="O93" t="inlineStr"/>
+      <c r="P93" t="inlineStr"/>
+      <c r="Q93" t="n">
         <v>577.9948569550667</v>
       </c>
-      <c r="P93" t="inlineStr"/>
-      <c r="Q93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
@@ -4004,14 +4480,16 @@
       <c r="I94" t="inlineStr"/>
       <c r="J94" t="inlineStr"/>
       <c r="K94" t="inlineStr"/>
-      <c r="L94" t="inlineStr"/>
+      <c r="L94" t="n">
+        <v>-1923240</v>
+      </c>
       <c r="M94" t="inlineStr"/>
       <c r="N94" t="inlineStr"/>
-      <c r="O94" t="n">
+      <c r="O94" t="inlineStr"/>
+      <c r="P94" t="inlineStr"/>
+      <c r="Q94" t="n">
         <v>577.8186401933471</v>
       </c>
-      <c r="P94" t="inlineStr"/>
-      <c r="Q94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
@@ -4035,14 +4513,16 @@
       <c r="I95" t="inlineStr"/>
       <c r="J95" t="inlineStr"/>
       <c r="K95" t="inlineStr"/>
-      <c r="L95" t="inlineStr"/>
+      <c r="L95" t="n">
+        <v>-2092099</v>
+      </c>
       <c r="M95" t="inlineStr"/>
       <c r="N95" t="inlineStr"/>
-      <c r="O95" t="n">
+      <c r="O95" t="inlineStr"/>
+      <c r="P95" t="inlineStr"/>
+      <c r="Q95" t="n">
         <v>578.730270551509</v>
       </c>
-      <c r="P95" t="inlineStr"/>
-      <c r="Q95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
@@ -4066,14 +4546,16 @@
       <c r="I96" t="inlineStr"/>
       <c r="J96" t="inlineStr"/>
       <c r="K96" t="inlineStr"/>
-      <c r="L96" t="inlineStr"/>
+      <c r="L96" t="n">
+        <v>-2478008</v>
+      </c>
       <c r="M96" t="inlineStr"/>
       <c r="N96" t="inlineStr"/>
-      <c r="O96" t="n">
+      <c r="O96" t="inlineStr"/>
+      <c r="P96" t="inlineStr"/>
+      <c r="Q96" t="n">
         <v>579.535806451613</v>
       </c>
-      <c r="P96" t="inlineStr"/>
-      <c r="Q96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
@@ -4095,14 +4577,16 @@
       <c r="I97" t="inlineStr"/>
       <c r="J97" t="inlineStr"/>
       <c r="K97" t="inlineStr"/>
-      <c r="L97" t="inlineStr"/>
+      <c r="L97" t="n">
+        <v>-2840192</v>
+      </c>
       <c r="M97" t="inlineStr"/>
       <c r="N97" t="inlineStr"/>
-      <c r="O97" t="n">
+      <c r="O97" t="inlineStr"/>
+      <c r="P97" t="inlineStr"/>
+      <c r="Q97" t="n">
         <v>580.0700000000001</v>
       </c>
-      <c r="P97" t="inlineStr"/>
-      <c r="Q97" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Draft for plotting is done. Need to beautify
</commit_message>
<xml_diff>
--- a/xlsx/analysis.xlsx
+++ b/xlsx/analysis.xlsx
@@ -527,52 +527,52 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>221.21</v>
+        <v>483.43</v>
       </c>
       <c r="C2" t="n">
-        <v>1541746</v>
+        <v>2152416</v>
       </c>
       <c r="D2" t="n">
-        <v>0.003532292414684335</v>
+        <v>0.00113835116969252</v>
       </c>
       <c r="E2" t="n">
-        <v>0.05313588580366626</v>
+        <v>0.03536765552462411</v>
       </c>
       <c r="F2" t="n">
-        <v>0.02725377323185425</v>
+        <v>0.03890127454137432</v>
       </c>
       <c r="G2" t="n">
-        <v>219.2201409953269</v>
+        <v>478.4021741722594</v>
       </c>
       <c r="H2" t="n">
-        <v>240.3118517010334</v>
+        <v>532.6817844559362</v>
       </c>
       <c r="I2" t="n">
-        <v>1833859.833333333</v>
+        <v>2781855.933333333</v>
       </c>
       <c r="J2" t="n">
-        <v>1479662.666666667</v>
+        <v>3445060.877777778</v>
       </c>
       <c r="K2" t="n">
-        <v>379.4582392776519</v>
+        <v>400.8687258687258</v>
       </c>
       <c r="L2" t="n">
-        <v>1541746</v>
+        <v>2152416</v>
       </c>
       <c r="M2" t="n">
-        <v>-12136297</v>
+        <v>-17729448</v>
       </c>
       <c r="N2" t="n">
-        <v>-12370858</v>
+        <v>-80024909</v>
       </c>
       <c r="O2" t="n">
-        <v>221.2226666666667</v>
+        <v>478.8986666666667</v>
       </c>
       <c r="P2" t="n">
-        <v>243.6136666666667</v>
+        <v>537.2432222222222</v>
       </c>
       <c r="Q2" t="n">
-        <v>223.5464979118738</v>
+        <v>486.6395954223248</v>
       </c>
     </row>
     <row r="3">
@@ -582,52 +582,52 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>220.43</v>
+        <v>482.88</v>
       </c>
       <c r="C3" t="n">
-        <v>1405406</v>
+        <v>2562865</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0008623233338944658</v>
+        <v>-0.005102104578750932</v>
       </c>
       <c r="E3" t="n">
-        <v>0.05303053931009264</v>
+        <v>0.03542220982864532</v>
       </c>
       <c r="F3" t="n">
-        <v>0.02724812820739908</v>
+        <v>0.03895312133992412</v>
       </c>
       <c r="G3" t="n">
-        <v>219.7834917927527</v>
+        <v>478.6639327048821</v>
       </c>
       <c r="H3" t="n">
-        <v>240.5052550054609</v>
+        <v>533.3567856095348</v>
       </c>
       <c r="I3" t="n">
-        <v>1826802.1</v>
+        <v>2875863.9</v>
       </c>
       <c r="J3" t="n">
-        <v>1472293.088888889</v>
+        <v>3442555.355555556</v>
       </c>
       <c r="K3" t="n">
-        <v>641.2000000000005</v>
+        <v>770.3007518797011</v>
       </c>
       <c r="L3" t="n">
-        <v>1405406</v>
+        <v>-2562865</v>
       </c>
       <c r="M3" t="n">
-        <v>-15008057</v>
+        <v>-24854519</v>
       </c>
       <c r="N3" t="n">
-        <v>-13034120</v>
+        <v>-80250406</v>
       </c>
       <c r="O3" t="n">
-        <v>222.007</v>
+        <v>478.955</v>
       </c>
       <c r="P3" t="n">
-        <v>243.7775555555556</v>
+        <v>538.3851111111112</v>
       </c>
       <c r="Q3" t="n">
-        <v>223.7076356988995</v>
+        <v>486.860946830761</v>
       </c>
     </row>
     <row r="4">
@@ -637,52 +637,52 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>220.24</v>
+        <v>485.35</v>
       </c>
       <c r="C4" t="n">
-        <v>1251171</v>
+        <v>3491638</v>
       </c>
       <c r="D4" t="n">
-        <v>0.02022680006347333</v>
+        <v>0.01955747346092096</v>
       </c>
       <c r="E4" t="n">
-        <v>0.05299674694339472</v>
+        <v>0.03687471262381947</v>
       </c>
       <c r="F4" t="n">
-        <v>0.02763749942431502</v>
+        <v>0.03930404669550656</v>
       </c>
       <c r="G4" t="n">
-        <v>220.423093339891</v>
+        <v>478.86985859123</v>
       </c>
       <c r="H4" t="n">
-        <v>240.662905281283</v>
+        <v>534.204648694748</v>
       </c>
       <c r="I4" t="n">
-        <v>1827880.5</v>
+        <v>2903879.3</v>
       </c>
       <c r="J4" t="n">
-        <v>1472761.011111111</v>
+        <v>3445523.022222222</v>
       </c>
       <c r="K4" t="n">
-        <v>452.3437499999996</v>
+        <v>378.6733837111665</v>
       </c>
       <c r="L4" t="n">
-        <v>1251171</v>
+        <v>3491638</v>
       </c>
       <c r="M4" t="n">
-        <v>-17851221</v>
+        <v>-25694981</v>
       </c>
       <c r="N4" t="n">
-        <v>-12992007</v>
+        <v>-74857586</v>
       </c>
       <c r="O4" t="n">
-        <v>222.8196666666667</v>
+        <v>479.0959999999999</v>
       </c>
       <c r="P4" t="n">
-        <v>243.9444444444445</v>
+        <v>539.4703333333333</v>
       </c>
       <c r="Q4" t="n">
-        <v>223.9336795402029</v>
+        <v>487.1354948880549</v>
       </c>
     </row>
     <row r="5">
@@ -692,52 +692,52 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>215.83</v>
+        <v>475.95</v>
       </c>
       <c r="C5" t="n">
-        <v>1883340</v>
+        <v>4287846</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.003792087415039447</v>
+        <v>-0.01493156429691744</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0514114572062234</v>
+        <v>0.03518612570774039</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02739633430973161</v>
+        <v>0.03912338232045677</v>
       </c>
       <c r="G5" t="n">
-        <v>221.0541096286866</v>
+        <v>479.1553580864267</v>
       </c>
       <c r="H5" t="n">
-        <v>240.7600741751373</v>
+        <v>534.9470117961548</v>
       </c>
       <c r="I5" t="n">
-        <v>1830377.366666667</v>
+        <v>2874305.633333333</v>
       </c>
       <c r="J5" t="n">
-        <v>1471506.844444444</v>
+        <v>3428096.377777778</v>
       </c>
       <c r="K5" t="n">
-        <v>1730.120481927689</v>
+        <v>-3051.28205128202</v>
       </c>
       <c r="L5" t="n">
-        <v>-1883340</v>
+        <v>-4287846</v>
       </c>
       <c r="M5" t="n">
-        <v>-20428469</v>
+        <v>-31791047</v>
       </c>
       <c r="N5" t="n">
-        <v>-13104882</v>
+        <v>-80272464</v>
       </c>
       <c r="O5" t="n">
-        <v>223.691</v>
+        <v>479.4846666666666</v>
       </c>
       <c r="P5" t="n">
-        <v>244.0475555555555</v>
+        <v>540.3508888888888</v>
       </c>
       <c r="Q5" t="n">
-        <v>224.1884160602169</v>
+        <v>487.2586324665414</v>
       </c>
     </row>
     <row r="6">
@@ -747,52 +747,52 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>216.65</v>
+        <v>483.11</v>
       </c>
       <c r="C6" t="n">
-        <v>1465619</v>
+        <v>2458192</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.005156311778940825</v>
+        <v>0.001698778117256161</v>
       </c>
       <c r="E6" t="n">
-        <v>0.05510161641905505</v>
+        <v>0.03450671475965837</v>
       </c>
       <c r="F6" t="n">
-        <v>0.02742882251666705</v>
+        <v>0.03907171119089434</v>
       </c>
       <c r="G6" t="n">
-        <v>222.0891003171579</v>
+        <v>480.0442540217421</v>
       </c>
       <c r="H6" t="n">
-        <v>240.9763125661949</v>
+        <v>535.9920601809156</v>
       </c>
       <c r="I6" t="n">
-        <v>1824002.033333333</v>
+        <v>2834153.2</v>
       </c>
       <c r="J6" t="n">
-        <v>1467834.5</v>
+        <v>3403699.188888889</v>
       </c>
       <c r="K6" t="n">
-        <v>-1121.875</v>
+        <v>390.9892262487743</v>
       </c>
       <c r="L6" t="n">
-        <v>-1465619</v>
+        <v>2458192</v>
       </c>
       <c r="M6" t="n">
-        <v>-20237209</v>
+        <v>-30586474</v>
       </c>
       <c r="N6" t="n">
-        <v>-9668713</v>
+        <v>-78076717</v>
       </c>
       <c r="O6" t="n">
-        <v>224.787</v>
+        <v>480.26</v>
       </c>
       <c r="P6" t="n">
-        <v>244.193</v>
+        <v>541.3631111111112</v>
       </c>
       <c r="Q6" t="n">
-        <v>224.7648585471284</v>
+        <v>488.0385381538891</v>
       </c>
     </row>
     <row r="7">
@@ -802,52 +802,52 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>217.77</v>
+        <v>482.29</v>
       </c>
       <c r="C7" t="n">
-        <v>1032861</v>
+        <v>2741116</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.003941343323937474</v>
+        <v>-0.0007461604176484116</v>
       </c>
       <c r="E7" t="n">
-        <v>0.05511270263635368</v>
+        <v>0.03452063001290907</v>
       </c>
       <c r="F7" t="n">
-        <v>0.02790813981184054</v>
+        <v>0.03912833073819739</v>
       </c>
       <c r="G7" t="n">
-        <v>222.7836528343808</v>
+        <v>480.4908320871507</v>
       </c>
       <c r="H7" t="n">
-        <v>241.1129212120166</v>
+        <v>536.7059491325657</v>
       </c>
       <c r="I7" t="n">
-        <v>1801534</v>
+        <v>2820747.8</v>
       </c>
       <c r="J7" t="n">
-        <v>1465760.322222222</v>
+        <v>3403919.366666667</v>
       </c>
       <c r="K7" t="n">
-        <v>2368.749999999943</v>
+        <v>292.9220779220773</v>
       </c>
       <c r="L7" t="n">
-        <v>-1032861</v>
+        <v>-2741116</v>
       </c>
       <c r="M7" t="n">
-        <v>-19563168</v>
+        <v>-35100696</v>
       </c>
       <c r="N7" t="n">
-        <v>-9482037</v>
+        <v>-83012917</v>
       </c>
       <c r="O7" t="n">
-        <v>226.2133333333333</v>
+        <v>480.8926666666667</v>
       </c>
       <c r="P7" t="n">
-        <v>244.3101111111111</v>
+        <v>542.3484444444445</v>
       </c>
       <c r="Q7" t="n">
-        <v>225.3245039641717</v>
+        <v>488.3784373369159</v>
       </c>
     </row>
     <row r="8">
@@ -857,50 +857,50 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>218.63</v>
+        <v>482.65</v>
       </c>
       <c r="C8" t="n">
-        <v>1487020</v>
+        <v>2301635</v>
       </c>
       <c r="D8" t="n">
-        <v>0.02163846042597051</v>
+        <v>-0.01122854959847785</v>
       </c>
       <c r="E8" t="n">
-        <v>0.05514066769479745</v>
+        <v>0.03453321999914554</v>
       </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
-        <v>223.5053107198614</v>
+        <v>481.5286440971489</v>
       </c>
       <c r="H8" t="n">
-        <v>241.2188368009967</v>
+        <v>537.5945803701691</v>
       </c>
       <c r="I8" t="n">
-        <v>1796975.033333333</v>
+        <v>2859277.366666667</v>
       </c>
       <c r="J8" t="n">
-        <v>1470322.977777778</v>
+        <v>3405020.211111111</v>
       </c>
       <c r="K8" t="n">
-        <v>741.314553990613</v>
+        <v>266.4775950085084</v>
       </c>
       <c r="L8" t="n">
-        <v>1487020</v>
+        <v>-2301635</v>
       </c>
       <c r="M8" t="n">
-        <v>-19426399</v>
+        <v>-28462577</v>
       </c>
       <c r="N8" t="n">
-        <v>-9892676</v>
+        <v>-83111993</v>
       </c>
       <c r="O8" t="n">
-        <v>227.635</v>
+        <v>481.6363333333333</v>
       </c>
       <c r="P8" t="n">
-        <v>244.4917777777778</v>
+        <v>543.4348888888888</v>
       </c>
       <c r="Q8" t="n">
-        <v>225.8455042375629</v>
+        <v>488.7983295670479</v>
       </c>
     </row>
     <row r="9">
@@ -910,42 +910,42 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>213.95</v>
+        <v>488.1</v>
       </c>
       <c r="C9" t="n">
-        <v>1189663</v>
+        <v>2165021</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.003126679636155316</v>
+        <v>-0.008507043562066663</v>
       </c>
       <c r="E9" t="n">
-        <v>0.05308590316759727</v>
+        <v>0.03422791723121955</v>
       </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
-        <v>224.3370588129573</v>
+        <v>482.6018842086505</v>
       </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
-        <v>1780485.766666667</v>
+        <v>2923503.366666667</v>
       </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="n">
-        <v>511.4457831325317</v>
+        <v>314.8793565683644</v>
       </c>
       <c r="L9" t="n">
-        <v>-1189663</v>
+        <v>-2165021</v>
       </c>
       <c r="M9" t="n">
-        <v>-21905761</v>
+        <v>-30389357</v>
       </c>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="n">
-        <v>229.0463333333333</v>
+        <v>482.3613333333333</v>
       </c>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="n">
-        <v>226.3431252194638</v>
+        <v>489.2223522958098</v>
       </c>
     </row>
     <row r="10">
@@ -955,42 +955,42 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>214.62</v>
+        <v>492.27</v>
       </c>
       <c r="C10" t="n">
-        <v>1860058</v>
+        <v>2518346</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.009644886043331802</v>
+        <v>-0.002677866611500157</v>
       </c>
       <c r="E10" t="n">
-        <v>0.05318691037793046</v>
+        <v>0.03401330847517651</v>
       </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
-        <v>225.2294700404046</v>
+        <v>483.2631420889487</v>
       </c>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
-        <v>1772159</v>
+        <v>2945113.633333333</v>
       </c>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="n">
-        <v>-5660.000000000316</v>
+        <v>263.6363636363638</v>
       </c>
       <c r="L10" t="n">
-        <v>-1860058</v>
+        <v>-2518346</v>
       </c>
       <c r="M10" t="n">
-        <v>-19776238</v>
+        <v>-25411007</v>
       </c>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
-        <v>230.637</v>
+        <v>483.0113333333333</v>
       </c>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="n">
-        <v>227.1978235104612</v>
+        <v>489.2997559024173</v>
       </c>
     </row>
     <row r="11">
@@ -1000,42 +1000,42 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>216.7</v>
+        <v>493.59</v>
       </c>
       <c r="C11" t="n">
-        <v>1343774</v>
+        <v>2104030</v>
       </c>
       <c r="D11" t="n">
-        <v>0.00699254973586072</v>
+        <v>0.01512628736597943</v>
       </c>
       <c r="E11" t="n">
-        <v>0.05316717968855935</v>
+        <v>0.03507220677132652</v>
       </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
-        <v>226.3531114313442</v>
+        <v>484.1489801771236</v>
       </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="n">
-        <v>1746043.133333333</v>
+        <v>3003736.633333333</v>
       </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="n">
-        <v>-147.1403812824955</v>
+        <v>270.4663212435242</v>
       </c>
       <c r="L11" t="n">
-        <v>1343774</v>
+        <v>2104030</v>
       </c>
       <c r="M11" t="n">
-        <v>-18992762</v>
+        <v>-18615625</v>
       </c>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="n">
-        <v>232.202</v>
+        <v>483.51</v>
       </c>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="n">
-        <v>228.065259614631</v>
+        <v>489.0949114818943</v>
       </c>
     </row>
     <row r="12">
@@ -1045,42 +1045,42 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>215.19</v>
+        <v>486.18</v>
       </c>
       <c r="C12" t="n">
-        <v>1197081</v>
+        <v>2833186</v>
       </c>
       <c r="D12" t="n">
-        <v>0.02465195167625023</v>
+        <v>0.01996430888377621</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0526997684200063</v>
+        <v>0.03601119675601534</v>
       </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
-        <v>227.2306967713073</v>
+        <v>484.8270782588708</v>
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="n">
-        <v>1731018.466666667</v>
+        <v>3114057.2</v>
       </c>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="n">
-        <v>-107.2072072072073</v>
+        <v>284.1417910447767</v>
       </c>
       <c r="L12" t="n">
-        <v>1197081</v>
+        <v>2833186</v>
       </c>
       <c r="M12" t="n">
-        <v>-21229570</v>
+        <v>-26133302</v>
       </c>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="n">
-        <v>233.7406666666666</v>
+        <v>483.7076666666667</v>
       </c>
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="n">
-        <v>228.8490706225365</v>
+        <v>488.7849053771974</v>
       </c>
     </row>
     <row r="13">
@@ -1090,42 +1090,42 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>209.95</v>
+        <v>476.57</v>
       </c>
       <c r="C13" t="n">
-        <v>1589246</v>
+        <v>2516422</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.003613373398513531</v>
+        <v>0.015180637418994</v>
       </c>
       <c r="E13" t="n">
-        <v>0.05095466069379427</v>
+        <v>0.03468464322173136</v>
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
-        <v>228.7498346078378</v>
+        <v>486.2231826836464</v>
       </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
-        <v>1747563.666666667</v>
+        <v>3193170.333333333</v>
       </c>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="n">
-        <v>-37.84683684794678</v>
+        <v>1454.838709677412</v>
       </c>
       <c r="L13" t="n">
-        <v>-1589246</v>
+        <v>2516422</v>
       </c>
       <c r="M13" t="n">
-        <v>-20733214</v>
+        <v>-34173068</v>
       </c>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
-        <v>235.426</v>
+        <v>484.5433333333334</v>
       </c>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="n">
-        <v>229.7910754930563</v>
+        <v>488.9645540239006</v>
       </c>
     </row>
     <row r="14">
@@ -1135,42 +1135,42 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>210.71</v>
+        <v>469.39</v>
       </c>
       <c r="C14" t="n">
-        <v>1687750</v>
+        <v>2490171</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.01010491174544548</v>
+        <v>0.01407416336167433</v>
       </c>
       <c r="E14" t="n">
-        <v>0.05359287087720721</v>
+        <v>0.03325130334787255</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
-        <v>230.1379240477245</v>
+        <v>487.9033216622183</v>
       </c>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="n">
-        <v>1736590.5</v>
+        <v>3250608.166666667</v>
       </c>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="n">
-        <v>-33.70675453047784</v>
+        <v>-194.0899932840836</v>
       </c>
       <c r="L14" t="n">
-        <v>-1687750</v>
+        <v>2490171</v>
       </c>
       <c r="M14" t="n">
-        <v>-17883917</v>
+        <v>-40929047</v>
       </c>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
-        <v>237.1753333333333</v>
+        <v>485.9623333333333</v>
       </c>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="n">
-        <v>231.1594255270602</v>
+        <v>489.8193508531351</v>
       </c>
     </row>
     <row r="15">
@@ -1180,42 +1180,42 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>212.85</v>
+        <v>462.83</v>
       </c>
       <c r="C15" t="n">
-        <v>1427716</v>
+        <v>3222618</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.01829532211344276</v>
+        <v>-0.02188355304935996</v>
       </c>
       <c r="E15" t="n">
-        <v>0.05383562880879578</v>
+        <v>0.03326504908992482</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
-        <v>231.2133279147745</v>
+        <v>490.6633957101307</v>
       </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="n">
-        <v>1708920.966666667</v>
+        <v>3403662.333333333</v>
       </c>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="n">
-        <v>-46.94189602446497</v>
+        <v>-91.59491594915943</v>
       </c>
       <c r="L15" t="n">
-        <v>-1427716</v>
+        <v>-3222618</v>
       </c>
       <c r="M15" t="n">
-        <v>-15338503</v>
+        <v>-36337422</v>
       </c>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="n">
-        <v>238.6913333333333</v>
+        <v>487.689</v>
       </c>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="n">
-        <v>232.5697307358229</v>
+        <v>491.2282716016272</v>
       </c>
     </row>
     <row r="16">
@@ -1225,42 +1225,42 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>216.78</v>
+        <v>473.07</v>
       </c>
       <c r="C16" t="n">
-        <v>1437021</v>
+        <v>2954736</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.005290895920115446</v>
+        <v>-0.009446437391583018</v>
       </c>
       <c r="E16" t="n">
-        <v>0.05364332137716318</v>
+        <v>0.03977446001681783</v>
       </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="n">
-        <v>232.1580451510276</v>
+        <v>493.0543219827908</v>
       </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="n">
-        <v>1691543.633333333</v>
+        <v>3531330.966666667</v>
       </c>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="n">
-        <v>-39.42215088282512</v>
+        <v>-114.681724845996</v>
       </c>
       <c r="L16" t="n">
-        <v>-1437021</v>
+        <v>-2954736</v>
       </c>
       <c r="M16" t="n">
-        <v>-13004391</v>
+        <v>-26062127</v>
       </c>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="n">
-        <v>240.1023333333333</v>
+        <v>489.39</v>
       </c>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="n">
-        <v>233.9297121658797</v>
+        <v>493.1867730913946</v>
       </c>
     </row>
     <row r="17">
@@ -1270,42 +1270,42 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>217.93</v>
+        <v>477.56</v>
       </c>
       <c r="C17" t="n">
-        <v>1277888</v>
+        <v>2460261</v>
       </c>
       <c r="D17" t="n">
-        <v>0.007045363335392629</v>
+        <v>0.008664617825288268</v>
       </c>
       <c r="E17" t="n">
-        <v>0.05398255727112791</v>
+        <v>0.0867579276186084</v>
       </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="n">
-        <v>233.8511939920211</v>
+        <v>493.4411426438375</v>
       </c>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="n">
-        <v>1744007.466666667</v>
+        <v>4085534.366666667</v>
       </c>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="n">
-        <v>-51.21602288984283</v>
+        <v>-455.5059523809553</v>
       </c>
       <c r="L17" t="n">
-        <v>1277888</v>
+        <v>2460261</v>
       </c>
       <c r="M17" t="n">
-        <v>-14578306</v>
+        <v>-42688229</v>
       </c>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="n">
-        <v>241.351</v>
+        <v>490.0363333333333</v>
       </c>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="n">
-        <v>235.1124509359403</v>
+        <v>494.5741367528701</v>
       </c>
     </row>
     <row r="18">
@@ -1315,42 +1315,42 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>216.4</v>
+        <v>473.44</v>
       </c>
       <c r="C18" t="n">
-        <v>2211585</v>
+        <v>2250913</v>
       </c>
       <c r="D18" t="n">
-        <v>0.00649051884466445</v>
+        <v>-0.007742842924473692</v>
       </c>
       <c r="E18" t="n">
-        <v>0.0536085849018046</v>
+        <v>0.08639123516373795</v>
       </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="n">
-        <v>234.8201147376491</v>
+        <v>497.3617351034494</v>
       </c>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="n">
-        <v>1742337.133333333</v>
+        <v>4200462.9</v>
       </c>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="n">
-        <v>-49.18842625264654</v>
+        <v>-226.7979452054798</v>
       </c>
       <c r="L18" t="n">
-        <v>2211585</v>
+        <v>-2250913</v>
       </c>
       <c r="M18" t="n">
-        <v>-17083972</v>
+        <v>-51056607</v>
       </c>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="n">
-        <v>242.7043333333333</v>
+        <v>493.1326666666666</v>
       </c>
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="n">
-        <v>236.297447552212</v>
+        <v>495.7475254944473</v>
       </c>
     </row>
     <row r="19">
@@ -1360,42 +1360,42 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>215</v>
+        <v>477.12</v>
       </c>
       <c r="C19" t="n">
-        <v>2628238</v>
+        <v>2338044</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.01353588218005708</v>
+        <v>0.008884081926542997</v>
       </c>
       <c r="E19" t="n">
-        <v>0.05339985840957057</v>
+        <v>0.08640628292196673</v>
       </c>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="n">
-        <v>236.1450128001251</v>
+        <v>499.8605046983944</v>
       </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="n">
-        <v>1706428.633333333</v>
+        <v>4240966.533333333</v>
       </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="n">
-        <v>-42.0664206642067</v>
+        <v>-265.1651651651654</v>
       </c>
       <c r="L19" t="n">
-        <v>-2628238</v>
+        <v>2338044</v>
       </c>
       <c r="M19" t="n">
-        <v>-20429887</v>
+        <v>-52271716</v>
       </c>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="n">
-        <v>244.1143333333333</v>
+        <v>496.4696666666667</v>
       </c>
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="n">
-        <v>237.6696853144335</v>
+        <v>497.2859755285471</v>
       </c>
     </row>
     <row r="20">
@@ -1405,42 +1405,42 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>217.93</v>
+        <v>472.9</v>
       </c>
       <c r="C20" t="n">
-        <v>1504576</v>
+        <v>2205836</v>
       </c>
       <c r="D20" t="n">
-        <v>0.003677657802039214</v>
+        <v>0.01279026576480202</v>
       </c>
       <c r="E20" t="n">
-        <v>0.05473709581839138</v>
+        <v>0.08854412693456494</v>
       </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="n">
-        <v>238.0223750751262</v>
+        <v>502.4173864749558</v>
       </c>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="n">
-        <v>1666751.066666667</v>
+        <v>4278670.433333334</v>
       </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="n">
-        <v>-44.07732864674878</v>
+        <v>-92.3683119037745</v>
       </c>
       <c r="L20" t="n">
-        <v>1504576</v>
+        <v>2205836</v>
       </c>
       <c r="M20" t="n">
-        <v>-16363738</v>
+        <v>-51140599</v>
       </c>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="n">
-        <v>245.707</v>
+        <v>499.8703333333333</v>
       </c>
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="n">
-        <v>239.2331118878427</v>
+        <v>498.6767324615503</v>
       </c>
     </row>
     <row r="21">
@@ -1450,42 +1450,42 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>217.13</v>
+        <v>466.89</v>
       </c>
       <c r="C21" t="n">
-        <v>1776476</v>
+        <v>2604256</v>
       </c>
       <c r="D21" t="n">
-        <v>0.002905705063136033</v>
+        <v>0.004013268469919673</v>
       </c>
       <c r="E21" t="n">
-        <v>0.05692461251473894</v>
+        <v>0.08873294906050881</v>
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
-        <v>239.2224956653163</v>
+        <v>504.2069079065534</v>
       </c>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="n">
-        <v>1665577.1</v>
+        <v>4300402.266666667</v>
       </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="n">
-        <v>-37.17542748575048</v>
+        <v>-50.30940594059422</v>
       </c>
       <c r="L21" t="n">
-        <v>1776476</v>
+        <v>2604256</v>
       </c>
       <c r="M21" t="n">
-        <v>-16398957</v>
+        <v>-50488644</v>
       </c>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
-        <v>247.0513333333333</v>
+        <v>502.7876666666667</v>
       </c>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="n">
-        <v>240.7022920180388</v>
+        <v>500.4544381485538</v>
       </c>
     </row>
     <row r="22">
@@ -1495,42 +1495,42 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>216.5</v>
+        <v>465.02</v>
       </c>
       <c r="C22" t="n">
-        <v>3157485</v>
+        <v>3282142</v>
       </c>
       <c r="D22" t="n">
-        <v>0.02748750774527675</v>
+        <v>-0.01739545036903412</v>
       </c>
       <c r="E22" t="n">
-        <v>0.05677898013946013</v>
+        <v>0.08858404670506242</v>
       </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="n">
-        <v>240.2493326618242</v>
+        <v>505.999767312758</v>
       </c>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="n">
-        <v>1635751.866666667</v>
+        <v>4308033.066666666</v>
       </c>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="n">
-        <v>-25.87331159757805</v>
+        <v>-38.81845157809562</v>
       </c>
       <c r="L22" t="n">
-        <v>3157485</v>
+        <v>-3282142</v>
       </c>
       <c r="M22" t="n">
-        <v>-19057152</v>
+        <v>-55926080</v>
       </c>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="n">
-        <v>248.209</v>
+        <v>505.6143333333333</v>
       </c>
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="n">
-        <v>242.3279673296277</v>
+        <v>502.769226986385</v>
       </c>
     </row>
     <row r="23">
@@ -1540,42 +1540,42 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>210.63</v>
+        <v>473.18</v>
       </c>
       <c r="C23" t="n">
-        <v>4609060</v>
+        <v>2389742</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.02016282616335285</v>
+        <v>-0.002680372635625261</v>
       </c>
       <c r="E23" t="n">
-        <v>0.05463821604566289</v>
+        <v>0.08969686303251832</v>
       </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
-        <v>242.2316837713826</v>
+        <v>508.0806016874097</v>
       </c>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="n">
-        <v>1576537.266666667</v>
+        <v>4287313.133333334</v>
       </c>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="n">
-        <v>-10.52420164691706</v>
+        <v>-45.79885423297276</v>
       </c>
       <c r="L23" t="n">
-        <v>-4609060</v>
+        <v>-2389742</v>
       </c>
       <c r="M23" t="n">
-        <v>-20833590</v>
+        <v>-49983394</v>
       </c>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="n">
-        <v>249.4536666666667</v>
+        <v>508.6483333333333</v>
       </c>
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="n">
-        <v>244.1092064558088</v>
+        <v>505.3726219509633</v>
       </c>
     </row>
     <row r="24">
@@ -1585,42 +1585,42 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>214.92</v>
+        <v>474.45</v>
       </c>
       <c r="C24" t="n">
-        <v>6357444</v>
+        <v>2034793</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.06013184104462432</v>
+        <v>-0.003723693911071635</v>
       </c>
       <c r="E24" t="n">
-        <v>0.05516767552836341</v>
+        <v>0.08969399695704329</v>
       </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="n">
-        <v>245.7696945431512</v>
+        <v>509.5930884791989</v>
       </c>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="n">
-        <v>1456503.6</v>
+        <v>4314647.266666667</v>
       </c>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="n">
-        <v>-11.37893593919654</v>
+        <v>-48.714524207012</v>
       </c>
       <c r="L24" t="n">
-        <v>-6357444</v>
+        <v>-2034793</v>
       </c>
       <c r="M24" t="n">
-        <v>-15216480</v>
+        <v>-50803418</v>
       </c>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
-        <v>250.8026666666667</v>
+        <v>510.9786666666666</v>
       </c>
       <c r="P24" t="inlineStr"/>
       <c r="Q24" t="n">
-        <v>246.4181172458646</v>
+        <v>507.5928027751676</v>
       </c>
     </row>
     <row r="25">
@@ -1630,42 +1630,42 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>228.24</v>
+        <v>476.22</v>
       </c>
       <c r="C25" t="n">
-        <v>2120161</v>
+        <v>2660097</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.006028061760421366</v>
+        <v>0.01293449430075455</v>
       </c>
       <c r="E25" t="n">
-        <v>0.05313401070612371</v>
+        <v>0.09179135018978782</v>
       </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="n">
-        <v>250.8462060053303</v>
+        <v>511.2834529935612</v>
       </c>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="n">
-        <v>1306266.2</v>
+        <v>4389715.3</v>
       </c>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="n">
-        <v>-15.67454382291358</v>
+        <v>-46.49458253664784</v>
       </c>
       <c r="L25" t="n">
-        <v>-2120161</v>
+        <v>2660097</v>
       </c>
       <c r="M25" t="n">
-        <v>-10709358</v>
+        <v>-53055459</v>
       </c>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="n">
-        <v>251.8816666666667</v>
+        <v>513.325</v>
       </c>
       <c r="P25" t="inlineStr"/>
       <c r="Q25" t="n">
-        <v>248.5904011938553</v>
+        <v>509.878513311386</v>
       </c>
     </row>
     <row r="26">
@@ -1675,42 +1675,42 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>229.62</v>
+        <v>470.1</v>
       </c>
       <c r="C26" t="n">
-        <v>1385762</v>
+        <v>3353225</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.03154998072292781</v>
+        <v>-0.008451739059037067</v>
       </c>
       <c r="E26" t="n">
-        <v>0.05344476791516741</v>
+        <v>0.09121476155296916</v>
       </c>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="n">
-        <v>252.5660161806162</v>
+        <v>513.09296796182</v>
       </c>
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="n">
-        <v>1300428.433333333</v>
+        <v>4386259.366666666</v>
       </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="n">
-        <v>-16.71361502347429</v>
+        <v>-23.80824131430136</v>
       </c>
       <c r="L26" t="n">
-        <v>-1385762</v>
+        <v>-3353225</v>
       </c>
       <c r="M26" t="n">
-        <v>-10534225</v>
+        <v>-58271975</v>
       </c>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="n">
-        <v>252.9636666666667</v>
+        <v>516.3823333333333</v>
       </c>
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="n">
-        <v>249.9938771382591</v>
+        <v>512.1997900914815</v>
       </c>
     </row>
     <row r="27">
@@ -1720,42 +1720,42 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>236.98</v>
+        <v>474.09</v>
       </c>
       <c r="C27" t="n">
-        <v>1617057</v>
+        <v>5621945</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.01707011577160333</v>
+        <v>-0.0212660747504172</v>
       </c>
       <c r="E27" t="n">
-        <v>0.0536255164497516</v>
+        <v>0.09218096384845327</v>
       </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="n">
-        <v>254.4637183969609</v>
+        <v>515.5001683078759</v>
       </c>
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="n">
-        <v>1382711.166666667</v>
+        <v>4373421.8</v>
       </c>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="n">
-        <v>-20.6336939721794</v>
+        <v>-65.08061344868312</v>
       </c>
       <c r="L27" t="n">
-        <v>-1617057</v>
+        <v>-5621945</v>
       </c>
       <c r="M27" t="n">
-        <v>-5294219</v>
+        <v>-51950652</v>
       </c>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="n">
-        <v>254.1343333333333</v>
+        <v>519.7433333333333</v>
       </c>
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="n">
-        <v>251.3989721133114</v>
+        <v>515.103223890894</v>
       </c>
     </row>
     <row r="28">
@@ -1765,42 +1765,42 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>241.06</v>
+        <v>484.28</v>
       </c>
       <c r="C28" t="n">
-        <v>1171342</v>
+        <v>2978539</v>
       </c>
       <c r="D28" t="n">
-        <v>0.008540473099812651</v>
+        <v>-0.006052514616702531</v>
       </c>
       <c r="E28" t="n">
-        <v>0.05355372040334539</v>
+        <v>0.09240243080309687</v>
       </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="n">
-        <v>255.4040901371328</v>
+        <v>518.6290500265889</v>
       </c>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="n">
-        <v>1439864.6</v>
+        <v>4314169.166666667</v>
       </c>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="n">
-        <v>-21.6281895504254</v>
+        <v>-61.36447905079757</v>
       </c>
       <c r="L28" t="n">
-        <v>1171342</v>
+        <v>-2978539</v>
       </c>
       <c r="M28" t="n">
-        <v>-345502</v>
+        <v>-42484341</v>
       </c>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="n">
-        <v>254.8406666666667</v>
+        <v>522.6163333333333</v>
       </c>
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="n">
-        <v>252.3933839831949</v>
+        <v>517.931722090266</v>
       </c>
     </row>
     <row r="29">
@@ -1810,42 +1810,42 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>239.01</v>
+        <v>487.22</v>
       </c>
       <c r="C29" t="n">
-        <v>1285050</v>
+        <v>2487870</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.03664105619777658</v>
+        <v>-0.0108802118454463</v>
       </c>
       <c r="E29" t="n">
-        <v>0.05329772715678836</v>
+        <v>0.09241211326084665</v>
       </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="n">
-        <v>255.7823277696683</v>
+        <v>520.0199197779642</v>
       </c>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="n">
-        <v>1457586.366666667</v>
+        <v>4291991.966666667</v>
       </c>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="n">
-        <v>-28.22374039282667</v>
+        <v>-51.84837092731877</v>
       </c>
       <c r="L29" t="n">
-        <v>-1285050</v>
+        <v>-2487870</v>
       </c>
       <c r="M29" t="n">
-        <v>-3219839</v>
+        <v>-41819025</v>
       </c>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="n">
-        <v>255.3136666666666</v>
+        <v>524.8676666666667</v>
       </c>
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="n">
-        <v>253.1749966716911</v>
+        <v>520.2525305102844</v>
       </c>
     </row>
     <row r="30">
@@ -1855,42 +1855,42 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>247.93</v>
+        <v>492.55</v>
       </c>
       <c r="C30" t="n">
-        <v>840676</v>
+        <v>2548566</v>
       </c>
       <c r="D30" t="n">
-        <v>0.008262166800716564</v>
+        <v>0.01693272646214883</v>
       </c>
       <c r="E30" t="n">
-        <v>0.049896066565735</v>
+        <v>0.09250331980762065</v>
       </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="n">
-        <v>256.3046115033046</v>
+        <v>521.4641109314838</v>
       </c>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="n">
-        <v>1446451.6</v>
+        <v>4317315.366666666</v>
       </c>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="n">
-        <v>-155.5690072639229</v>
+        <v>-57.78631284916239</v>
       </c>
       <c r="L30" t="n">
-        <v>840676</v>
+        <v>2548566</v>
       </c>
       <c r="M30" t="n">
-        <v>-2885796</v>
+        <v>-42578727</v>
       </c>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="n">
-        <v>255.9116666666667</v>
+        <v>527.0433333333334</v>
       </c>
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="n">
-        <v>254.1518929938767</v>
+        <v>522.5306360627178</v>
       </c>
     </row>
     <row r="31">
@@ -1900,42 +1900,42 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>245.89</v>
+        <v>484.28</v>
       </c>
       <c r="C31" t="n">
-        <v>1273523</v>
+        <v>3439211</v>
       </c>
       <c r="D31" t="n">
-        <v>0.004687858899922404</v>
+        <v>-0.001733031174413036</v>
       </c>
       <c r="E31" t="n">
-        <v>0.04963712340657329</v>
+        <v>0.09224536645111683</v>
       </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="n">
-        <v>256.4900241284614</v>
+        <v>523.2896580674462</v>
       </c>
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="n">
-        <v>1451356.533333333</v>
+        <v>4374068.266666667</v>
       </c>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="n">
-        <v>-127.2335844994614</v>
+        <v>-52.77214334009503</v>
       </c>
       <c r="L31" t="n">
-        <v>1273523</v>
+        <v>-3439211</v>
       </c>
       <c r="M31" t="n">
-        <v>-2738648</v>
+        <v>-40876140</v>
       </c>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="n">
-        <v>256.2256666666667</v>
+        <v>529.3076666666667</v>
       </c>
       <c r="P31" t="inlineStr"/>
       <c r="Q31" t="n">
-        <v>254.5809890624199</v>
+        <v>524.5982661360086</v>
       </c>
     </row>
     <row r="32">
@@ -1945,42 +1945,42 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>244.74</v>
+        <v>485.12</v>
       </c>
       <c r="C32" t="n">
-        <v>1330014</v>
+        <v>4972655</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.0002859769195264761</v>
+        <v>-0.004093687253180711</v>
       </c>
       <c r="E32" t="n">
-        <v>0.04954009614686979</v>
+        <v>0.09393516349109694</v>
       </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="n">
-        <v>256.8168528580974</v>
+        <v>525.3393964797115</v>
       </c>
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="n">
-        <v>1436288.8</v>
+        <v>4410977.366666666</v>
       </c>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="n">
-        <v>-122.2105263157896</v>
+        <v>-504.223433242511</v>
       </c>
       <c r="L32" t="n">
-        <v>-1330014</v>
+        <v>-4972655</v>
       </c>
       <c r="M32" t="n">
-        <v>-3190680</v>
+        <v>-32890445</v>
       </c>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="n">
-        <v>256.6026666666667</v>
+        <v>531.6130000000001</v>
       </c>
       <c r="P32" t="inlineStr"/>
       <c r="Q32" t="n">
-        <v>255.1803676184488</v>
+        <v>527.3788362143541</v>
       </c>
     </row>
     <row r="33">
@@ -1990,42 +1990,42 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>244.81</v>
+        <v>487.11</v>
       </c>
       <c r="C33" t="n">
-        <v>1437758</v>
+        <v>3403327</v>
       </c>
       <c r="D33" t="n">
-        <v>-0.006392660056778965</v>
+        <v>-0.02012017635142271</v>
       </c>
       <c r="E33" t="n">
-        <v>0.05056377167092719</v>
+        <v>0.09393841981142968</v>
       </c>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="n">
-        <v>257.1959273785197</v>
+        <v>527.3142887263923</v>
       </c>
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="n">
-        <v>1427884.233333333</v>
+        <v>4412668.766666667</v>
       </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="n">
-        <v>-84.6209912536446</v>
+        <v>-44.40844732421425</v>
       </c>
       <c r="L33" t="n">
-        <v>-1437758</v>
+        <v>-3403327</v>
       </c>
       <c r="M33" t="n">
-        <v>-782789</v>
+        <v>-32941187</v>
       </c>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="n">
-        <v>257.0106666666667</v>
+        <v>533.3613333333334</v>
       </c>
       <c r="P33" t="inlineStr"/>
       <c r="Q33" t="n">
-        <v>255.9003929714453</v>
+        <v>530.2932387118958</v>
       </c>
     </row>
     <row r="34">
@@ -2035,42 +2035,42 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>246.38</v>
+        <v>497.01</v>
       </c>
       <c r="C34" t="n">
-        <v>1326077</v>
+        <v>2604428</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.009412499554421139</v>
+        <v>-0.004416702287305618</v>
       </c>
       <c r="E34" t="n">
-        <v>0.05075207569584388</v>
+        <v>0.09350694208025999</v>
       </c>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="n">
-        <v>257.536141699755</v>
+        <v>528.7167103723795</v>
       </c>
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="n">
-        <v>1404702.5</v>
+        <v>4449009.033333333</v>
       </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="n">
-        <v>-94.23701298701314</v>
+        <v>-48.35380193362971</v>
       </c>
       <c r="L34" t="n">
-        <v>-1326077</v>
+        <v>-2604428</v>
       </c>
       <c r="M34" t="n">
-        <v>-87337</v>
+        <v>-34031395</v>
       </c>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="n">
-        <v>257.2676666666667</v>
+        <v>535.075</v>
       </c>
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="n">
-        <v>256.6652476591311</v>
+        <v>533.2713931058197</v>
       </c>
     </row>
     <row r="35">
@@ -2080,42 +2080,42 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>248.71</v>
+        <v>499.21</v>
       </c>
       <c r="C35" t="n">
-        <v>1692080</v>
+        <v>3083273</v>
       </c>
       <c r="D35" t="n">
-        <v>-0.04223790291081375</v>
+        <v>-0.005752537585141049</v>
       </c>
       <c r="E35" t="n">
-        <v>0.05088216044876848</v>
+        <v>0.09355522566601722</v>
       </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="n">
-        <v>257.818521848397</v>
+        <v>529.9480388377322</v>
       </c>
       <c r="H35" t="inlineStr"/>
       <c r="I35" t="n">
-        <v>1403083.866666667</v>
+        <v>4581113.7</v>
       </c>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="n">
-        <v>-82.51599147121567</v>
+        <v>-46.30301513824617</v>
       </c>
       <c r="L35" t="n">
-        <v>-1692080</v>
+        <v>-3083273</v>
       </c>
       <c r="M35" t="n">
-        <v>-38778</v>
+        <v>-37994535</v>
       </c>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="n">
-        <v>257.5636666666667</v>
+        <v>536.5716666666667</v>
       </c>
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="n">
-        <v>257.3745750838988</v>
+        <v>535.7721788372555</v>
       </c>
     </row>
     <row r="36">
@@ -2125,42 +2125,42 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>259.44</v>
+        <v>502.09</v>
       </c>
       <c r="C36" t="n">
-        <v>791578</v>
+        <v>2056030</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.003770250301520228</v>
+        <v>-0.004986649715955416</v>
       </c>
       <c r="E36" t="n">
-        <v>0.04607543704472732</v>
+        <v>0.1014303964785909</v>
       </c>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="n">
-        <v>258.2032896758886</v>
+        <v>531.7961421568878</v>
       </c>
       <c r="H36" t="inlineStr"/>
       <c r="I36" t="n">
-        <v>1392329.666666667</v>
+        <v>4822616.366666666</v>
       </c>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="n">
-        <v>1366.94915254236</v>
+        <v>-95.54260243442516</v>
       </c>
       <c r="L36" t="n">
-        <v>-791578</v>
+        <v>-2056030</v>
       </c>
       <c r="M36" t="n">
-        <v>283848</v>
+        <v>-45239615</v>
       </c>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="n">
-        <v>257.8833333333333</v>
+        <v>538.1533333333333</v>
       </c>
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="n">
-        <v>257.9721319862366</v>
+        <v>538.2937084122386</v>
       </c>
     </row>
     <row r="37">
@@ -2170,42 +2170,42 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>260.42</v>
+        <v>504.6</v>
       </c>
       <c r="C37" t="n">
-        <v>896092</v>
+        <v>3897003</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.0021097458869761</v>
+        <v>0.0003964321161937789</v>
       </c>
       <c r="E37" t="n">
-        <v>0.04606996379236913</v>
+        <v>0.1018954089749918</v>
       </c>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="n">
-        <v>258.232746326244</v>
+        <v>533.687676822758</v>
       </c>
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="n">
-        <v>1390094.133333333</v>
+        <v>4876660.633333334</v>
       </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="n">
-        <v>263.2009345794389</v>
+        <v>-136.8868124867276</v>
       </c>
       <c r="L37" t="n">
-        <v>-896092</v>
+        <v>3897003</v>
       </c>
       <c r="M37" t="n">
-        <v>350914</v>
+        <v>-46860943</v>
       </c>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="n">
-        <v>257.9436666666667</v>
+        <v>541.0983333333332</v>
       </c>
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="n">
-        <v>257.8708997094253</v>
+        <v>540.7905158889447</v>
       </c>
     </row>
     <row r="38">
@@ -2215,42 +2215,42 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>260.97</v>
+        <v>504.4</v>
       </c>
       <c r="C38" t="n">
-        <v>992342</v>
+        <v>4228415</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.002678709699104331</v>
+        <v>-0.006324131749468442</v>
       </c>
       <c r="E38" t="n">
-        <v>0.04738108780727073</v>
+        <v>0.1019961788166949</v>
       </c>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="n">
-        <v>258.2731014054758</v>
+        <v>535.2706984893236</v>
       </c>
       <c r="H38" t="inlineStr"/>
       <c r="I38" t="n">
-        <v>1391075.766666667</v>
+        <v>4800597.833333333</v>
       </c>
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="n">
-        <v>315.9887798036451</v>
+        <v>-124.4384198295896</v>
       </c>
       <c r="L38" t="n">
-        <v>-992342</v>
+        <v>-4228415</v>
       </c>
       <c r="M38" t="n">
-        <v>2172547</v>
+        <v>-49142827</v>
       </c>
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="n">
-        <v>258.002</v>
+        <v>544.4336666666667</v>
       </c>
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="n">
-        <v>257.6950996893857</v>
+        <v>543.2864135364581</v>
       </c>
     </row>
     <row r="39">
@@ -2260,42 +2260,42 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>261.67</v>
+        <v>507.6</v>
       </c>
       <c r="C39" t="n">
-        <v>939860</v>
+        <v>2813329</v>
       </c>
       <c r="D39" t="n">
-        <v>0.0003822337788301766</v>
+        <v>0.0007291862014220385</v>
       </c>
       <c r="E39" t="n">
-        <v>0.04863578574157289</v>
+        <v>0.102147721850943</v>
       </c>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="n">
-        <v>258.1612661167261</v>
+        <v>537.5778891970526</v>
       </c>
       <c r="H39" t="inlineStr"/>
       <c r="I39" t="n">
-        <v>1402717.166666667</v>
+        <v>4759158.6</v>
       </c>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="n">
-        <v>239.0728476821186</v>
+        <v>-217.5542406311637</v>
       </c>
       <c r="L39" t="n">
-        <v>939860</v>
+        <v>2813329</v>
       </c>
       <c r="M39" t="n">
-        <v>1823305</v>
+        <v>-47899650</v>
       </c>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="n">
-        <v>257.8616666666666</v>
+        <v>547.6833333333333</v>
       </c>
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="n">
-        <v>257.4692444955502</v>
+        <v>545.9682351596621</v>
       </c>
     </row>
     <row r="40">
@@ -2305,42 +2305,42 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>261.57</v>
+        <v>507.23</v>
       </c>
       <c r="C40" t="n">
-        <v>1076582</v>
+        <v>4277036</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.004919636946029371</v>
+        <v>0.01531691231174293</v>
       </c>
       <c r="E40" t="n">
-        <v>0.04950797984613337</v>
+        <v>0.1025372709846265</v>
       </c>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="n">
-        <v>258.1801391711418</v>
+        <v>539.3801321335113</v>
       </c>
       <c r="H40" t="inlineStr"/>
       <c r="I40" t="n">
-        <v>1406572.733333333</v>
+        <v>4742622.266666667</v>
       </c>
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="n">
-        <v>202.9411764705879</v>
+        <v>-204.3073650624832</v>
       </c>
       <c r="L40" t="n">
-        <v>-1076582</v>
+        <v>4277036</v>
       </c>
       <c r="M40" t="n">
-        <v>-172082</v>
+        <v>-53030218</v>
       </c>
       <c r="N40" t="inlineStr"/>
       <c r="O40" t="n">
-        <v>257.874</v>
+        <v>551.158</v>
       </c>
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="n">
-        <v>257.1795372193812</v>
+        <v>548.614320343087</v>
       </c>
     </row>
     <row r="41">
@@ -2350,42 +2350,42 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>262.86</v>
+        <v>499.52</v>
       </c>
       <c r="C41" t="n">
-        <v>893034</v>
+        <v>5413647</v>
       </c>
       <c r="D41" t="n">
-        <v>-0.01093444616819461</v>
+        <v>-0.02321107002994438</v>
       </c>
       <c r="E41" t="n">
-        <v>0.05058062620408701</v>
+        <v>0.1027352127155134</v>
       </c>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="n">
-        <v>258.4570613940065</v>
+        <v>541.672827447213</v>
       </c>
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="n">
-        <v>1431640.833333333</v>
+        <v>4669766.166666667</v>
       </c>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="n">
-        <v>1341.666666666651</v>
+        <v>-101.0377082724348</v>
       </c>
       <c r="L41" t="n">
-        <v>-893034</v>
+        <v>-5413647</v>
       </c>
       <c r="M41" t="n">
-        <v>2733125</v>
+        <v>-55215901</v>
       </c>
       <c r="N41" t="inlineStr"/>
       <c r="O41" t="n">
-        <v>258.0443333333333</v>
+        <v>555.1573333333333</v>
       </c>
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="n">
-        <v>256.8767466827869</v>
+        <v>551.4684114012309</v>
       </c>
     </row>
     <row r="42">
@@ -2395,42 +2395,42 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>265.75</v>
+        <v>511.25</v>
       </c>
       <c r="C42" t="n">
-        <v>1693437</v>
+        <v>5206580</v>
       </c>
       <c r="D42" t="n">
-        <v>0.01257163741892331</v>
+        <v>-0.01531488895132149</v>
       </c>
       <c r="E42" t="n">
-        <v>0.05056826582773676</v>
+        <v>0.1024068905138023</v>
       </c>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="n">
-        <v>258.4202211116746</v>
+        <v>544.3315386711545</v>
       </c>
       <c r="H42" t="inlineStr"/>
       <c r="I42" t="n">
-        <v>1427577.266666667</v>
+        <v>4549834</v>
       </c>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="n">
-        <v>2869.306930693096</v>
+        <v>-115.8344504021448</v>
       </c>
       <c r="L42" t="n">
-        <v>1693437</v>
+        <v>-5206580</v>
       </c>
       <c r="M42" t="n">
-        <v>4397286</v>
+        <v>-47986572</v>
       </c>
       <c r="N42" t="inlineStr"/>
       <c r="O42" t="n">
-        <v>257.9993333333334</v>
+        <v>559.0353333333334</v>
       </c>
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="n">
-        <v>256.464108522979</v>
+        <v>555.0510604633847</v>
       </c>
     </row>
     <row r="43">
@@ -2440,42 +2440,42 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>262.43</v>
+        <v>519.14</v>
       </c>
       <c r="C43" t="n">
-        <v>1260051</v>
+        <v>4239557</v>
       </c>
       <c r="D43" t="n">
-        <v>0.02406502310851355</v>
+        <v>-0.003941062265584883</v>
       </c>
       <c r="E43" t="n">
-        <v>0.05095044592402371</v>
+        <v>0.1028387894383462</v>
       </c>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="n">
-        <v>258.1267572418979</v>
+        <v>546.8593611778165</v>
       </c>
       <c r="H43" t="inlineStr"/>
       <c r="I43" t="n">
-        <v>1408636.266666667</v>
+        <v>4453408.8</v>
       </c>
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="n">
-        <v>756.5727699530526</v>
+        <v>-193.9231891103547</v>
       </c>
       <c r="L43" t="n">
-        <v>1260051</v>
+        <v>-4239557</v>
       </c>
       <c r="M43" t="n">
-        <v>3829056</v>
+        <v>-40466168</v>
       </c>
       <c r="N43" t="inlineStr"/>
       <c r="O43" t="n">
-        <v>257.7553333333333</v>
+        <v>562.522</v>
       </c>
       <c r="P43" t="inlineStr"/>
       <c r="Q43" t="n">
-        <v>255.823702214219</v>
+        <v>558.0718232539629</v>
       </c>
     </row>
     <row r="44">
@@ -2485,42 +2485,42 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>256.19</v>
+        <v>521.1900000000001</v>
       </c>
       <c r="C44" t="n">
-        <v>857664</v>
+        <v>7081796</v>
       </c>
       <c r="D44" t="n">
-        <v>0.003950178201022503</v>
+        <v>0.01416380376001936</v>
       </c>
       <c r="E44" t="n">
-        <v>0.04942687469482131</v>
+        <v>0.1042635955866898</v>
       </c>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="n">
-        <v>257.9115382833801</v>
+        <v>549.3040852719537</v>
       </c>
       <c r="H44" t="inlineStr"/>
       <c r="I44" t="n">
-        <v>1395473.7</v>
+        <v>4426631.7</v>
       </c>
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="n">
-        <v>3075.531914893626</v>
+        <v>-288.083578191315</v>
       </c>
       <c r="L44" t="n">
-        <v>857664</v>
+        <v>7081796</v>
       </c>
       <c r="M44" t="n">
-        <v>3434179</v>
+        <v>-39662855</v>
       </c>
       <c r="N44" t="inlineStr"/>
       <c r="O44" t="n">
-        <v>257.4736666666666</v>
+        <v>565.4553333333333</v>
       </c>
       <c r="P44" t="inlineStr"/>
       <c r="Q44" t="n">
-        <v>255.368095470372</v>
+        <v>560.7567765818224</v>
       </c>
     </row>
     <row r="45">
@@ -2530,42 +2530,42 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>255.18</v>
+        <v>513.86</v>
       </c>
       <c r="C45" t="n">
-        <v>906396</v>
+        <v>7052677</v>
       </c>
       <c r="D45" t="n">
-        <v>0.003690475705191432</v>
+        <v>0.04253761577424964</v>
       </c>
       <c r="E45" t="n">
-        <v>0.04999155488766274</v>
+        <v>0.103657478779518</v>
       </c>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="n">
-        <v>257.7854301199511</v>
+        <v>552.2149281445055</v>
       </c>
       <c r="H45" t="inlineStr"/>
       <c r="I45" t="n">
-        <v>1411422.166666667</v>
+        <v>4261613.333333333</v>
       </c>
       <c r="J45" t="inlineStr"/>
       <c r="K45" t="n">
-        <v>-1576.271186440692</v>
+        <v>-209.4486150660103</v>
       </c>
       <c r="L45" t="n">
-        <v>906396</v>
+        <v>7052677</v>
       </c>
       <c r="M45" t="n">
-        <v>1240397</v>
+        <v>-48875896</v>
       </c>
       <c r="N45" t="inlineStr"/>
       <c r="O45" t="n">
-        <v>257.361</v>
+        <v>569.099</v>
       </c>
       <c r="P45" t="inlineStr"/>
       <c r="Q45" t="n">
-        <v>255.3114123993631</v>
+        <v>563.4855197943618</v>
       </c>
     </row>
     <row r="46">
@@ -2575,42 +2575,42 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>254.24</v>
+        <v>492.46</v>
       </c>
       <c r="C46" t="n">
-        <v>3010936</v>
+        <v>19580838</v>
       </c>
       <c r="D46" t="n">
-        <v>-0.01673303858492226</v>
+        <v>-0.147012284002729</v>
       </c>
       <c r="E46" t="n">
-        <v>0.05003777429349054</v>
+        <v>0.1005776835781166</v>
       </c>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="n">
-        <v>257.7908766162499</v>
+        <v>556.109880074659</v>
       </c>
       <c r="H46" t="inlineStr"/>
       <c r="I46" t="n">
-        <v>1434305.3</v>
+        <v>4111282.866666667</v>
       </c>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="n">
-        <v>-866.8810289389028</v>
+        <v>-87.48897383122568</v>
       </c>
       <c r="L46" t="n">
-        <v>-3010936</v>
+        <v>-19580838</v>
       </c>
       <c r="M46" t="n">
-        <v>1926891</v>
+        <v>-53385810</v>
       </c>
       <c r="N46" t="inlineStr"/>
       <c r="O46" t="n">
-        <v>257.4033333333334</v>
+        <v>573.129</v>
       </c>
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="n">
-        <v>255.3204753234571</v>
+        <v>566.9079694353522</v>
       </c>
     </row>
     <row r="47">
@@ -2620,42 +2620,42 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>258.53</v>
+        <v>570.45</v>
       </c>
       <c r="C47" t="n">
-        <v>1227778</v>
+        <v>5908117</v>
       </c>
       <c r="D47" t="n">
-        <v>-0.0006573478186551185</v>
+        <v>-0.005419593684898416</v>
       </c>
       <c r="E47" t="n">
-        <v>0.04926057969197383</v>
+        <v>0.06664082041118792</v>
       </c>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="n">
-        <v>257.9700604288649</v>
+        <v>569.0785881349376</v>
       </c>
       <c r="H47" t="inlineStr"/>
       <c r="I47" t="n">
-        <v>1374409.4</v>
+        <v>3514842.033333333</v>
       </c>
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="n">
-        <v>2038.34586466168</v>
+        <v>391.2404467960009</v>
       </c>
       <c r="L47" t="n">
-        <v>-1227778</v>
+        <v>-5908117</v>
       </c>
       <c r="M47" t="n">
-        <v>6151886</v>
+        <v>-32117359</v>
       </c>
       <c r="N47" t="inlineStr"/>
       <c r="O47" t="n">
-        <v>257.431</v>
+        <v>577.6440000000001</v>
       </c>
       <c r="P47" t="inlineStr"/>
       <c r="Q47" t="n">
-        <v>255.3949908630059</v>
+        <v>572.0423121550317</v>
       </c>
     </row>
     <row r="48">
@@ -2665,42 +2665,42 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>258.7</v>
+        <v>573.55</v>
       </c>
       <c r="C48" t="n">
-        <v>1134330</v>
+        <v>3466022</v>
       </c>
       <c r="D48" t="n">
-        <v>-0.01564809102169207</v>
+        <v>-0.009699127818073805</v>
       </c>
       <c r="E48" t="n">
-        <v>0.04960361183779246</v>
+        <v>0.06702163413979741</v>
       </c>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="n">
-        <v>257.7539846317226</v>
+        <v>570.2700614860962</v>
       </c>
       <c r="H48" t="inlineStr"/>
       <c r="I48" t="n">
-        <v>1400729.533333333</v>
+        <v>3406797.3</v>
       </c>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="n">
-        <v>1588.953488372119</v>
+        <v>229.071706503613</v>
       </c>
       <c r="L48" t="n">
-        <v>-1134330</v>
+        <v>-3466022</v>
       </c>
       <c r="M48" t="n">
-        <v>5362282</v>
+        <v>-28876017</v>
       </c>
       <c r="N48" t="inlineStr"/>
       <c r="O48" t="n">
-        <v>257.2736666666667</v>
+        <v>579.2216666666667</v>
       </c>
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="n">
-        <v>255.1787833363166</v>
+        <v>572.1521267864132</v>
       </c>
     </row>
     <row r="49">
@@ -2710,42 +2710,42 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>262.78</v>
+        <v>579.14</v>
       </c>
       <c r="C49" t="n">
-        <v>1437911</v>
+        <v>3469161</v>
       </c>
       <c r="D49" t="n">
-        <v>0.01735035079517022</v>
+        <v>0.03285774192560975</v>
       </c>
       <c r="E49" t="n">
-        <v>0.04887179742595546</v>
+        <v>0.06692326564188041</v>
       </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="n">
-        <v>257.6917509321909</v>
+        <v>571.306737733419</v>
       </c>
       <c r="H49" t="inlineStr"/>
       <c r="I49" t="n">
-        <v>1403065.566666667</v>
+        <v>3358177.633333333</v>
       </c>
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="n">
-        <v>309.8440545808978</v>
+        <v>202.9049729197433</v>
       </c>
       <c r="L49" t="n">
-        <v>1437911</v>
+        <v>3469161</v>
       </c>
       <c r="M49" t="n">
-        <v>5292201</v>
+        <v>-27417427</v>
       </c>
       <c r="N49" t="inlineStr"/>
       <c r="O49" t="n">
-        <v>257.1993333333333</v>
+        <v>581.0353333333334</v>
       </c>
       <c r="P49" t="inlineStr"/>
       <c r="Q49" t="n">
-        <v>254.9359408077867</v>
+        <v>572.0557217372003</v>
       </c>
     </row>
     <row r="50">
@@ -2755,42 +2755,42 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>258.26</v>
+        <v>560.42</v>
       </c>
       <c r="C50" t="n">
-        <v>1469357</v>
+        <v>2857791</v>
       </c>
       <c r="D50" t="n">
-        <v>0.0250934518408048</v>
+        <v>0.01570020829863328</v>
       </c>
       <c r="E50" t="n">
-        <v>0.04877169083683121</v>
+        <v>0.06598183981524074</v>
       </c>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="n">
-        <v>257.5054319216337</v>
+        <v>572.9198369735478</v>
       </c>
       <c r="H50" t="inlineStr"/>
       <c r="I50" t="n">
-        <v>1386379.966666667</v>
+        <v>3349611.833333333</v>
       </c>
       <c r="J50" t="inlineStr"/>
       <c r="K50" t="n">
-        <v>909.0000000000006</v>
+        <v>344.1383036196637</v>
       </c>
       <c r="L50" t="n">
-        <v>1469357</v>
+        <v>2857791</v>
       </c>
       <c r="M50" t="n">
-        <v>4791633</v>
+        <v>-27674401</v>
       </c>
       <c r="N50" t="inlineStr"/>
       <c r="O50" t="n">
-        <v>257.0143333333334</v>
+        <v>582.7383333333332</v>
       </c>
       <c r="P50" t="inlineStr"/>
       <c r="Q50" t="n">
-        <v>254.3949712083237</v>
+        <v>571.5671508225245</v>
       </c>
     </row>
     <row r="51">
@@ -2800,42 +2800,42 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>251.86</v>
+        <v>551.6900000000001</v>
       </c>
       <c r="C51" t="n">
-        <v>881719</v>
+        <v>2833180</v>
       </c>
       <c r="D51" t="n">
-        <v>-0.007830769697239504</v>
+        <v>-0.00785393978778437</v>
       </c>
       <c r="E51" t="n">
-        <v>0.04699134280826229</v>
+        <v>0.06540724057847283</v>
       </c>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="n">
-        <v>257.3768690918707</v>
+        <v>574.1566486856885</v>
       </c>
       <c r="H51" t="inlineStr"/>
       <c r="I51" t="n">
-        <v>1368742.6</v>
+        <v>3325613.166666667</v>
       </c>
       <c r="J51" t="inlineStr"/>
       <c r="K51" t="n">
-        <v>-324.0683229813671</v>
+        <v>1092.842942345903</v>
       </c>
       <c r="L51" t="n">
-        <v>-881719</v>
+        <v>-2833180</v>
       </c>
       <c r="M51" t="n">
-        <v>4262512</v>
+        <v>-32670023</v>
       </c>
       <c r="N51" t="inlineStr"/>
       <c r="O51" t="n">
-        <v>256.8413333333334</v>
+        <v>584.522</v>
       </c>
       <c r="P51" t="inlineStr"/>
       <c r="Q51" t="n">
-        <v>254.1284174985529</v>
+        <v>572.3359198447675</v>
       </c>
     </row>
     <row r="52">
@@ -2845,42 +2845,42 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>253.84</v>
+        <v>556.04</v>
       </c>
       <c r="C52" t="n">
-        <v>1381047</v>
+        <v>2660544</v>
       </c>
       <c r="D52" t="n">
-        <v>0.01085288111140059</v>
+        <v>0.02356518205292968</v>
       </c>
       <c r="E52" t="n">
-        <v>0.0468400213746609</v>
+        <v>0.06728576494287829</v>
       </c>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="n">
-        <v>257.3425901015</v>
+        <v>576.6180122600018</v>
       </c>
       <c r="H52" t="inlineStr"/>
       <c r="I52" t="n">
-        <v>1376554.033333333</v>
+        <v>3358047.333333333</v>
       </c>
       <c r="J52" t="inlineStr"/>
       <c r="K52" t="n">
-        <v>-281.6464237516875</v>
+        <v>-159.7965116279059</v>
       </c>
       <c r="L52" t="n">
-        <v>1381047</v>
+        <v>2660544</v>
       </c>
       <c r="M52" t="n">
-        <v>4028169</v>
+        <v>-26030638</v>
       </c>
       <c r="N52" t="inlineStr"/>
       <c r="O52" t="n">
-        <v>256.8376666666667</v>
+        <v>586.8850000000001</v>
       </c>
       <c r="P52" t="inlineStr"/>
       <c r="Q52" t="n">
-        <v>254.28486008466</v>
+        <v>573.7597763857859</v>
       </c>
     </row>
     <row r="53">
@@ -2890,42 +2890,42 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>251.1</v>
+        <v>543.09</v>
       </c>
       <c r="C53" t="n">
-        <v>1008050</v>
+        <v>3209766</v>
       </c>
       <c r="D53" t="n">
-        <v>0.01528952917029347</v>
+        <v>-0.003217121523178434</v>
       </c>
       <c r="E53" t="n">
-        <v>0.04647274640176043</v>
+        <v>0.06649403132514584</v>
       </c>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="n">
-        <v>257.3264730574904</v>
+        <v>578.0456526953902</v>
       </c>
       <c r="H53" t="inlineStr"/>
       <c r="I53" t="n">
-        <v>1369667.633333333</v>
+        <v>3369330.266666667</v>
       </c>
       <c r="J53" t="inlineStr"/>
       <c r="K53" t="n">
-        <v>-163.7759710930442</v>
+        <v>-68.24752314438834</v>
       </c>
       <c r="L53" t="n">
-        <v>1008050</v>
+        <v>-3209766</v>
       </c>
       <c r="M53" t="n">
-        <v>1472667</v>
+        <v>-25692150</v>
       </c>
       <c r="N53" t="inlineStr"/>
       <c r="O53" t="n">
-        <v>256.7983333333333</v>
+        <v>588.5663333333334</v>
       </c>
       <c r="P53" t="inlineStr"/>
       <c r="Q53" t="n">
-        <v>254.3155400904986</v>
+        <v>574.9818299296331</v>
       </c>
     </row>
     <row r="54">
@@ -2935,42 +2935,42 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>247.29</v>
+        <v>544.84</v>
       </c>
       <c r="C54" t="n">
-        <v>1850322</v>
+        <v>4286834</v>
       </c>
       <c r="D54" t="n">
-        <v>-0.05280858394621024</v>
+        <v>-0.04152360575955072</v>
       </c>
       <c r="E54" t="n">
-        <v>0.04591970916200373</v>
+        <v>0.06661278084842709</v>
       </c>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="n">
-        <v>257.3652303649248</v>
+        <v>579.6790681838075</v>
       </c>
       <c r="H54" t="inlineStr"/>
       <c r="I54" t="n">
-        <v>1370401.766666667</v>
+        <v>3353120.166666667</v>
       </c>
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="n">
-        <v>-208.3421330517428</v>
+        <v>-78.51007887817684</v>
       </c>
       <c r="L54" t="n">
-        <v>-1850322</v>
+        <v>-4286834</v>
       </c>
       <c r="M54" t="n">
-        <v>1494691</v>
+        <v>-25205847</v>
       </c>
       <c r="N54" t="inlineStr"/>
       <c r="O54" t="n">
-        <v>256.8543333333333</v>
+        <v>590.3693333333334</v>
       </c>
       <c r="P54" t="inlineStr"/>
       <c r="Q54" t="n">
-        <v>254.5373014760502</v>
+        <v>577.1812664765044</v>
       </c>
     </row>
     <row r="55">
@@ -2980,42 +2980,42 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>260.7</v>
+        <v>567.9400000000001</v>
       </c>
       <c r="C55" t="n">
-        <v>1945028</v>
+        <v>2556419</v>
       </c>
       <c r="D55" t="n">
-        <v>-0.0153778913461684</v>
+        <v>-0.005250830858353872</v>
       </c>
       <c r="E55" t="n">
-        <v>0.03609104966142567</v>
+        <v>0.06352919850384618</v>
       </c>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="n">
-        <v>257.5904571054107</v>
+        <v>582.2254459518539</v>
       </c>
       <c r="H55" t="inlineStr"/>
       <c r="I55" t="n">
-        <v>1356758.533333333</v>
+        <v>3359825.7</v>
       </c>
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="n">
-        <v>-1472.38805970146</v>
+        <v>-102.0273348519359</v>
       </c>
       <c r="L55" t="n">
-        <v>-1945028</v>
+        <v>-2556419</v>
       </c>
       <c r="M55" t="n">
-        <v>4786038</v>
+        <v>-25407013</v>
       </c>
       <c r="N55" t="inlineStr"/>
       <c r="O55" t="n">
-        <v>256.971</v>
+        <v>592.3276666666667</v>
       </c>
       <c r="P55" t="inlineStr"/>
       <c r="Q55" t="n">
-        <v>255.0371153709502</v>
+        <v>579.4116986472978</v>
       </c>
     </row>
     <row r="56">
@@ -3025,42 +3025,42 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>264.74</v>
+        <v>570.9299999999999</v>
       </c>
       <c r="C56" t="n">
-        <v>3854244</v>
+        <v>2968098</v>
       </c>
       <c r="D56" t="n">
-        <v>0.02512992962432214</v>
+        <v>0.01882995142619937</v>
       </c>
       <c r="E56" t="n">
-        <v>0.03795577584929169</v>
+        <v>0.06572839836790101</v>
       </c>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="n">
-        <v>257.1690732237741</v>
+        <v>583.6632133039798</v>
       </c>
       <c r="H56" t="inlineStr"/>
       <c r="I56" t="n">
-        <v>1332115.166666667</v>
+        <v>3399789.666666667</v>
       </c>
       <c r="J56" t="inlineStr"/>
       <c r="K56" t="n">
-        <v>-1017.010309278355</v>
+        <v>-79.58422174840049</v>
       </c>
       <c r="L56" t="n">
-        <v>3854244</v>
+        <v>2968098</v>
       </c>
       <c r="M56" t="n">
-        <v>7936793</v>
+        <v>-19095256</v>
       </c>
       <c r="N56" t="inlineStr"/>
       <c r="O56" t="n">
-        <v>256.569</v>
+        <v>593.7813333333335</v>
       </c>
       <c r="P56" t="inlineStr"/>
       <c r="Q56" t="n">
-        <v>254.6465716034295</v>
+        <v>580.2028502781459</v>
       </c>
     </row>
     <row r="57">
@@ -3070,42 +3070,42 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>258.17</v>
+        <v>560.28</v>
       </c>
       <c r="C57" t="n">
-        <v>3331660</v>
+        <v>3844366</v>
       </c>
       <c r="D57" t="n">
-        <v>0.01137482561652803</v>
+        <v>0.01521475262818406</v>
       </c>
       <c r="E57" t="n">
-        <v>0.03630083469513012</v>
+        <v>0.06480679263056284</v>
       </c>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="n">
-        <v>255.9348946028815</v>
+        <v>584.3097739853628</v>
       </c>
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="n">
-        <v>1238397.233333333</v>
+        <v>3393973.4</v>
       </c>
       <c r="J57" t="inlineStr"/>
       <c r="K57" t="n">
-        <v>-548.8023952095874</v>
+        <v>-81.845987765383</v>
       </c>
       <c r="L57" t="n">
-        <v>3331660</v>
+        <v>3844366</v>
       </c>
       <c r="M57" t="n">
-        <v>5125255</v>
+        <v>-24856964</v>
       </c>
       <c r="N57" t="inlineStr"/>
       <c r="O57" t="n">
-        <v>255.7836666666667</v>
+        <v>594.5403333333335</v>
       </c>
       <c r="P57" t="inlineStr"/>
       <c r="Q57" t="n">
-        <v>253.9504730933212</v>
+        <v>580.84235719388</v>
       </c>
     </row>
     <row r="58">
@@ -3115,42 +3115,42 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>255.25</v>
+        <v>551.8200000000001</v>
       </c>
       <c r="C58" t="n">
-        <v>1702995</v>
+        <v>2313223</v>
       </c>
       <c r="D58" t="n">
-        <v>-0.00663805639346382</v>
+        <v>-0.00121342753793563</v>
       </c>
       <c r="E58" t="n">
-        <v>0.03684662750174533</v>
+        <v>0.06411273250622607</v>
       </c>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="n">
-        <v>255.0620268825716</v>
+        <v>585.5318501755251</v>
       </c>
       <c r="H58" t="inlineStr"/>
       <c r="I58" t="n">
-        <v>1171688.5</v>
+        <v>3352104.3</v>
       </c>
       <c r="J58" t="inlineStr"/>
       <c r="K58" t="n">
-        <v>-581.4465408805032</v>
+        <v>-57.84788380446662</v>
       </c>
       <c r="L58" t="n">
-        <v>-1702995</v>
+        <v>-2313223</v>
       </c>
       <c r="M58" t="n">
-        <v>463197</v>
+        <v>-31289623</v>
       </c>
       <c r="N58" t="inlineStr"/>
       <c r="O58" t="n">
-        <v>255.127</v>
+        <v>595.7343333333333</v>
       </c>
       <c r="P58" t="inlineStr"/>
       <c r="Q58" t="n">
-        <v>253.6594712376882</v>
+        <v>582.2604507934579</v>
       </c>
     </row>
     <row r="59">
@@ -3160,42 +3160,42 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>256.95</v>
+        <v>552.49</v>
       </c>
       <c r="C59" t="n">
-        <v>951007</v>
+        <v>3247572</v>
       </c>
       <c r="D59" t="n">
-        <v>-0.001555512660525338</v>
+        <v>-0.01435822576857948</v>
       </c>
       <c r="E59" t="n">
-        <v>0.03669148072195758</v>
+        <v>0.06415443490003665</v>
       </c>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="n">
-        <v>254.5211394057025</v>
+        <v>586.5660730762121</v>
       </c>
       <c r="H59" t="inlineStr"/>
       <c r="I59" t="n">
-        <v>1160415.466666667</v>
+        <v>3345866.733333333</v>
       </c>
       <c r="J59" t="inlineStr"/>
       <c r="K59" t="n">
-        <v>772.390572390574</v>
+        <v>-83.71454711802383</v>
       </c>
       <c r="L59" t="n">
-        <v>-951007</v>
+        <v>-3247572</v>
       </c>
       <c r="M59" t="n">
-        <v>801388</v>
+        <v>-26850304</v>
       </c>
       <c r="N59" t="inlineStr"/>
       <c r="O59" t="n">
-        <v>254.6686666666667</v>
+        <v>597.263</v>
       </c>
       <c r="P59" t="inlineStr"/>
       <c r="Q59" t="n">
-        <v>253.549779598908</v>
+        <v>584.3597922274895</v>
       </c>
     </row>
     <row r="60">
@@ -3205,42 +3205,42 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>257.35</v>
+        <v>560.48</v>
       </c>
       <c r="C60" t="n">
-        <v>987824</v>
+        <v>4251153</v>
       </c>
       <c r="D60" t="n">
-        <v>0.0005830337352996651</v>
+        <v>0.01264021426031814</v>
       </c>
       <c r="E60" t="n">
-        <v>0.03675092933672316</v>
+        <v>0.0638290544444587</v>
       </c>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="n">
-        <v>254.1041050443286</v>
+        <v>587.8373411078838</v>
       </c>
       <c r="H60" t="inlineStr"/>
       <c r="I60" t="n">
-        <v>1162469.866666667</v>
+        <v>3286686.566666667</v>
       </c>
       <c r="J60" t="inlineStr"/>
       <c r="K60" t="n">
-        <v>531.0572687224656</v>
+        <v>-65.33847472150813</v>
       </c>
       <c r="L60" t="n">
-        <v>987824</v>
+        <v>4251153</v>
       </c>
       <c r="M60" t="n">
-        <v>2765034</v>
+        <v>-25074899</v>
       </c>
       <c r="N60" t="inlineStr"/>
       <c r="O60" t="n">
-        <v>254.185</v>
+        <v>598.7313333333334</v>
       </c>
       <c r="P60" t="inlineStr"/>
       <c r="Q60" t="n">
-        <v>253.315281640212</v>
+        <v>586.5577089328335</v>
       </c>
     </row>
     <row r="61">
@@ -3250,42 +3250,42 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>257.2</v>
+        <v>553.4400000000001</v>
       </c>
       <c r="C61" t="n">
-        <v>821491</v>
+        <v>4546484</v>
       </c>
       <c r="D61" t="n">
-        <v>0.0008557315081292316</v>
+        <v>0.02909436110842467</v>
       </c>
       <c r="E61" t="n">
-        <v>0.03684828392259942</v>
+        <v>0.06371721141515538</v>
       </c>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="n">
-        <v>253.6133675005126</v>
+        <v>589.2730752119587</v>
       </c>
       <c r="H61" t="inlineStr"/>
       <c r="I61" t="n">
-        <v>1164057.333333333</v>
+        <v>3222709.133333333</v>
       </c>
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="n">
-        <v>3194.666666666665</v>
+        <v>-47.60206591244474</v>
       </c>
       <c r="L61" t="n">
-        <v>821491</v>
+        <v>4546484</v>
       </c>
       <c r="M61" t="n">
-        <v>2812658</v>
+        <v>-26994222</v>
       </c>
       <c r="N61" t="inlineStr"/>
       <c r="O61" t="n">
-        <v>253.6283333333334</v>
+        <v>599.965</v>
       </c>
       <c r="P61" t="inlineStr"/>
       <c r="Q61" t="n">
-        <v>253.037025201606</v>
+        <v>588.3561716178565</v>
       </c>
     </row>
     <row r="62">
@@ -3295,42 +3295,42 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>256.98</v>
+        <v>537.5700000000001</v>
       </c>
       <c r="C62" t="n">
-        <v>1077877</v>
+        <v>5023397</v>
       </c>
       <c r="D62" t="n">
-        <v>0.01750780735591029</v>
+        <v>-0.001765652030599973</v>
       </c>
       <c r="E62" t="n">
-        <v>0.03718055651391287</v>
+        <v>0.06167235567272367</v>
       </c>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="n">
-        <v>253.1222456701421</v>
+        <v>591.0410385216029</v>
       </c>
       <c r="H62" t="inlineStr"/>
       <c r="I62" t="n">
-        <v>1168839.366666667</v>
+        <v>3142349.333333333</v>
       </c>
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="n">
-        <v>1315.183246073281</v>
+        <v>-32.86473323002002</v>
       </c>
       <c r="L62" t="n">
-        <v>1077877</v>
+        <v>-5023397</v>
       </c>
       <c r="M62" t="n">
-        <v>2956119</v>
+        <v>-29405016</v>
       </c>
       <c r="N62" t="inlineStr"/>
       <c r="O62" t="n">
-        <v>253.0156666666667</v>
+        <v>601.2180000000001</v>
       </c>
       <c r="P62" t="inlineStr"/>
       <c r="Q62" t="n">
-        <v>252.7499234913719</v>
+        <v>590.7641834535707</v>
       </c>
     </row>
     <row r="63">
@@ -3340,42 +3340,42 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>252.52</v>
+        <v>538.52</v>
       </c>
       <c r="C63" t="n">
-        <v>742306</v>
+        <v>4493535</v>
       </c>
       <c r="D63" t="n">
-        <v>-0.0107921800551205</v>
+        <v>-0.006275299879992424</v>
       </c>
       <c r="E63" t="n">
-        <v>0.03630393341082253</v>
+        <v>0.0620292649493256</v>
       </c>
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="n">
-        <v>252.5705603650777</v>
+        <v>593.8848093301863</v>
       </c>
       <c r="H63" t="inlineStr"/>
       <c r="I63" t="n">
-        <v>1162192.933333333</v>
+        <v>3039133.4</v>
       </c>
       <c r="J63" t="inlineStr"/>
       <c r="K63" t="n">
-        <v>-1699.224806201567</v>
+        <v>-50.23971738581886</v>
       </c>
       <c r="L63" t="n">
-        <v>-742306</v>
+        <v>-4493535</v>
       </c>
       <c r="M63" t="n">
-        <v>2756726</v>
+        <v>-22454700</v>
       </c>
       <c r="N63" t="inlineStr"/>
       <c r="O63" t="n">
-        <v>252.315</v>
+        <v>602.8389999999999</v>
       </c>
       <c r="P63" t="inlineStr"/>
       <c r="Q63" t="n">
-        <v>252.4581940769837</v>
+        <v>594.4327478296789</v>
       </c>
     </row>
     <row r="64">
@@ -3385,42 +3385,42 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>255.26</v>
+        <v>541.91</v>
       </c>
       <c r="C64" t="n">
-        <v>1277518</v>
+        <v>6567568</v>
       </c>
       <c r="D64" t="n">
-        <v>-0.01183906654724964</v>
+        <v>-0.008727100962795831</v>
       </c>
       <c r="E64" t="n">
-        <v>0.03756229427922167</v>
+        <v>0.06402583482395495</v>
       </c>
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="n">
-        <v>251.8749149106037</v>
+        <v>596.2425995566191</v>
       </c>
       <c r="H64" t="inlineStr"/>
       <c r="I64" t="n">
-        <v>1185700.033333333</v>
+        <v>2983680.733333333</v>
       </c>
       <c r="J64" t="inlineStr"/>
       <c r="K64" t="n">
-        <v>-1811.570247933834</v>
+        <v>-46.27542126670542</v>
       </c>
       <c r="L64" t="n">
-        <v>-1277518</v>
+        <v>-6567568</v>
       </c>
       <c r="M64" t="n">
-        <v>4946551</v>
+        <v>-15131210</v>
       </c>
       <c r="N64" t="inlineStr"/>
       <c r="O64" t="n">
-        <v>251.746</v>
+        <v>604.24</v>
       </c>
       <c r="P64" t="inlineStr"/>
       <c r="Q64" t="n">
-        <v>252.4539315995343</v>
+        <v>598.2887994041395</v>
       </c>
     </row>
     <row r="65">
@@ -3430,42 +3430,42 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>258.3</v>
+        <v>546.66</v>
       </c>
       <c r="C65" t="n">
-        <v>1369454</v>
+        <v>10328353</v>
       </c>
       <c r="D65" t="n">
-        <v>-0.01135610317722602</v>
+        <v>-0.07704098471497378</v>
       </c>
       <c r="E65" t="n">
-        <v>0.03661448795853822</v>
+        <v>0.06392161986598364</v>
       </c>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="n">
-        <v>251.0346800085878</v>
+        <v>599.7301729217089</v>
       </c>
       <c r="H65" t="inlineStr"/>
       <c r="I65" t="n">
-        <v>1181059.3</v>
+        <v>2828869.8</v>
       </c>
       <c r="J65" t="inlineStr"/>
       <c r="K65" t="n">
-        <v>2048.59813084113</v>
+        <v>-47.64867775517536</v>
       </c>
       <c r="L65" t="n">
-        <v>-1369454</v>
+        <v>-10328353</v>
       </c>
       <c r="M65" t="n">
-        <v>7362365</v>
+        <v>-10486882</v>
       </c>
       <c r="N65" t="inlineStr"/>
       <c r="O65" t="n">
-        <v>250.888</v>
+        <v>604.9963333333333</v>
       </c>
       <c r="P65" t="inlineStr"/>
       <c r="Q65" t="n">
-        <v>252.2604096408815</v>
+        <v>602.1769924664939</v>
       </c>
     </row>
     <row r="66">
@@ -3475,42 +3475,42 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>261.25</v>
+        <v>590.4400000000001</v>
       </c>
       <c r="C66" t="n">
-        <v>724512</v>
+        <v>3677358</v>
       </c>
       <c r="D66" t="n">
-        <v>-0.003515345028541894</v>
+        <v>-0.02379829491907248</v>
       </c>
       <c r="E66" t="n">
-        <v>0.03566936390348929</v>
+        <v>0.04888611626965295</v>
       </c>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="n">
-        <v>249.7911127909204</v>
+        <v>605.9908844489299</v>
       </c>
       <c r="H66" t="inlineStr"/>
       <c r="I66" t="n">
-        <v>1187171.8</v>
+        <v>2554328</v>
       </c>
       <c r="J66" t="inlineStr"/>
       <c r="K66" t="n">
-        <v>318.8264058679707</v>
+        <v>-238.91017454236</v>
       </c>
       <c r="L66" t="n">
-        <v>-724512</v>
+        <v>-3677358</v>
       </c>
       <c r="M66" t="n">
-        <v>10284648</v>
+        <v>-2250628</v>
       </c>
       <c r="N66" t="inlineStr"/>
       <c r="O66" t="n">
-        <v>249.9086666666666</v>
+        <v>605.6759999999999</v>
       </c>
       <c r="P66" t="inlineStr"/>
       <c r="Q66" t="n">
-        <v>251.8438861678388</v>
+        <v>606.0057505676314</v>
       </c>
     </row>
     <row r="67">
@@ -3520,42 +3520,42 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>262.17</v>
+        <v>604.66</v>
       </c>
       <c r="C67" t="n">
-        <v>925541</v>
+        <v>1615119</v>
       </c>
       <c r="D67" t="n">
-        <v>0.02085135186398546</v>
+        <v>0.004591612227649478</v>
       </c>
       <c r="E67" t="n">
-        <v>0.03993752551651393</v>
+        <v>0.04773864799702436</v>
       </c>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="n">
-        <v>248.7624132278543</v>
+        <v>605.6254633050906</v>
       </c>
       <c r="H67" t="inlineStr"/>
       <c r="I67" t="n">
-        <v>1205652.833333333</v>
+        <v>2514349.666666667</v>
       </c>
       <c r="J67" t="inlineStr"/>
       <c r="K67" t="n">
-        <v>262.9558541266794</v>
+        <v>-313.1696428571422</v>
       </c>
       <c r="L67" t="n">
-        <v>925541</v>
+        <v>1615119</v>
       </c>
       <c r="M67" t="n">
-        <v>9730217</v>
+        <v>-1051278</v>
       </c>
       <c r="N67" t="inlineStr"/>
       <c r="O67" t="n">
-        <v>248.7733333333333</v>
+        <v>605.0543333333334</v>
       </c>
       <c r="P67" t="inlineStr"/>
       <c r="Q67" t="n">
-        <v>251.1951886621725</v>
+        <v>607.0792506067783</v>
       </c>
     </row>
     <row r="68">
@@ -3565,40 +3565,40 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>256.76</v>
+        <v>601.89</v>
       </c>
       <c r="C68" t="n">
-        <v>1341584</v>
+        <v>2985238</v>
       </c>
       <c r="D68" t="n">
-        <v>-0.02035536742009825</v>
+        <v>-0.01639610606276243</v>
       </c>
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="n">
-        <v>247.8480539902044</v>
+        <v>604.6989410602854</v>
       </c>
       <c r="H68" t="inlineStr"/>
       <c r="I68" t="n">
-        <v>1222918.133333333</v>
+        <v>2555185.433333333</v>
       </c>
       <c r="J68" t="inlineStr"/>
       <c r="K68" t="n">
-        <v>536.341463414635</v>
+        <v>-1513.071895424828</v>
       </c>
       <c r="L68" t="n">
-        <v>-1341584</v>
+        <v>-2985238</v>
       </c>
       <c r="M68" t="n">
-        <v>7361176</v>
+        <v>-5506589</v>
       </c>
       <c r="N68" t="inlineStr"/>
       <c r="O68" t="n">
-        <v>247.8383333333333</v>
+        <v>604.2346666666667</v>
       </c>
       <c r="P68" t="inlineStr"/>
       <c r="Q68" t="n">
-        <v>250.4383051216327</v>
+        <v>607.2460954762112</v>
       </c>
     </row>
     <row r="69">
@@ -3608,13 +3608,13 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>262.04</v>
+        <v>611.84</v>
       </c>
       <c r="C69" t="n">
-        <v>1055527</v>
+        <v>2317239</v>
       </c>
       <c r="D69" t="n">
-        <v>-0.01755227388618419</v>
+        <v>-0.02481060236366517</v>
       </c>
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr"/>
@@ -3623,17 +3623,17 @@
       <c r="I69" t="inlineStr"/>
       <c r="J69" t="inlineStr"/>
       <c r="K69" t="n">
-        <v>237.4730021598268</v>
+        <v>537.1759890859469</v>
       </c>
       <c r="L69" t="n">
-        <v>-1055527</v>
+        <v>-2317239</v>
       </c>
       <c r="M69" t="inlineStr"/>
       <c r="N69" t="inlineStr"/>
       <c r="O69" t="inlineStr"/>
       <c r="P69" t="inlineStr"/>
       <c r="Q69" t="n">
-        <v>250.0023261645039</v>
+        <v>607.6154813711222</v>
       </c>
     </row>
     <row r="70">
@@ -3643,13 +3643,13 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>266.68</v>
+        <v>627.21</v>
       </c>
       <c r="C70" t="n">
-        <v>1828625</v>
+        <v>2091353</v>
       </c>
       <c r="D70" t="n">
-        <v>0.01957691405826534</v>
+        <v>0.01826174781075984</v>
       </c>
       <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr"/>
@@ -3658,17 +3658,17 @@
       <c r="I70" t="inlineStr"/>
       <c r="J70" t="inlineStr"/>
       <c r="K70" t="n">
-        <v>150.9125235997482</v>
+        <v>333.4038950042346</v>
       </c>
       <c r="L70" t="n">
-        <v>1828625</v>
+        <v>2091353</v>
       </c>
       <c r="M70" t="inlineStr"/>
       <c r="N70" t="inlineStr"/>
       <c r="O70" t="inlineStr"/>
       <c r="P70" t="inlineStr"/>
       <c r="Q70" t="n">
-        <v>249.1721417620559</v>
+        <v>607.3241352587858</v>
       </c>
     </row>
     <row r="71">
@@ -3678,13 +3678,13 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>261.51</v>
+        <v>615.86</v>
       </c>
       <c r="C71" t="n">
-        <v>771127</v>
+        <v>1815682</v>
       </c>
       <c r="D71" t="n">
-        <v>0.01184765945091559</v>
+        <v>1.623758839386369e-05</v>
       </c>
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr"/>
@@ -3693,17 +3693,17 @@
       <c r="I71" t="inlineStr"/>
       <c r="J71" t="inlineStr"/>
       <c r="K71" t="n">
-        <v>162.8593628593628</v>
+        <v>1563.805104408332</v>
       </c>
       <c r="L71" t="n">
-        <v>771127</v>
+        <v>1815682</v>
       </c>
       <c r="M71" t="inlineStr"/>
       <c r="N71" t="inlineStr"/>
       <c r="O71" t="inlineStr"/>
       <c r="P71" t="inlineStr"/>
       <c r="Q71" t="n">
-        <v>247.9647032628873</v>
+        <v>605.9526963111157</v>
       </c>
     </row>
     <row r="72">
@@ -3713,13 +3713,13 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>258.43</v>
+        <v>615.85</v>
       </c>
       <c r="C72" t="n">
-        <v>1125207</v>
+        <v>2313824</v>
       </c>
       <c r="D72" t="n">
-        <v>0.01736934047979144</v>
+        <v>0.0142440204177694</v>
       </c>
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr"/>
@@ -3728,17 +3728,17 @@
       <c r="I72" t="inlineStr"/>
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="n">
-        <v>146.8985507246377</v>
+        <v>384.8306997742673</v>
       </c>
       <c r="L72" t="n">
-        <v>1125207</v>
+        <v>2313824</v>
       </c>
       <c r="M72" t="inlineStr"/>
       <c r="N72" t="inlineStr"/>
       <c r="O72" t="inlineStr"/>
       <c r="P72" t="inlineStr"/>
       <c r="Q72" t="n">
-        <v>247.0305448672243</v>
+        <v>605.2694339877443</v>
       </c>
     </row>
     <row r="73">
@@ -3748,13 +3748,13 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>253.98</v>
+        <v>607.14</v>
       </c>
       <c r="C73" t="n">
-        <v>865174</v>
+        <v>3436244</v>
       </c>
       <c r="D73" t="n">
-        <v>0.004617305308515895</v>
+        <v>-0.03775374843525103</v>
       </c>
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr"/>
@@ -3763,17 +3763,17 @@
       <c r="I73" t="inlineStr"/>
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="n">
-        <v>152.1598968407479</v>
+        <v>693.206521739133</v>
       </c>
       <c r="L73" t="n">
-        <v>865174</v>
+        <v>-3436244</v>
       </c>
       <c r="M73" t="inlineStr"/>
       <c r="N73" t="inlineStr"/>
       <c r="O73" t="inlineStr"/>
       <c r="P73" t="inlineStr"/>
       <c r="Q73" t="n">
-        <v>246.2443755477225</v>
+        <v>604.5397397800024</v>
       </c>
     </row>
     <row r="74">
@@ -3783,13 +3783,13 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>252.81</v>
+        <v>630.5</v>
       </c>
       <c r="C74" t="n">
-        <v>1336118</v>
+        <v>2131245</v>
       </c>
       <c r="D74" t="n">
-        <v>-0.01429549538290598</v>
+        <v>-0.006733819289666876</v>
       </c>
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr"/>
@@ -3798,17 +3798,17 @@
       <c r="I74" t="inlineStr"/>
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="n">
-        <v>198.3200707338639</v>
+        <v>233.1809872029249</v>
       </c>
       <c r="L74" t="n">
-        <v>-1336118</v>
+        <v>-2131245</v>
       </c>
       <c r="M74" t="inlineStr"/>
       <c r="N74" t="inlineStr"/>
       <c r="O74" t="inlineStr"/>
       <c r="P74" t="inlineStr"/>
       <c r="Q74" t="n">
-        <v>245.7108842061862</v>
+        <v>604.3604114889681</v>
       </c>
     </row>
     <row r="75">
@@ -3818,13 +3818,13 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>256.45</v>
+        <v>634.76</v>
       </c>
       <c r="C75" t="n">
-        <v>1592890</v>
+        <v>2542763</v>
       </c>
       <c r="D75" t="n">
-        <v>0.005395696543851969</v>
+        <v>0.01085013059851381</v>
       </c>
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr"/>
@@ -3833,17 +3833,17 @@
       <c r="I75" t="inlineStr"/>
       <c r="J75" t="inlineStr"/>
       <c r="K75" t="n">
-        <v>160.0999286224127</v>
+        <v>203.2182103610675</v>
       </c>
       <c r="L75" t="n">
-        <v>1592890</v>
+        <v>2542763</v>
       </c>
       <c r="M75" t="inlineStr"/>
       <c r="N75" t="inlineStr"/>
       <c r="O75" t="inlineStr"/>
       <c r="P75" t="inlineStr"/>
       <c r="Q75" t="n">
-        <v>245.2212900135093</v>
+        <v>602.557681246828</v>
       </c>
     </row>
     <row r="76">
@@ -3853,13 +3853,13 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>255.07</v>
+        <v>627.91</v>
       </c>
       <c r="C76" t="n">
-        <v>1214059</v>
+        <v>1687613</v>
       </c>
       <c r="D76" t="n">
-        <v>0.004952061684110554</v>
+        <v>0.01626443707188674</v>
       </c>
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr"/>
@@ -3868,17 +3868,17 @@
       <c r="I76" t="inlineStr"/>
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="n">
-        <v>158.3911234396673</v>
+        <v>232.8073635765948</v>
       </c>
       <c r="L76" t="n">
-        <v>1214059</v>
+        <v>1687613</v>
       </c>
       <c r="M76" t="inlineStr"/>
       <c r="N76" t="inlineStr"/>
       <c r="O76" t="inlineStr"/>
       <c r="P76" t="inlineStr"/>
       <c r="Q76" t="n">
-        <v>244.4468962213376</v>
+        <v>600.3368316776437</v>
       </c>
     </row>
     <row r="77">
@@ -3888,13 +3888,13 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>253.81</v>
+        <v>617.78</v>
       </c>
       <c r="C77" t="n">
-        <v>2017382</v>
+        <v>2666775</v>
       </c>
       <c r="D77" t="n">
-        <v>-0.01042574309893762</v>
+        <v>-0.01634406314787551</v>
       </c>
       <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr"/>
@@ -3903,17 +3903,17 @@
       <c r="I77" t="inlineStr"/>
       <c r="J77" t="inlineStr"/>
       <c r="K77" t="n">
-        <v>156.170780520347</v>
+        <v>251.0280373831779</v>
       </c>
       <c r="L77" t="n">
-        <v>-2017382</v>
+        <v>-2666775</v>
       </c>
       <c r="M77" t="inlineStr"/>
       <c r="N77" t="inlineStr"/>
       <c r="O77" t="inlineStr"/>
       <c r="P77" t="inlineStr"/>
       <c r="Q77" t="n">
-        <v>243.7142683745332</v>
+        <v>598.4352338623087</v>
       </c>
     </row>
     <row r="78">
@@ -3923,13 +3923,13 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>256.47</v>
+        <v>627.96</v>
       </c>
       <c r="C78" t="n">
-        <v>1204411</v>
+        <v>2007432</v>
       </c>
       <c r="D78" t="n">
-        <v>-0.002958927601709682</v>
+        <v>-0.003608361953284955</v>
       </c>
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr"/>
@@ -3938,17 +3938,17 @@
       <c r="I78" t="inlineStr"/>
       <c r="J78" t="inlineStr"/>
       <c r="K78" t="n">
-        <v>128.0838615309604</v>
+        <v>172.3659003831419</v>
       </c>
       <c r="L78" t="n">
-        <v>-1204411</v>
+        <v>-2007432</v>
       </c>
       <c r="M78" t="inlineStr"/>
       <c r="N78" t="inlineStr"/>
       <c r="O78" t="inlineStr"/>
       <c r="P78" t="inlineStr"/>
       <c r="Q78" t="n">
-        <v>243.0180110210528</v>
+        <v>597.1011120597092</v>
       </c>
     </row>
     <row r="79">
@@ -3958,13 +3958,13 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>257.23</v>
+        <v>630.23</v>
       </c>
       <c r="C79" t="n">
-        <v>937343</v>
+        <v>3212187</v>
       </c>
       <c r="D79" t="n">
-        <v>0.01630449600735329</v>
+        <v>0.02620391699215396</v>
       </c>
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr"/>
@@ -3973,17 +3973,17 @@
       <c r="I79" t="inlineStr"/>
       <c r="J79" t="inlineStr"/>
       <c r="K79" t="n">
-        <v>122.9568411386593</v>
+        <v>156.2600644122383</v>
       </c>
       <c r="L79" t="n">
-        <v>937343</v>
+        <v>3212187</v>
       </c>
       <c r="M79" t="inlineStr"/>
       <c r="N79" t="inlineStr"/>
       <c r="O79" t="inlineStr"/>
       <c r="P79" t="inlineStr"/>
       <c r="Q79" t="n">
-        <v>242.0902876431943</v>
+        <v>594.9729128914132</v>
       </c>
     </row>
     <row r="80">
@@ -3993,13 +3993,13 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>253.07</v>
+        <v>613.9299999999999</v>
       </c>
       <c r="C80" t="n">
-        <v>940236</v>
+        <v>2137831</v>
       </c>
       <c r="D80" t="n">
-        <v>0.005229598701936844</v>
+        <v>-0.01399121900461608</v>
       </c>
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr"/>
@@ -4008,17 +4008,17 @@
       <c r="I80" t="inlineStr"/>
       <c r="J80" t="inlineStr"/>
       <c r="K80" t="n">
-        <v>121.2314225053079</v>
+        <v>156.6592337320091</v>
       </c>
       <c r="L80" t="n">
-        <v>940236</v>
+        <v>-2137831</v>
       </c>
       <c r="M80" t="inlineStr"/>
       <c r="N80" t="inlineStr"/>
       <c r="O80" t="inlineStr"/>
       <c r="P80" t="inlineStr"/>
       <c r="Q80" t="n">
-        <v>241.0461695496215</v>
+        <v>592.5413896425451</v>
       </c>
     </row>
     <row r="81">
@@ -4028,13 +4028,13 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>251.75</v>
+        <v>622.58</v>
       </c>
       <c r="C81" t="n">
-        <v>1116062</v>
+        <v>3806205</v>
       </c>
       <c r="D81" t="n">
-        <v>-0.003608179803219258</v>
+        <v>0.02620038238981515</v>
       </c>
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr"/>
@@ -4043,17 +4043,17 @@
       <c r="I81" t="inlineStr"/>
       <c r="J81" t="inlineStr"/>
       <c r="K81" t="n">
-        <v>121.9010074463425</v>
+        <v>139.1680172879522</v>
       </c>
       <c r="L81" t="n">
-        <v>-1116062</v>
+        <v>3806205</v>
       </c>
       <c r="M81" t="inlineStr"/>
       <c r="N81" t="inlineStr"/>
       <c r="O81" t="inlineStr"/>
       <c r="P81" t="inlineStr"/>
       <c r="Q81" t="n">
-        <v>240.2169398633885</v>
+        <v>591.0663130661688</v>
       </c>
     </row>
     <row r="82">
@@ -4063,13 +4063,13 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>252.66</v>
+        <v>606.48</v>
       </c>
       <c r="C82" t="n">
-        <v>1174455</v>
+        <v>2999032</v>
       </c>
       <c r="D82" t="n">
-        <v>-0.0004748338170887934</v>
+        <v>0.01545317626202092</v>
       </c>
       <c r="E82" t="inlineStr"/>
       <c r="F82" t="inlineStr"/>
@@ -4078,17 +4078,17 @@
       <c r="I82" t="inlineStr"/>
       <c r="J82" t="inlineStr"/>
       <c r="K82" t="n">
-        <v>116.0581075775422</v>
+        <v>176.3620639953873</v>
       </c>
       <c r="L82" t="n">
-        <v>-1174455</v>
+        <v>2999032</v>
       </c>
       <c r="M82" t="inlineStr"/>
       <c r="N82" t="inlineStr"/>
       <c r="O82" t="inlineStr"/>
       <c r="P82" t="inlineStr"/>
       <c r="Q82" t="n">
-        <v>239.4215564056911</v>
+        <v>588.8929553465942</v>
       </c>
     </row>
     <row r="83">
@@ -4098,13 +4098,13 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>252.78</v>
+        <v>597.1799999999999</v>
       </c>
       <c r="C83" t="n">
-        <v>1030074</v>
+        <v>2723463</v>
       </c>
       <c r="D83" t="n">
-        <v>0.007903609663433286</v>
+        <v>-0.01067658400733951</v>
       </c>
       <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr"/>
@@ -4113,17 +4113,17 @@
       <c r="I83" t="inlineStr"/>
       <c r="J83" t="inlineStr"/>
       <c r="K83" t="n">
-        <v>158.4137191854234</v>
+        <v>303.2144944476925</v>
       </c>
       <c r="L83" t="n">
-        <v>1030074</v>
+        <v>-2723463</v>
       </c>
       <c r="M83" t="inlineStr"/>
       <c r="N83" t="inlineStr"/>
       <c r="O83" t="inlineStr"/>
       <c r="P83" t="inlineStr"/>
       <c r="Q83" t="n">
-        <v>238.5085602957388</v>
+        <v>587.6800557153249</v>
       </c>
     </row>
     <row r="84">
@@ -4133,13 +4133,13 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>250.79</v>
+        <v>603.59</v>
       </c>
       <c r="C84" t="n">
-        <v>1441025</v>
+        <v>4488000</v>
       </c>
       <c r="D84" t="n">
-        <v>0.008609868376264096</v>
+        <v>-0.01310155844000516</v>
       </c>
       <c r="E84" t="inlineStr"/>
       <c r="F84" t="inlineStr"/>
@@ -4148,17 +4148,17 @@
       <c r="I84" t="inlineStr"/>
       <c r="J84" t="inlineStr"/>
       <c r="K84" t="n">
-        <v>165.386922615477</v>
+        <v>220.5782312925167</v>
       </c>
       <c r="L84" t="n">
-        <v>1441025</v>
+        <v>-4488000</v>
       </c>
       <c r="M84" t="inlineStr"/>
       <c r="N84" t="inlineStr"/>
       <c r="O84" t="inlineStr"/>
       <c r="P84" t="inlineStr"/>
       <c r="Q84" t="n">
-        <v>237.5243230747552</v>
+        <v>587.0248871439679</v>
       </c>
     </row>
     <row r="85">
@@ -4168,13 +4168,13 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>248.64</v>
+        <v>611.55</v>
       </c>
       <c r="C85" t="n">
-        <v>1205727</v>
+        <v>3755338</v>
       </c>
       <c r="D85" t="n">
-        <v>0.03046252450383591</v>
+        <v>0.02962257665674262</v>
       </c>
       <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr"/>
@@ -4184,14 +4184,14 @@
       <c r="J85" t="inlineStr"/>
       <c r="K85" t="inlineStr"/>
       <c r="L85" t="n">
-        <v>1205727</v>
+        <v>3755338</v>
       </c>
       <c r="M85" t="inlineStr"/>
       <c r="N85" t="inlineStr"/>
       <c r="O85" t="inlineStr"/>
       <c r="P85" t="inlineStr"/>
       <c r="Q85" t="n">
-        <v>236.6094488040487</v>
+        <v>585.8824655676898</v>
       </c>
     </row>
     <row r="86">
@@ -4201,13 +4201,13 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>241.18</v>
+        <v>593.7</v>
       </c>
       <c r="C86" t="n">
-        <v>1042706</v>
+        <v>2793610</v>
       </c>
       <c r="D86" t="n">
-        <v>0.01130002642231531</v>
+        <v>-0.004034296949251726</v>
       </c>
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr"/>
@@ -4217,14 +4217,14 @@
       <c r="J86" t="inlineStr"/>
       <c r="K86" t="inlineStr"/>
       <c r="L86" t="n">
-        <v>1042706</v>
+        <v>-2793610</v>
       </c>
       <c r="M86" t="inlineStr"/>
       <c r="N86" t="inlineStr"/>
       <c r="O86" t="inlineStr"/>
       <c r="P86" t="inlineStr"/>
       <c r="Q86" t="n">
-        <v>235.779755618121</v>
+        <v>584.1122907792545</v>
       </c>
     </row>
     <row r="87">
@@ -4234,13 +4234,13 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>238.47</v>
+        <v>596.1</v>
       </c>
       <c r="C87" t="n">
-        <v>1330398</v>
+        <v>2588293</v>
       </c>
       <c r="D87" t="n">
-        <v>-0.01262595683949641</v>
+        <v>-0.002647055441664214</v>
       </c>
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr"/>
@@ -4250,14 +4250,14 @@
       <c r="J87" t="inlineStr"/>
       <c r="K87" t="inlineStr"/>
       <c r="L87" t="n">
-        <v>-1330398</v>
+        <v>-2588293</v>
       </c>
       <c r="M87" t="inlineStr"/>
       <c r="N87" t="inlineStr"/>
       <c r="O87" t="inlineStr"/>
       <c r="P87" t="inlineStr"/>
       <c r="Q87" t="n">
-        <v>235.4073249710949</v>
+        <v>583.4510694536859</v>
       </c>
     </row>
     <row r="88">
@@ -4267,13 +4267,13 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>241.5</v>
+        <v>597.6799999999999</v>
       </c>
       <c r="C88" t="n">
-        <v>1364804</v>
+        <v>2126096</v>
       </c>
       <c r="D88" t="n">
-        <v>-0.003884783990456775</v>
+        <v>0.001909196540466063</v>
       </c>
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr"/>
@@ -4283,14 +4283,14 @@
       <c r="J88" t="inlineStr"/>
       <c r="K88" t="inlineStr"/>
       <c r="L88" t="n">
-        <v>-1364804</v>
+        <v>2126096</v>
       </c>
       <c r="M88" t="inlineStr"/>
       <c r="N88" t="inlineStr"/>
       <c r="O88" t="inlineStr"/>
       <c r="P88" t="inlineStr"/>
       <c r="Q88" t="n">
-        <v>235.1961060035841</v>
+        <v>582.578729416009</v>
       </c>
     </row>
     <row r="89">
@@ -4300,13 +4300,13 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>242.44</v>
+        <v>596.54</v>
       </c>
       <c r="C89" t="n">
-        <v>1012639</v>
+        <v>1472167</v>
       </c>
       <c r="D89" t="n">
-        <v>0.007410661333966395</v>
+        <v>-0.001591250136857347</v>
       </c>
       <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr"/>
@@ -4316,14 +4316,14 @@
       <c r="J89" t="inlineStr"/>
       <c r="K89" t="inlineStr"/>
       <c r="L89" t="n">
-        <v>1012639</v>
+        <v>-1472167</v>
       </c>
       <c r="M89" t="inlineStr"/>
       <c r="N89" t="inlineStr"/>
       <c r="O89" t="inlineStr"/>
       <c r="P89" t="inlineStr"/>
       <c r="Q89" t="n">
-        <v>234.7613546934865</v>
+        <v>581.537262479182</v>
       </c>
     </row>
     <row r="90">
@@ -4333,13 +4333,13 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>240.65</v>
+        <v>597.49</v>
       </c>
       <c r="C90" t="n">
-        <v>1035448</v>
+        <v>2331830</v>
       </c>
       <c r="D90" t="n">
-        <v>0.007633465643879234</v>
+        <v>0.01087076972483647</v>
       </c>
       <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr"/>
@@ -4349,14 +4349,14 @@
       <c r="J90" t="inlineStr"/>
       <c r="K90" t="inlineStr"/>
       <c r="L90" t="n">
-        <v>1035448</v>
+        <v>2331830</v>
       </c>
       <c r="M90" t="inlineStr"/>
       <c r="N90" t="inlineStr"/>
       <c r="O90" t="inlineStr"/>
       <c r="P90" t="inlineStr"/>
       <c r="Q90" t="n">
-        <v>234.2317929482096</v>
+        <v>580.5025909260221</v>
       </c>
     </row>
     <row r="91">
@@ -4366,13 +4366,13 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>238.82</v>
+        <v>591.03</v>
       </c>
       <c r="C91" t="n">
-        <v>964952</v>
+        <v>2135690</v>
       </c>
       <c r="D91" t="n">
-        <v>0.01204783097036444</v>
+        <v>0.008205749262308437</v>
       </c>
       <c r="E91" t="inlineStr"/>
       <c r="F91" t="inlineStr"/>
@@ -4382,14 +4382,14 @@
       <c r="J91" t="inlineStr"/>
       <c r="K91" t="inlineStr"/>
       <c r="L91" t="n">
-        <v>964952</v>
+        <v>2135690</v>
       </c>
       <c r="M91" t="inlineStr"/>
       <c r="N91" t="inlineStr"/>
       <c r="O91" t="inlineStr"/>
       <c r="P91" t="inlineStr"/>
       <c r="Q91" t="n">
-        <v>233.7891579791206</v>
+        <v>579.3310454726443</v>
       </c>
     </row>
     <row r="92">
@@ -4399,13 +4399,13 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>235.96</v>
+        <v>586.2</v>
       </c>
       <c r="C92" t="n">
-        <v>878484</v>
+        <v>1926919</v>
       </c>
       <c r="D92" t="n">
-        <v>0.002163722445311045</v>
+        <v>0.009685098203776832</v>
       </c>
       <c r="E92" t="inlineStr"/>
       <c r="F92" t="inlineStr"/>
@@ -4415,14 +4415,14 @@
       <c r="J92" t="inlineStr"/>
       <c r="K92" t="inlineStr"/>
       <c r="L92" t="n">
-        <v>878484</v>
+        <v>1926919</v>
       </c>
       <c r="M92" t="inlineStr"/>
       <c r="N92" t="inlineStr"/>
       <c r="O92" t="inlineStr"/>
       <c r="P92" t="inlineStr"/>
       <c r="Q92" t="n">
-        <v>233.442203356991</v>
+        <v>578.5242210224818</v>
       </c>
     </row>
     <row r="93">
@@ -4432,13 +4432,13 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>235.45</v>
+        <v>580.55</v>
       </c>
       <c r="C93" t="n">
-        <v>1447519</v>
+        <v>2829955</v>
       </c>
       <c r="D93" t="n">
-        <v>0.02550840501645357</v>
+        <v>0.02785841425362623</v>
       </c>
       <c r="E93" t="inlineStr"/>
       <c r="F93" t="inlineStr"/>
@@ -4448,14 +4448,14 @@
       <c r="J93" t="inlineStr"/>
       <c r="K93" t="inlineStr"/>
       <c r="L93" t="n">
-        <v>1447519</v>
+        <v>2829955</v>
       </c>
       <c r="M93" t="inlineStr"/>
       <c r="N93" t="inlineStr"/>
       <c r="O93" t="inlineStr"/>
       <c r="P93" t="inlineStr"/>
       <c r="Q93" t="n">
-        <v>233.2685622091973</v>
+        <v>577.9948569550667</v>
       </c>
     </row>
     <row r="94">
@@ -4465,13 +4465,13 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>229.52</v>
+        <v>564.6</v>
       </c>
       <c r="C94" t="n">
-        <v>1138296</v>
+        <v>1923240</v>
       </c>
       <c r="D94" t="n">
-        <v>0.002617574132208311</v>
+        <v>-0.004329967441950799</v>
       </c>
       <c r="E94" t="inlineStr"/>
       <c r="F94" t="inlineStr"/>
@@ -4481,14 +4481,14 @@
       <c r="J94" t="inlineStr"/>
       <c r="K94" t="inlineStr"/>
       <c r="L94" t="n">
-        <v>1138296</v>
+        <v>-1923240</v>
       </c>
       <c r="M94" t="inlineStr"/>
       <c r="N94" t="inlineStr"/>
       <c r="O94" t="inlineStr"/>
       <c r="P94" t="inlineStr"/>
       <c r="Q94" t="n">
-        <v>233.1181182236246</v>
+        <v>577.8186401933471</v>
       </c>
     </row>
     <row r="95">
@@ -4498,13 +4498,13 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>228.92</v>
+        <v>567.05</v>
       </c>
       <c r="C95" t="n">
-        <v>1552829</v>
+        <v>2092099</v>
       </c>
       <c r="D95" t="n">
-        <v>0.007585925747060962</v>
+        <v>-0.008324307841554912</v>
       </c>
       <c r="E95" t="inlineStr"/>
       <c r="F95" t="inlineStr"/>
@@ -4514,14 +4514,14 @@
       <c r="J95" t="inlineStr"/>
       <c r="K95" t="inlineStr"/>
       <c r="L95" t="n">
-        <v>1552829</v>
+        <v>-2092099</v>
       </c>
       <c r="M95" t="inlineStr"/>
       <c r="N95" t="inlineStr"/>
       <c r="O95" t="inlineStr"/>
       <c r="P95" t="inlineStr"/>
       <c r="Q95" t="n">
-        <v>233.3662643080125</v>
+        <v>578.730270551509</v>
       </c>
     </row>
     <row r="96">
@@ -4531,13 +4531,13 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>227.19</v>
+        <v>571.79</v>
       </c>
       <c r="C96" t="n">
-        <v>1278943</v>
+        <v>2478008</v>
       </c>
       <c r="D96" t="n">
-        <v>-0.03004713262917935</v>
+        <v>-0.01437699481033228</v>
       </c>
       <c r="E96" t="inlineStr"/>
       <c r="F96" t="inlineStr"/>
@@ -4547,14 +4547,14 @@
       <c r="J96" t="inlineStr"/>
       <c r="K96" t="inlineStr"/>
       <c r="L96" t="n">
-        <v>-1278943</v>
+        <v>-2478008</v>
       </c>
       <c r="M96" t="inlineStr"/>
       <c r="N96" t="inlineStr"/>
       <c r="O96" t="inlineStr"/>
       <c r="P96" t="inlineStr"/>
       <c r="Q96" t="n">
-        <v>233.6729032258065</v>
+        <v>579.535806451613</v>
       </c>
     </row>
     <row r="97">
@@ -4564,10 +4564,10 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>234.12</v>
+        <v>580.0700000000001</v>
       </c>
       <c r="C97" t="n">
-        <v>1443500</v>
+        <v>2840192</v>
       </c>
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="inlineStr"/>
@@ -4578,14 +4578,14 @@
       <c r="J97" t="inlineStr"/>
       <c r="K97" t="inlineStr"/>
       <c r="L97" t="n">
-        <v>-1443500</v>
+        <v>-2840192</v>
       </c>
       <c r="M97" t="inlineStr"/>
       <c r="N97" t="inlineStr"/>
       <c r="O97" t="inlineStr"/>
       <c r="P97" t="inlineStr"/>
       <c r="Q97" t="n">
-        <v>234.12</v>
+        <v>580.0700000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>